<commit_message>
Raw data now in report
</commit_message>
<xml_diff>
--- a/hydrofia/hydrofia_ph_template.xlsx
+++ b/hydrofia/hydrofia_ph_template.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\mw\git\hydrofia\hydrofia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92053806-DE1E-4DD6-8259-A5421435230A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E89A0025-D37E-4ACB-A73C-E48C200C9CA4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-15" yWindow="165" windowWidth="15600" windowHeight="11610" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Rådata" sheetId="2" r:id="rId1"/>
+    <sheet name="Rådata" sheetId="4" r:id="rId1"/>
     <sheet name="Rapport för utskrift" sheetId="1" r:id="rId2"/>
     <sheet name="Verifiering" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">OFFSET('Rapport för utskrift'!$A$1,0,0,12+COUNTA(Rådata!$A:$A),12)</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">OFFSET('Rapport för utskrift'!$A$1,0,0,12+COUNTA(#REF!),12)</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'Rapport för utskrift'!$1:$11</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="839" uniqueCount="836">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="834">
   <si>
     <t>Djup</t>
   </si>
@@ -2575,9 +2575,6 @@
     <t>Lagt till villkorsstyrd formatering (fyllda celler) för kolumnen syrgashalt</t>
   </si>
   <si>
-    <t>Kopiera in rådata här</t>
-  </si>
-  <si>
     <t>191212/JLyc</t>
   </si>
   <si>
@@ -2594,9 +2591,6 @@
   </si>
   <si>
     <t>pH</t>
-  </si>
-  <si>
-    <t>Kopiera in CRM-data här</t>
   </si>
   <si>
     <t>Djup (ref)</t>
@@ -2942,6 +2936,26 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2971,26 +2985,6 @@
     </xf>
     <xf numFmtId="49" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3405,1111 +3399,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
-    <tabColor theme="6"/>
-  </sheetPr>
-  <dimension ref="A1:P148"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8B184CC-18AA-4DD3-91F3-47A3A5EC6B5D}">
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="27" style="2" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="7.5703125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="8.28515625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="21.7109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="8.5703125" style="5" customWidth="1"/>
-    <col min="8" max="8" width="6.28515625" style="6" customWidth="1"/>
-    <col min="9" max="9" width="5.28515625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="8.5703125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="8.42578125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="4.85546875" style="2" customWidth="1"/>
-    <col min="13" max="13" width="5.28515625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="26.5703125" style="2" customWidth="1"/>
-    <col min="15" max="15" width="12.5703125" style="2" customWidth="1"/>
-    <col min="16" max="16384" width="11.42578125" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>832</v>
-      </c>
-      <c r="C1" s="2"/>
-      <c r="E1" s="3"/>
-      <c r="G1" s="2"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="7"/>
-    </row>
-    <row r="2" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C2" s="2"/>
-      <c r="E2" s="3"/>
-      <c r="G2" s="2"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-    </row>
-    <row r="3" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>825</v>
-      </c>
-      <c r="C3" s="2"/>
-      <c r="E3" s="3"/>
-      <c r="G3" s="2"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-    </row>
-    <row r="4" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C4" s="2"/>
-      <c r="E4" s="3"/>
-      <c r="G4" s="2"/>
-      <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="1"/>
-      <c r="N4" s="8"/>
-      <c r="O4" s="8"/>
-    </row>
-    <row r="5" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C5" s="2"/>
-      <c r="E5" s="3"/>
-      <c r="G5" s="2"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="8"/>
-    </row>
-    <row r="6" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C6" s="2"/>
-      <c r="E6" s="3"/>
-      <c r="G6" s="2"/>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="9"/>
-    </row>
-    <row r="7" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C7" s="2"/>
-      <c r="E7" s="3"/>
-      <c r="G7" s="2"/>
-      <c r="I7" s="1"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="N7" s="8"/>
-      <c r="O7" s="8"/>
-    </row>
-    <row r="8" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C8" s="2"/>
-      <c r="E8" s="3"/>
-      <c r="G8" s="2"/>
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="N8" s="8"/>
-      <c r="O8" s="8"/>
-    </row>
-    <row r="9" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C9" s="2"/>
-      <c r="E9" s="3"/>
-      <c r="G9" s="2"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="N9" s="8"/>
-      <c r="O9" s="8"/>
-      <c r="P9" s="8"/>
-    </row>
-    <row r="10" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C10" s="2"/>
-      <c r="E10" s="3"/>
-      <c r="G10" s="2"/>
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="N10" s="8"/>
-    </row>
-    <row r="11" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C11" s="2"/>
-      <c r="E11" s="3"/>
-      <c r="G11" s="2"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="N11" s="8"/>
-    </row>
-    <row r="12" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C12" s="2"/>
-      <c r="E12" s="3"/>
-      <c r="G12" s="2"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="N12" s="8"/>
-    </row>
-    <row r="13" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C13" s="2"/>
-      <c r="E13" s="3"/>
-      <c r="G13" s="2"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="N13" s="8"/>
-    </row>
-    <row r="14" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C14" s="2"/>
-      <c r="E14" s="3"/>
-      <c r="G14" s="2"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="N14" s="8"/>
-    </row>
-    <row r="15" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C15" s="2"/>
-      <c r="E15" s="3"/>
-      <c r="G15" s="2"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="N15" s="8"/>
-    </row>
-    <row r="16" spans="1:16" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C16" s="2"/>
-      <c r="E16" s="3"/>
-      <c r="G16" s="2"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="N16" s="8"/>
-    </row>
-    <row r="17" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C17" s="2"/>
-      <c r="E17" s="3"/>
-      <c r="G17" s="2"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="N17" s="8"/>
-    </row>
-    <row r="18" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C18" s="2"/>
-      <c r="E18" s="3"/>
-      <c r="G18" s="2"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="N18" s="8"/>
-    </row>
-    <row r="19" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C19" s="2"/>
-      <c r="E19" s="3"/>
-      <c r="G19" s="2"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="N19" s="8"/>
-    </row>
-    <row r="20" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C20" s="2"/>
-      <c r="E20" s="3"/>
-      <c r="G20" s="2"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="N20" s="8"/>
-    </row>
-    <row r="21" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C21" s="2"/>
-      <c r="E21" s="3"/>
-      <c r="G21" s="2"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="N21" s="8"/>
-    </row>
-    <row r="22" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C22" s="2"/>
-      <c r="E22" s="3"/>
-      <c r="G22" s="2"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="N22" s="8"/>
-    </row>
-    <row r="23" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C23" s="2"/>
-      <c r="E23" s="3"/>
-      <c r="G23" s="2"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="N23" s="8"/>
-    </row>
-    <row r="24" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C24" s="2"/>
-      <c r="E24" s="3"/>
-      <c r="G24" s="2"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="N24" s="8"/>
-    </row>
-    <row r="25" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C25" s="2"/>
-      <c r="E25" s="3"/>
-      <c r="G25" s="2"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="N25" s="8"/>
-    </row>
-    <row r="26" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C26" s="2"/>
-      <c r="E26" s="3"/>
-      <c r="G26" s="2"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="N26" s="8"/>
-    </row>
-    <row r="27" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C27" s="2"/>
-      <c r="E27" s="3"/>
-      <c r="G27" s="2"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
-      <c r="N27" s="8"/>
-    </row>
-    <row r="28" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C28" s="2"/>
-      <c r="E28" s="3"/>
-      <c r="G28" s="2"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-      <c r="N28" s="8"/>
-    </row>
-    <row r="29" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C29" s="2"/>
-      <c r="E29" s="3"/>
-      <c r="G29" s="2"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-      <c r="K29" s="1"/>
-      <c r="N29" s="8"/>
-    </row>
-    <row r="30" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C30" s="2"/>
-      <c r="E30" s="3"/>
-      <c r="G30" s="2"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-      <c r="K30" s="1"/>
-      <c r="N30" s="8"/>
-    </row>
-    <row r="31" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C31" s="2"/>
-      <c r="E31" s="3"/>
-      <c r="G31" s="2"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
-      <c r="K31" s="1"/>
-      <c r="N31" s="8"/>
-    </row>
-    <row r="32" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C32" s="2"/>
-      <c r="E32" s="3"/>
-      <c r="G32" s="2"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
-      <c r="K32" s="1"/>
-      <c r="N32" s="8"/>
-    </row>
-    <row r="33" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C33" s="2"/>
-      <c r="E33" s="3"/>
-      <c r="G33" s="2"/>
-      <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
-      <c r="K33" s="1"/>
-      <c r="N33" s="8"/>
-    </row>
-    <row r="34" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C34" s="2"/>
-      <c r="E34" s="3"/>
-      <c r="G34" s="2"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="1"/>
-      <c r="N34" s="8"/>
-    </row>
-    <row r="35" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C35" s="2"/>
-      <c r="E35" s="3"/>
-      <c r="G35" s="2"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-      <c r="K35" s="1"/>
-      <c r="N35" s="8"/>
-    </row>
-    <row r="36" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C36" s="2"/>
-      <c r="E36" s="3"/>
-      <c r="G36" s="2"/>
-      <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
-      <c r="K36" s="1"/>
-      <c r="N36" s="8"/>
-    </row>
-    <row r="37" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C37" s="2"/>
-      <c r="E37" s="3"/>
-      <c r="G37" s="2"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-      <c r="K37" s="1"/>
-      <c r="N37" s="8"/>
-    </row>
-    <row r="38" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C38" s="2"/>
-      <c r="E38" s="3"/>
-      <c r="G38" s="2"/>
-      <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
-      <c r="K38" s="1"/>
-      <c r="N38" s="8"/>
-    </row>
-    <row r="39" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C39" s="2"/>
-      <c r="E39" s="3"/>
-      <c r="G39" s="2"/>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
-      <c r="K39" s="1"/>
-      <c r="N39" s="8"/>
-    </row>
-    <row r="40" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C40" s="2"/>
-      <c r="E40" s="3"/>
-      <c r="G40" s="2"/>
-      <c r="I40" s="1"/>
-      <c r="J40" s="1"/>
-      <c r="K40" s="1"/>
-      <c r="N40" s="8"/>
-    </row>
-    <row r="41" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C41" s="2"/>
-      <c r="E41" s="3"/>
-      <c r="G41" s="2"/>
-      <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
-      <c r="K41" s="1"/>
-      <c r="N41" s="8"/>
-    </row>
-    <row r="42" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C42" s="2"/>
-      <c r="E42" s="3"/>
-      <c r="G42" s="2"/>
-      <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
-      <c r="K42" s="1"/>
-      <c r="N42" s="8"/>
-    </row>
-    <row r="43" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C43" s="2"/>
-      <c r="E43" s="3"/>
-      <c r="G43" s="2"/>
-      <c r="I43" s="1"/>
-      <c r="J43" s="1"/>
-      <c r="K43" s="1"/>
-      <c r="N43" s="8"/>
-    </row>
-    <row r="44" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C44" s="2"/>
-      <c r="E44" s="3"/>
-      <c r="G44" s="2"/>
-      <c r="I44" s="1"/>
-      <c r="J44" s="1"/>
-      <c r="K44" s="1"/>
-      <c r="N44" s="8"/>
-    </row>
-    <row r="45" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C45" s="2"/>
-      <c r="E45" s="3"/>
-      <c r="G45" s="2"/>
-      <c r="I45" s="1"/>
-      <c r="J45" s="1"/>
-      <c r="K45" s="1"/>
-      <c r="N45" s="8"/>
-    </row>
-    <row r="46" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C46" s="2"/>
-      <c r="E46" s="3"/>
-      <c r="G46" s="2"/>
-      <c r="I46" s="1"/>
-      <c r="J46" s="1"/>
-      <c r="K46" s="1"/>
-      <c r="N46" s="8"/>
-    </row>
-    <row r="47" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C47" s="2"/>
-      <c r="E47" s="3"/>
-      <c r="G47" s="2"/>
-      <c r="I47" s="1"/>
-      <c r="J47" s="1"/>
-      <c r="K47" s="1"/>
-      <c r="N47" s="8"/>
-    </row>
-    <row r="48" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C48" s="2"/>
-      <c r="E48" s="3"/>
-      <c r="G48" s="2"/>
-      <c r="I48" s="1"/>
-      <c r="J48" s="1"/>
-      <c r="K48" s="1"/>
-      <c r="N48" s="8"/>
-    </row>
-    <row r="49" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C49" s="2"/>
-      <c r="E49" s="3"/>
-      <c r="G49" s="2"/>
-      <c r="I49" s="1"/>
-      <c r="J49" s="1"/>
-      <c r="K49" s="1"/>
-      <c r="N49" s="8"/>
-    </row>
-    <row r="50" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C50" s="2"/>
-      <c r="E50" s="3"/>
-      <c r="G50" s="2"/>
-      <c r="I50" s="1"/>
-      <c r="J50" s="1"/>
-      <c r="K50" s="1"/>
-      <c r="N50" s="8"/>
-    </row>
-    <row r="51" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C51" s="2"/>
-      <c r="E51" s="3"/>
-      <c r="G51" s="2"/>
-      <c r="I51" s="1"/>
-      <c r="J51" s="1"/>
-      <c r="K51" s="1"/>
-      <c r="N51" s="8"/>
-    </row>
-    <row r="52" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C52" s="2"/>
-      <c r="E52" s="3"/>
-      <c r="G52" s="2"/>
-      <c r="I52" s="1"/>
-      <c r="J52" s="1"/>
-      <c r="K52" s="1"/>
-      <c r="N52" s="8"/>
-    </row>
-    <row r="53" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C53" s="2"/>
-      <c r="E53" s="3"/>
-      <c r="G53" s="2"/>
-      <c r="I53" s="1"/>
-      <c r="J53" s="1"/>
-      <c r="K53" s="1"/>
-      <c r="N53" s="8"/>
-    </row>
-    <row r="54" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C54" s="2"/>
-      <c r="E54" s="3"/>
-      <c r="G54" s="2"/>
-      <c r="I54" s="1"/>
-      <c r="J54" s="1"/>
-      <c r="K54" s="1"/>
-      <c r="N54" s="8"/>
-    </row>
-    <row r="55" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C55" s="2"/>
-      <c r="E55" s="3"/>
-      <c r="G55" s="2"/>
-      <c r="I55" s="1"/>
-      <c r="J55" s="1"/>
-      <c r="K55" s="1"/>
-      <c r="N55" s="8"/>
-    </row>
-    <row r="56" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C56" s="2"/>
-      <c r="E56" s="3"/>
-      <c r="G56" s="2"/>
-      <c r="I56" s="1"/>
-      <c r="J56" s="1"/>
-      <c r="K56" s="1"/>
-      <c r="N56" s="8"/>
-    </row>
-    <row r="57" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C57" s="2"/>
-      <c r="E57" s="3"/>
-      <c r="G57" s="2"/>
-      <c r="I57" s="1"/>
-      <c r="J57" s="1"/>
-      <c r="K57" s="1"/>
-      <c r="N57" s="8"/>
-    </row>
-    <row r="58" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C58" s="2"/>
-      <c r="E58" s="3"/>
-      <c r="G58" s="2"/>
-      <c r="I58" s="1"/>
-      <c r="J58" s="1"/>
-      <c r="K58" s="1"/>
-      <c r="N58" s="8"/>
-    </row>
-    <row r="59" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C59" s="2"/>
-      <c r="E59" s="3"/>
-      <c r="G59" s="2"/>
-      <c r="I59" s="1"/>
-      <c r="J59" s="1"/>
-      <c r="K59" s="1"/>
-      <c r="N59" s="8"/>
-    </row>
-    <row r="60" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C60" s="2"/>
-      <c r="E60" s="3"/>
-      <c r="G60" s="2"/>
-      <c r="I60" s="1"/>
-      <c r="J60" s="1"/>
-      <c r="K60" s="1"/>
-      <c r="N60" s="8"/>
-    </row>
-    <row r="61" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C61" s="2"/>
-      <c r="E61" s="3"/>
-      <c r="G61" s="2"/>
-      <c r="I61" s="1"/>
-      <c r="J61" s="1"/>
-      <c r="K61" s="1"/>
-      <c r="N61" s="8"/>
-    </row>
-    <row r="62" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C62" s="2"/>
-      <c r="E62" s="3"/>
-      <c r="G62" s="2"/>
-      <c r="I62" s="1"/>
-      <c r="J62" s="1"/>
-      <c r="K62" s="1"/>
-      <c r="N62" s="8"/>
-    </row>
-    <row r="63" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C63" s="2"/>
-      <c r="E63" s="3"/>
-      <c r="G63" s="2"/>
-      <c r="I63" s="1"/>
-      <c r="J63" s="1"/>
-      <c r="K63" s="1"/>
-      <c r="N63" s="8"/>
-    </row>
-    <row r="64" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C64" s="2"/>
-      <c r="E64" s="3"/>
-      <c r="G64" s="2"/>
-      <c r="I64" s="1"/>
-      <c r="J64" s="1"/>
-      <c r="K64" s="1"/>
-      <c r="N64" s="8"/>
-    </row>
-    <row r="65" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C65" s="2"/>
-      <c r="E65" s="3"/>
-      <c r="G65" s="2"/>
-      <c r="I65" s="1"/>
-      <c r="J65" s="1"/>
-      <c r="K65" s="1"/>
-      <c r="N65" s="8"/>
-    </row>
-    <row r="66" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C66" s="2"/>
-      <c r="E66" s="3"/>
-      <c r="G66" s="2"/>
-      <c r="I66" s="1"/>
-      <c r="J66" s="1"/>
-      <c r="K66" s="1"/>
-      <c r="N66" s="8"/>
-    </row>
-    <row r="67" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C67" s="2"/>
-      <c r="E67" s="3"/>
-      <c r="G67" s="2"/>
-      <c r="I67" s="1"/>
-      <c r="J67" s="1"/>
-      <c r="K67" s="1"/>
-      <c r="N67" s="8"/>
-    </row>
-    <row r="68" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C68" s="2"/>
-      <c r="E68" s="3"/>
-      <c r="G68" s="2"/>
-      <c r="I68" s="1"/>
-      <c r="J68" s="1"/>
-      <c r="K68" s="1"/>
-      <c r="N68" s="8"/>
-    </row>
-    <row r="69" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C69" s="2"/>
-      <c r="E69" s="3"/>
-      <c r="G69" s="2"/>
-      <c r="I69" s="1"/>
-      <c r="J69" s="1"/>
-      <c r="K69" s="1"/>
-      <c r="N69" s="8"/>
-    </row>
-    <row r="70" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C70" s="2"/>
-      <c r="E70" s="3"/>
-      <c r="G70" s="2"/>
-      <c r="I70" s="1"/>
-      <c r="J70" s="1"/>
-      <c r="K70" s="1"/>
-      <c r="N70" s="8"/>
-    </row>
-    <row r="71" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C71" s="2"/>
-      <c r="E71" s="3"/>
-      <c r="G71" s="2"/>
-      <c r="I71" s="1"/>
-      <c r="J71" s="1"/>
-      <c r="K71" s="1"/>
-      <c r="N71" s="8"/>
-    </row>
-    <row r="72" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C72" s="2"/>
-      <c r="E72" s="3"/>
-      <c r="G72" s="2"/>
-      <c r="I72" s="1"/>
-      <c r="J72" s="1"/>
-      <c r="K72" s="1"/>
-      <c r="N72" s="8"/>
-    </row>
-    <row r="73" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C73" s="2"/>
-      <c r="E73" s="3"/>
-      <c r="G73" s="2"/>
-      <c r="I73" s="1"/>
-      <c r="J73" s="1"/>
-      <c r="K73" s="1"/>
-      <c r="N73" s="8"/>
-    </row>
-    <row r="74" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C74" s="2"/>
-      <c r="E74" s="3"/>
-      <c r="G74" s="2"/>
-      <c r="I74" s="1"/>
-      <c r="J74" s="1"/>
-      <c r="K74" s="1"/>
-      <c r="N74" s="8"/>
-    </row>
-    <row r="75" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C75" s="2"/>
-      <c r="E75" s="3"/>
-      <c r="G75" s="2"/>
-      <c r="I75" s="1"/>
-      <c r="J75" s="1"/>
-      <c r="K75" s="1"/>
-      <c r="N75" s="8"/>
-    </row>
-    <row r="76" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C76" s="2"/>
-      <c r="E76" s="3"/>
-      <c r="G76" s="2"/>
-      <c r="I76" s="1"/>
-      <c r="J76" s="1"/>
-      <c r="K76" s="1"/>
-      <c r="N76" s="8"/>
-    </row>
-    <row r="77" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C77" s="2"/>
-      <c r="E77" s="3"/>
-      <c r="G77" s="2"/>
-      <c r="I77" s="1"/>
-      <c r="J77" s="1"/>
-      <c r="K77" s="1"/>
-      <c r="N77" s="8"/>
-    </row>
-    <row r="78" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C78" s="2"/>
-      <c r="E78" s="3"/>
-      <c r="G78" s="2"/>
-      <c r="I78" s="1"/>
-      <c r="J78" s="1"/>
-      <c r="K78" s="1"/>
-      <c r="N78" s="8"/>
-    </row>
-    <row r="79" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C79" s="2"/>
-      <c r="E79" s="3"/>
-      <c r="G79" s="2"/>
-      <c r="I79" s="1"/>
-      <c r="J79" s="1"/>
-      <c r="K79" s="1"/>
-      <c r="N79" s="8"/>
-    </row>
-    <row r="80" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C80" s="2"/>
-      <c r="E80" s="3"/>
-      <c r="G80" s="2"/>
-      <c r="I80" s="1"/>
-      <c r="J80" s="1"/>
-      <c r="K80" s="1"/>
-      <c r="N80" s="8"/>
-    </row>
-    <row r="81" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C81" s="2"/>
-      <c r="E81" s="3"/>
-      <c r="G81" s="2"/>
-      <c r="I81" s="1"/>
-      <c r="J81" s="1"/>
-      <c r="K81" s="1"/>
-      <c r="N81" s="8"/>
-    </row>
-    <row r="82" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C82" s="2"/>
-      <c r="E82" s="3"/>
-      <c r="G82" s="2"/>
-      <c r="I82" s="1"/>
-      <c r="J82" s="1"/>
-      <c r="K82" s="1"/>
-      <c r="N82" s="8"/>
-    </row>
-    <row r="83" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C83" s="2"/>
-      <c r="E83" s="3"/>
-      <c r="G83" s="2"/>
-      <c r="I83" s="1"/>
-      <c r="J83" s="1"/>
-      <c r="K83" s="1"/>
-      <c r="N83" s="8"/>
-    </row>
-    <row r="84" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C84" s="2"/>
-      <c r="E84" s="3"/>
-      <c r="G84" s="2"/>
-      <c r="I84" s="1"/>
-      <c r="J84" s="1"/>
-      <c r="K84" s="1"/>
-      <c r="N84" s="8"/>
-    </row>
-    <row r="85" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C85" s="2"/>
-      <c r="E85" s="3"/>
-      <c r="G85" s="2"/>
-      <c r="I85" s="1"/>
-      <c r="J85" s="1"/>
-      <c r="K85" s="1"/>
-      <c r="N85" s="8"/>
-    </row>
-    <row r="86" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C86" s="2"/>
-      <c r="E86" s="3"/>
-      <c r="G86" s="2"/>
-      <c r="I86" s="1"/>
-      <c r="J86" s="1"/>
-      <c r="K86" s="1"/>
-      <c r="N86" s="8"/>
-    </row>
-    <row r="87" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C87" s="2"/>
-      <c r="E87" s="3"/>
-      <c r="G87" s="2"/>
-      <c r="I87" s="1"/>
-      <c r="J87" s="1"/>
-      <c r="K87" s="1"/>
-      <c r="N87" s="8"/>
-    </row>
-    <row r="88" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C88" s="2"/>
-      <c r="E88" s="3"/>
-      <c r="G88" s="2"/>
-      <c r="I88" s="1"/>
-      <c r="J88" s="1"/>
-      <c r="K88" s="1"/>
-      <c r="N88" s="8"/>
-    </row>
-    <row r="89" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C89" s="2"/>
-      <c r="E89" s="3"/>
-      <c r="G89" s="2"/>
-      <c r="I89" s="1"/>
-      <c r="J89" s="1"/>
-      <c r="K89" s="1"/>
-      <c r="N89" s="8"/>
-    </row>
-    <row r="90" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C90" s="2"/>
-      <c r="E90" s="3"/>
-      <c r="G90" s="2"/>
-      <c r="I90" s="1"/>
-      <c r="J90" s="1"/>
-      <c r="K90" s="1"/>
-      <c r="N90" s="8"/>
-    </row>
-    <row r="91" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C91" s="2"/>
-      <c r="E91" s="3"/>
-      <c r="G91" s="2"/>
-      <c r="I91" s="1"/>
-      <c r="J91" s="1"/>
-      <c r="K91" s="1"/>
-      <c r="N91" s="8"/>
-    </row>
-    <row r="92" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C92" s="2"/>
-      <c r="E92" s="3"/>
-      <c r="G92" s="2"/>
-      <c r="I92" s="1"/>
-      <c r="J92" s="1"/>
-      <c r="K92" s="1"/>
-      <c r="N92" s="8"/>
-    </row>
-    <row r="93" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C93" s="2"/>
-      <c r="E93" s="3"/>
-      <c r="G93" s="2"/>
-      <c r="I93" s="1"/>
-      <c r="J93" s="1"/>
-      <c r="K93" s="1"/>
-      <c r="N93" s="8"/>
-    </row>
-    <row r="94" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C94" s="2"/>
-      <c r="E94" s="3"/>
-      <c r="G94" s="2"/>
-      <c r="I94" s="1"/>
-      <c r="J94" s="1"/>
-      <c r="K94" s="1"/>
-      <c r="N94" s="8"/>
-    </row>
-    <row r="95" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C95" s="2"/>
-      <c r="E95" s="3"/>
-      <c r="G95" s="2"/>
-      <c r="I95" s="1"/>
-      <c r="J95" s="1"/>
-      <c r="K95" s="1"/>
-      <c r="N95" s="8"/>
-    </row>
-    <row r="96" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C96" s="2"/>
-      <c r="E96" s="3"/>
-      <c r="G96" s="2"/>
-      <c r="I96" s="1"/>
-      <c r="J96" s="1"/>
-      <c r="K96" s="1"/>
-      <c r="N96" s="8"/>
-    </row>
-    <row r="97" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C97" s="2"/>
-      <c r="E97" s="3"/>
-      <c r="G97" s="2"/>
-      <c r="I97" s="1"/>
-      <c r="J97" s="1"/>
-      <c r="K97" s="1"/>
-      <c r="N97" s="8"/>
-    </row>
-    <row r="98" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C98" s="2"/>
-      <c r="E98" s="3"/>
-      <c r="G98" s="2"/>
-      <c r="I98" s="1"/>
-      <c r="J98" s="1"/>
-      <c r="K98" s="1"/>
-      <c r="N98" s="8"/>
-    </row>
-    <row r="99" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C99" s="2"/>
-      <c r="E99" s="3"/>
-      <c r="G99" s="2"/>
-      <c r="I99" s="1"/>
-      <c r="J99" s="1"/>
-      <c r="K99" s="1"/>
-      <c r="N99" s="8"/>
-    </row>
-    <row r="100" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C100" s="2"/>
-      <c r="E100" s="3"/>
-      <c r="G100" s="2"/>
-      <c r="I100" s="1"/>
-      <c r="J100" s="1"/>
-      <c r="K100" s="1"/>
-      <c r="N100" s="8"/>
-    </row>
-    <row r="101" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C101" s="2"/>
-      <c r="G101" s="2"/>
-    </row>
-    <row r="102" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C102" s="2"/>
-      <c r="G102" s="2"/>
-    </row>
-    <row r="103" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C103" s="2"/>
-      <c r="G103" s="2"/>
-    </row>
-    <row r="104" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C104" s="2"/>
-      <c r="G104" s="2"/>
-    </row>
-    <row r="105" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C105" s="2"/>
-      <c r="G105" s="2"/>
-    </row>
-    <row r="106" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C106" s="2"/>
-      <c r="G106" s="2"/>
-    </row>
-    <row r="107" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C107" s="2"/>
-      <c r="G107" s="2"/>
-    </row>
-    <row r="108" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C108" s="2"/>
-      <c r="G108" s="2"/>
-    </row>
-    <row r="109" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C109" s="2"/>
-      <c r="G109" s="2"/>
-    </row>
-    <row r="110" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C110" s="2"/>
-      <c r="G110" s="2"/>
-    </row>
-    <row r="111" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C111" s="2"/>
-      <c r="G111" s="2"/>
-    </row>
-    <row r="112" spans="3:14" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C112" s="2"/>
-      <c r="G112" s="2"/>
-    </row>
-    <row r="113" spans="4:4" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D113" s="3"/>
-    </row>
-    <row r="114" spans="4:4" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D114" s="3"/>
-    </row>
-    <row r="115" spans="4:4" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D115" s="3"/>
-    </row>
-    <row r="116" spans="4:4" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D116" s="3"/>
-    </row>
-    <row r="117" spans="4:4" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D117" s="3"/>
-    </row>
-    <row r="118" spans="4:4" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D118" s="3"/>
-    </row>
-    <row r="119" spans="4:4" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D119" s="3"/>
-    </row>
-    <row r="120" spans="4:4" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D120" s="3"/>
-    </row>
-    <row r="121" spans="4:4" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D121" s="3"/>
-    </row>
-    <row r="122" spans="4:4" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D122" s="3"/>
-    </row>
-    <row r="123" spans="4:4" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D123" s="3"/>
-    </row>
-    <row r="124" spans="4:4" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D124" s="3"/>
-    </row>
-    <row r="125" spans="4:4" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D125" s="3"/>
-    </row>
-    <row r="126" spans="4:4" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D126" s="3"/>
-    </row>
-    <row r="127" spans="4:4" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D127" s="3"/>
-    </row>
-    <row r="128" spans="4:4" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D128" s="3"/>
-    </row>
-    <row r="129" spans="4:4" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D129" s="3"/>
-    </row>
-    <row r="130" spans="4:4" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D130" s="3"/>
-    </row>
-    <row r="131" spans="4:4" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D131" s="3"/>
-    </row>
-    <row r="132" spans="4:4" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D132" s="3"/>
-    </row>
-    <row r="133" spans="4:4" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D133" s="3"/>
-    </row>
-    <row r="134" spans="4:4" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D134" s="3"/>
-    </row>
-    <row r="135" spans="4:4" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D135" s="3"/>
-    </row>
-    <row r="136" spans="4:4" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D136" s="3"/>
-    </row>
-    <row r="137" spans="4:4" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D137" s="3"/>
-    </row>
-    <row r="138" spans="4:4" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D138" s="3"/>
-    </row>
-    <row r="139" spans="4:4" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D139" s="3"/>
-    </row>
-    <row r="140" spans="4:4" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D140" s="3"/>
-    </row>
-    <row r="141" spans="4:4" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D141" s="3"/>
-    </row>
-    <row r="142" spans="4:4" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D142" s="3"/>
-    </row>
-    <row r="143" spans="4:4" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D143" s="3"/>
-    </row>
-    <row r="144" spans="4:4" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D144" s="3"/>
-    </row>
-    <row r="145" spans="4:4" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D145" s="3"/>
-    </row>
-    <row r="146" spans="4:4" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D146" s="3"/>
-    </row>
-    <row r="147" spans="4:4" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D147" s="3"/>
-    </row>
-    <row r="148" spans="4:4" s="2" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D148" s="3"/>
-    </row>
-  </sheetData>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4521,7 +3420,7 @@
   <dimension ref="A1:EK112"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+      <selection activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.7109375" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4543,15 +3442,15 @@
     <row r="1" spans="1:141" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10"/>
       <c r="B1" s="10"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="38" t="s">
-        <v>828</v>
-      </c>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="K1" s="46" t="s">
-        <v>835</v>
+      <c r="D1" s="35"/>
+      <c r="E1" s="44" t="s">
+        <v>827</v>
+      </c>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
+      <c r="H1" s="44"/>
+      <c r="K1" s="36" t="s">
+        <v>833</v>
       </c>
       <c r="M1" s="12"/>
       <c r="S1" s="13"/>
@@ -4679,12 +3578,12 @@
       <c r="EK1" s="13"/>
     </row>
     <row r="2" spans="1:141" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D2" s="45"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="K2" s="46" t="s">
+      <c r="D2" s="35"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="K2" s="36" t="s">
         <v>2</v>
       </c>
       <c r="M2" s="12"/>
@@ -4817,14 +3716,14 @@
         <v>1</v>
       </c>
       <c r="B3" s="14"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="38"/>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="J3" s="47"/>
-      <c r="K3" s="47"/>
-      <c r="L3" s="47"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="44"/>
+      <c r="F3" s="44"/>
+      <c r="G3" s="44"/>
+      <c r="H3" s="44"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="37"/>
+      <c r="L3" s="37"/>
       <c r="M3" s="12"/>
       <c r="S3" s="13"/>
       <c r="T3" s="13"/>
@@ -4951,13 +3850,13 @@
       <c r="EK3" s="13"/>
     </row>
     <row r="4" spans="1:141" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D4" s="45"/>
-      <c r="E4" s="48"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="48"/>
-      <c r="H4" s="48"/>
-      <c r="J4" s="46"/>
-      <c r="K4" s="46"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="36"/>
       <c r="S4" s="13"/>
       <c r="T4" s="13"/>
       <c r="U4" s="13"/>
@@ -5083,27 +3982,27 @@
       <c r="EK4" s="13"/>
     </row>
     <row r="5" spans="1:141" s="4" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="42" t="s">
+      <c r="A5" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="42"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="42" t="s">
+      <c r="B5" s="48"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="42"/>
-      <c r="H5" s="42" t="s">
+      <c r="G5" s="48"/>
+      <c r="H5" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="42"/>
-      <c r="J5" s="42" t="s">
+      <c r="I5" s="48"/>
+      <c r="J5" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="42"/>
-      <c r="L5" s="42"/>
-      <c r="M5" s="42"/>
+      <c r="K5" s="48"/>
+      <c r="L5" s="48"/>
+      <c r="M5" s="48"/>
       <c r="N5" s="15"/>
       <c r="S5" s="16"/>
       <c r="T5" s="16"/>
@@ -5230,19 +4129,19 @@
       <c r="EK5" s="16"/>
     </row>
     <row r="6" spans="1:141" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="41"/>
-      <c r="B6" s="41"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="41"/>
+      <c r="A6" s="47"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
       <c r="E6" s="31"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="41"/>
-      <c r="H6" s="41"/>
-      <c r="I6" s="41"/>
-      <c r="J6" s="41"/>
-      <c r="K6" s="41"/>
-      <c r="L6" s="41"/>
-      <c r="M6" s="41"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
+      <c r="J6" s="47"/>
+      <c r="K6" s="47"/>
+      <c r="L6" s="47"/>
+      <c r="M6" s="47"/>
       <c r="N6" s="17"/>
       <c r="S6" s="13"/>
       <c r="T6" s="13"/>
@@ -5369,34 +4268,34 @@
       <c r="EK6" s="13"/>
     </row>
     <row r="7" spans="1:141" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="41"/>
-      <c r="B7" s="41"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
+      <c r="A7" s="47"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
       <c r="E7" s="31"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="41"/>
-      <c r="H7" s="41"/>
-      <c r="I7" s="41"/>
-      <c r="J7" s="41"/>
-      <c r="K7" s="41"/>
-      <c r="L7" s="41"/>
-      <c r="M7" s="41"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="47"/>
+      <c r="J7" s="47"/>
+      <c r="K7" s="47"/>
+      <c r="L7" s="47"/>
+      <c r="M7" s="47"/>
     </row>
     <row r="8" spans="1:141" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="41"/>
-      <c r="B8" s="41"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
+      <c r="A8" s="47"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
       <c r="E8" s="31"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="41"/>
-      <c r="H8" s="41"/>
-      <c r="I8" s="41"/>
-      <c r="J8" s="41"/>
-      <c r="K8" s="41"/>
-      <c r="L8" s="41"/>
-      <c r="M8" s="41"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="47"/>
+      <c r="I8" s="47"/>
+      <c r="J8" s="47"/>
+      <c r="K8" s="47"/>
+      <c r="L8" s="47"/>
+      <c r="M8" s="47"/>
     </row>
     <row r="9" spans="1:141" s="13" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="18"/>
@@ -5414,46 +4313,46 @@
       <c r="M9" s="19"/>
     </row>
     <row r="10" spans="1:141" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="39" t="s">
+      <c r="A10" s="45" t="s">
         <v>416</v>
       </c>
-      <c r="B10" s="43"/>
-      <c r="C10" s="39" t="s">
+      <c r="B10" s="49"/>
+      <c r="C10" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="39" t="s">
+      <c r="D10" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="39"/>
+      <c r="E10" s="45"/>
       <c r="F10" s="30" t="s">
         <v>0</v>
       </c>
       <c r="G10" s="22" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="H10" s="21" t="s">
+        <v>828</v>
+      </c>
+      <c r="I10" s="21" t="s">
         <v>829</v>
       </c>
-      <c r="I10" s="21" t="s">
+      <c r="J10" s="21" t="s">
+        <v>832</v>
+      </c>
+      <c r="K10" s="21" t="s">
         <v>830</v>
       </c>
-      <c r="J10" s="21" t="s">
-        <v>834</v>
-      </c>
-      <c r="K10" s="21" t="s">
-        <v>831</v>
-      </c>
       <c r="L10" s="22"/>
-      <c r="M10" s="39" t="s">
+      <c r="M10" s="45" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:141" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="40"/>
-      <c r="B11" s="44"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40"/>
+      <c r="A11" s="46"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="46"/>
+      <c r="D11" s="46"/>
+      <c r="E11" s="46"/>
       <c r="F11" s="23" t="s">
         <v>5</v>
       </c>
@@ -5463,7 +4362,7 @@
       <c r="H11" s="24" t="s">
         <v>417</v>
       </c>
-      <c r="I11" s="50" t="s">
+      <c r="I11" s="40" t="s">
         <v>417</v>
       </c>
       <c r="J11" s="24" t="s">
@@ -5471,14 +4370,14 @@
       </c>
       <c r="K11" s="24"/>
       <c r="L11" s="24"/>
-      <c r="M11" s="40"/>
+      <c r="M11" s="46"/>
     </row>
     <row r="12" spans="1:141" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="32"/>
       <c r="B12" s="32"/>
       <c r="C12" s="32"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="32"/>
       <c r="G12" s="32"/>
       <c r="H12" s="32"/>
@@ -5492,8 +4391,8 @@
       <c r="A13" s="32"/>
       <c r="B13" s="32"/>
       <c r="C13" s="32"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
       <c r="F13" s="32"/>
       <c r="G13" s="32"/>
       <c r="H13" s="32"/>
@@ -5507,8 +4406,8 @@
       <c r="A14" s="32"/>
       <c r="B14" s="32"/>
       <c r="C14" s="32"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="35"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
       <c r="F14" s="32"/>
       <c r="G14" s="32"/>
       <c r="H14" s="32"/>
@@ -5522,8 +4421,8 @@
       <c r="A15" s="32"/>
       <c r="B15" s="32"/>
       <c r="C15" s="32"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
       <c r="F15" s="32"/>
       <c r="G15" s="32"/>
       <c r="H15" s="32"/>
@@ -5537,8 +4436,8 @@
       <c r="A16" s="32"/>
       <c r="B16" s="32"/>
       <c r="C16" s="32"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="35"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
       <c r="F16" s="32"/>
       <c r="G16" s="32"/>
       <c r="H16" s="32"/>
@@ -5552,8 +4451,8 @@
       <c r="A17" s="32"/>
       <c r="B17" s="32"/>
       <c r="C17" s="32"/>
-      <c r="D17" s="35"/>
-      <c r="E17" s="35"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
       <c r="F17" s="32"/>
       <c r="G17" s="32"/>
       <c r="H17" s="32"/>
@@ -5567,8 +4466,8 @@
       <c r="A18" s="32"/>
       <c r="B18" s="32"/>
       <c r="C18" s="32"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
       <c r="F18" s="32"/>
       <c r="G18" s="32"/>
       <c r="H18" s="32"/>
@@ -5582,8 +4481,8 @@
       <c r="A19" s="32"/>
       <c r="B19" s="32"/>
       <c r="C19" s="32"/>
-      <c r="D19" s="35"/>
-      <c r="E19" s="35"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
       <c r="F19" s="32"/>
       <c r="G19" s="32"/>
       <c r="H19" s="32"/>
@@ -5597,8 +4496,8 @@
       <c r="A20" s="32"/>
       <c r="B20" s="32"/>
       <c r="C20" s="32"/>
-      <c r="D20" s="35"/>
-      <c r="E20" s="35"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="41"/>
       <c r="F20" s="32"/>
       <c r="G20" s="32"/>
       <c r="H20" s="32"/>
@@ -5612,8 +4511,8 @@
       <c r="A21" s="32"/>
       <c r="B21" s="32"/>
       <c r="C21" s="32"/>
-      <c r="D21" s="35"/>
-      <c r="E21" s="35"/>
+      <c r="D21" s="41"/>
+      <c r="E21" s="41"/>
       <c r="F21" s="32"/>
       <c r="G21" s="32"/>
       <c r="H21" s="32"/>
@@ -5627,8 +4526,8 @@
       <c r="A22" s="32"/>
       <c r="B22" s="32"/>
       <c r="C22" s="32"/>
-      <c r="D22" s="35"/>
-      <c r="E22" s="35"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="41"/>
       <c r="F22" s="32"/>
       <c r="G22" s="32"/>
       <c r="H22" s="32"/>
@@ -5642,8 +4541,8 @@
       <c r="A23" s="32"/>
       <c r="B23" s="32"/>
       <c r="C23" s="32"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="35"/>
+      <c r="D23" s="41"/>
+      <c r="E23" s="41"/>
       <c r="F23" s="32"/>
       <c r="G23" s="32"/>
       <c r="H23" s="32"/>
@@ -5657,8 +4556,8 @@
       <c r="A24" s="32"/>
       <c r="B24" s="32"/>
       <c r="C24" s="32"/>
-      <c r="D24" s="35"/>
-      <c r="E24" s="35"/>
+      <c r="D24" s="41"/>
+      <c r="E24" s="41"/>
       <c r="F24" s="32"/>
       <c r="G24" s="32"/>
       <c r="H24" s="32"/>
@@ -5672,8 +4571,8 @@
       <c r="A25" s="32"/>
       <c r="B25" s="32"/>
       <c r="C25" s="32"/>
-      <c r="D25" s="35"/>
-      <c r="E25" s="35"/>
+      <c r="D25" s="41"/>
+      <c r="E25" s="41"/>
       <c r="F25" s="32"/>
       <c r="G25" s="32"/>
       <c r="H25" s="32"/>
@@ -5687,8 +4586,8 @@
       <c r="A26" s="32"/>
       <c r="B26" s="32"/>
       <c r="C26" s="32"/>
-      <c r="D26" s="35"/>
-      <c r="E26" s="35"/>
+      <c r="D26" s="41"/>
+      <c r="E26" s="41"/>
       <c r="F26" s="32"/>
       <c r="G26" s="32"/>
       <c r="H26" s="32"/>
@@ -5702,8 +4601,8 @@
       <c r="A27" s="32"/>
       <c r="B27" s="32"/>
       <c r="C27" s="32"/>
-      <c r="D27" s="35"/>
-      <c r="E27" s="35"/>
+      <c r="D27" s="41"/>
+      <c r="E27" s="41"/>
       <c r="F27" s="32"/>
       <c r="G27" s="32"/>
       <c r="H27" s="32"/>
@@ -5717,8 +4616,8 @@
       <c r="A28" s="32"/>
       <c r="B28" s="32"/>
       <c r="C28" s="32"/>
-      <c r="D28" s="35"/>
-      <c r="E28" s="35"/>
+      <c r="D28" s="41"/>
+      <c r="E28" s="41"/>
       <c r="F28" s="32"/>
       <c r="G28" s="32"/>
       <c r="H28" s="32"/>
@@ -5732,8 +4631,8 @@
       <c r="A29" s="32"/>
       <c r="B29" s="32"/>
       <c r="C29" s="32"/>
-      <c r="D29" s="35"/>
-      <c r="E29" s="35"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="41"/>
       <c r="F29" s="32"/>
       <c r="G29" s="32"/>
       <c r="H29" s="32"/>
@@ -5747,8 +4646,8 @@
       <c r="A30" s="32"/>
       <c r="B30" s="32"/>
       <c r="C30" s="32"/>
-      <c r="D30" s="35"/>
-      <c r="E30" s="35"/>
+      <c r="D30" s="41"/>
+      <c r="E30" s="41"/>
       <c r="F30" s="32"/>
       <c r="G30" s="32"/>
       <c r="H30" s="32"/>
@@ -5762,8 +4661,8 @@
       <c r="A31" s="32"/>
       <c r="B31" s="32"/>
       <c r="C31" s="32"/>
-      <c r="D31" s="35"/>
-      <c r="E31" s="35"/>
+      <c r="D31" s="41"/>
+      <c r="E31" s="41"/>
       <c r="F31" s="32"/>
       <c r="G31" s="32"/>
       <c r="H31" s="32"/>
@@ -5777,8 +4676,8 @@
       <c r="A32" s="32"/>
       <c r="B32" s="32"/>
       <c r="C32" s="32"/>
-      <c r="D32" s="35"/>
-      <c r="E32" s="35"/>
+      <c r="D32" s="41"/>
+      <c r="E32" s="41"/>
       <c r="F32" s="32"/>
       <c r="G32" s="32"/>
       <c r="H32" s="32"/>
@@ -5792,8 +4691,8 @@
       <c r="A33" s="32"/>
       <c r="B33" s="32"/>
       <c r="C33" s="32"/>
-      <c r="D33" s="35"/>
-      <c r="E33" s="35"/>
+      <c r="D33" s="41"/>
+      <c r="E33" s="41"/>
       <c r="F33" s="32"/>
       <c r="G33" s="32"/>
       <c r="H33" s="32"/>
@@ -5807,8 +4706,8 @@
       <c r="A34" s="32"/>
       <c r="B34" s="32"/>
       <c r="C34" s="32"/>
-      <c r="D34" s="35"/>
-      <c r="E34" s="35"/>
+      <c r="D34" s="41"/>
+      <c r="E34" s="41"/>
       <c r="F34" s="32"/>
       <c r="G34" s="32"/>
       <c r="H34" s="32"/>
@@ -5822,8 +4721,8 @@
       <c r="A35" s="32"/>
       <c r="B35" s="32"/>
       <c r="C35" s="32"/>
-      <c r="D35" s="35"/>
-      <c r="E35" s="35"/>
+      <c r="D35" s="41"/>
+      <c r="E35" s="41"/>
       <c r="F35" s="32"/>
       <c r="G35" s="32"/>
       <c r="H35" s="32"/>
@@ -5837,8 +4736,8 @@
       <c r="A36" s="32"/>
       <c r="B36" s="32"/>
       <c r="C36" s="32"/>
-      <c r="D36" s="35"/>
-      <c r="E36" s="35"/>
+      <c r="D36" s="41"/>
+      <c r="E36" s="41"/>
       <c r="F36" s="32"/>
       <c r="G36" s="32"/>
       <c r="H36" s="32"/>
@@ -5852,8 +4751,8 @@
       <c r="A37" s="32"/>
       <c r="B37" s="32"/>
       <c r="C37" s="32"/>
-      <c r="D37" s="35"/>
-      <c r="E37" s="35"/>
+      <c r="D37" s="41"/>
+      <c r="E37" s="41"/>
       <c r="F37" s="32"/>
       <c r="G37" s="32"/>
       <c r="H37" s="32"/>
@@ -5867,8 +4766,8 @@
       <c r="A38" s="32"/>
       <c r="B38" s="32"/>
       <c r="C38" s="32"/>
-      <c r="D38" s="35"/>
-      <c r="E38" s="35"/>
+      <c r="D38" s="41"/>
+      <c r="E38" s="41"/>
       <c r="F38" s="32"/>
       <c r="G38" s="32"/>
       <c r="H38" s="32"/>
@@ -5882,8 +4781,8 @@
       <c r="A39" s="32"/>
       <c r="B39" s="32"/>
       <c r="C39" s="32"/>
-      <c r="D39" s="35"/>
-      <c r="E39" s="35"/>
+      <c r="D39" s="41"/>
+      <c r="E39" s="41"/>
       <c r="F39" s="32"/>
       <c r="G39" s="32"/>
       <c r="H39" s="32"/>
@@ -5897,8 +4796,8 @@
       <c r="A40" s="32"/>
       <c r="B40" s="32"/>
       <c r="C40" s="32"/>
-      <c r="D40" s="35"/>
-      <c r="E40" s="35"/>
+      <c r="D40" s="41"/>
+      <c r="E40" s="41"/>
       <c r="F40" s="32"/>
       <c r="G40" s="32"/>
       <c r="H40" s="32"/>
@@ -5912,8 +4811,8 @@
       <c r="A41" s="32"/>
       <c r="B41" s="32"/>
       <c r="C41" s="32"/>
-      <c r="D41" s="35"/>
-      <c r="E41" s="35"/>
+      <c r="D41" s="41"/>
+      <c r="E41" s="41"/>
       <c r="F41" s="32"/>
       <c r="G41" s="32"/>
       <c r="H41" s="32"/>
@@ -5927,8 +4826,8 @@
       <c r="A42" s="32"/>
       <c r="B42" s="32"/>
       <c r="C42" s="32"/>
-      <c r="D42" s="35"/>
-      <c r="E42" s="35"/>
+      <c r="D42" s="41"/>
+      <c r="E42" s="41"/>
       <c r="F42" s="32"/>
       <c r="G42" s="32"/>
       <c r="H42" s="32"/>
@@ -5942,8 +4841,8 @@
       <c r="A43" s="32"/>
       <c r="B43" s="32"/>
       <c r="C43" s="32"/>
-      <c r="D43" s="35"/>
-      <c r="E43" s="35"/>
+      <c r="D43" s="41"/>
+      <c r="E43" s="41"/>
       <c r="F43" s="32"/>
       <c r="G43" s="32"/>
       <c r="H43" s="32"/>
@@ -5957,8 +4856,8 @@
       <c r="A44" s="32"/>
       <c r="B44" s="32"/>
       <c r="C44" s="32"/>
-      <c r="D44" s="35"/>
-      <c r="E44" s="35"/>
+      <c r="D44" s="41"/>
+      <c r="E44" s="41"/>
       <c r="F44" s="32"/>
       <c r="G44" s="32"/>
       <c r="H44" s="32"/>
@@ -5972,8 +4871,8 @@
       <c r="A45" s="32"/>
       <c r="B45" s="32"/>
       <c r="C45" s="32"/>
-      <c r="D45" s="35"/>
-      <c r="E45" s="35"/>
+      <c r="D45" s="41"/>
+      <c r="E45" s="41"/>
       <c r="F45" s="32"/>
       <c r="G45" s="32"/>
       <c r="H45" s="32"/>
@@ -5987,8 +4886,8 @@
       <c r="A46" s="32"/>
       <c r="B46" s="32"/>
       <c r="C46" s="32"/>
-      <c r="D46" s="35"/>
-      <c r="E46" s="35"/>
+      <c r="D46" s="41"/>
+      <c r="E46" s="41"/>
       <c r="F46" s="32"/>
       <c r="G46" s="32"/>
       <c r="H46" s="32"/>
@@ -6002,8 +4901,8 @@
       <c r="A47" s="32"/>
       <c r="B47" s="32"/>
       <c r="C47" s="32"/>
-      <c r="D47" s="35"/>
-      <c r="E47" s="35"/>
+      <c r="D47" s="41"/>
+      <c r="E47" s="41"/>
       <c r="F47" s="32"/>
       <c r="G47" s="32"/>
       <c r="H47" s="32"/>
@@ -6017,8 +4916,8 @@
       <c r="A48" s="32"/>
       <c r="B48" s="32"/>
       <c r="C48" s="32"/>
-      <c r="D48" s="35"/>
-      <c r="E48" s="35"/>
+      <c r="D48" s="41"/>
+      <c r="E48" s="41"/>
       <c r="F48" s="32"/>
       <c r="G48" s="32"/>
       <c r="H48" s="32"/>
@@ -6032,8 +4931,8 @@
       <c r="A49" s="32"/>
       <c r="B49" s="32"/>
       <c r="C49" s="32"/>
-      <c r="D49" s="35"/>
-      <c r="E49" s="35"/>
+      <c r="D49" s="41"/>
+      <c r="E49" s="41"/>
       <c r="F49" s="32"/>
       <c r="G49" s="32"/>
       <c r="H49" s="32"/>
@@ -6047,8 +4946,8 @@
       <c r="A50" s="32"/>
       <c r="B50" s="32"/>
       <c r="C50" s="32"/>
-      <c r="D50" s="35"/>
-      <c r="E50" s="35"/>
+      <c r="D50" s="41"/>
+      <c r="E50" s="41"/>
       <c r="F50" s="32"/>
       <c r="G50" s="32"/>
       <c r="H50" s="32"/>
@@ -6062,8 +4961,8 @@
       <c r="A51" s="32"/>
       <c r="B51" s="32"/>
       <c r="C51" s="32"/>
-      <c r="D51" s="35"/>
-      <c r="E51" s="35"/>
+      <c r="D51" s="41"/>
+      <c r="E51" s="41"/>
       <c r="F51" s="32"/>
       <c r="G51" s="32"/>
       <c r="H51" s="32"/>
@@ -6077,8 +4976,8 @@
       <c r="A52" s="32"/>
       <c r="B52" s="32"/>
       <c r="C52" s="32"/>
-      <c r="D52" s="35"/>
-      <c r="E52" s="35"/>
+      <c r="D52" s="41"/>
+      <c r="E52" s="41"/>
       <c r="F52" s="32"/>
       <c r="G52" s="32"/>
       <c r="H52" s="32"/>
@@ -6092,8 +4991,8 @@
       <c r="A53" s="32"/>
       <c r="B53" s="32"/>
       <c r="C53" s="32"/>
-      <c r="D53" s="35"/>
-      <c r="E53" s="35"/>
+      <c r="D53" s="41"/>
+      <c r="E53" s="41"/>
       <c r="F53" s="32"/>
       <c r="G53" s="32"/>
       <c r="H53" s="32"/>
@@ -6107,8 +5006,8 @@
       <c r="A54" s="32"/>
       <c r="B54" s="32"/>
       <c r="C54" s="32"/>
-      <c r="D54" s="35"/>
-      <c r="E54" s="35"/>
+      <c r="D54" s="41"/>
+      <c r="E54" s="41"/>
       <c r="F54" s="32"/>
       <c r="G54" s="32"/>
       <c r="H54" s="32"/>
@@ -6122,8 +5021,8 @@
       <c r="A55" s="32"/>
       <c r="B55" s="32"/>
       <c r="C55" s="32"/>
-      <c r="D55" s="35"/>
-      <c r="E55" s="35"/>
+      <c r="D55" s="41"/>
+      <c r="E55" s="41"/>
       <c r="F55" s="32"/>
       <c r="G55" s="32"/>
       <c r="H55" s="32"/>
@@ -6137,8 +5036,8 @@
       <c r="A56" s="32"/>
       <c r="B56" s="32"/>
       <c r="C56" s="32"/>
-      <c r="D56" s="35"/>
-      <c r="E56" s="35"/>
+      <c r="D56" s="41"/>
+      <c r="E56" s="41"/>
       <c r="F56" s="32"/>
       <c r="G56" s="32"/>
       <c r="H56" s="32"/>
@@ -6152,8 +5051,8 @@
       <c r="A57" s="32"/>
       <c r="B57" s="32"/>
       <c r="C57" s="32"/>
-      <c r="D57" s="35"/>
-      <c r="E57" s="35"/>
+      <c r="D57" s="41"/>
+      <c r="E57" s="41"/>
       <c r="F57" s="32"/>
       <c r="G57" s="32"/>
       <c r="H57" s="32"/>
@@ -6167,8 +5066,8 @@
       <c r="A58" s="32"/>
       <c r="B58" s="32"/>
       <c r="C58" s="32"/>
-      <c r="D58" s="35"/>
-      <c r="E58" s="35"/>
+      <c r="D58" s="41"/>
+      <c r="E58" s="41"/>
       <c r="F58" s="32"/>
       <c r="G58" s="32"/>
       <c r="H58" s="32"/>
@@ -6182,8 +5081,8 @@
       <c r="A59" s="32"/>
       <c r="B59" s="32"/>
       <c r="C59" s="32"/>
-      <c r="D59" s="35"/>
-      <c r="E59" s="35"/>
+      <c r="D59" s="41"/>
+      <c r="E59" s="41"/>
       <c r="F59" s="32"/>
       <c r="G59" s="32"/>
       <c r="H59" s="32"/>
@@ -6197,8 +5096,8 @@
       <c r="A60" s="32"/>
       <c r="B60" s="32"/>
       <c r="C60" s="32"/>
-      <c r="D60" s="35"/>
-      <c r="E60" s="35"/>
+      <c r="D60" s="41"/>
+      <c r="E60" s="41"/>
       <c r="F60" s="32"/>
       <c r="G60" s="32"/>
       <c r="H60" s="32"/>
@@ -6212,8 +5111,8 @@
       <c r="A61" s="32"/>
       <c r="B61" s="32"/>
       <c r="C61" s="32"/>
-      <c r="D61" s="35"/>
-      <c r="E61" s="35"/>
+      <c r="D61" s="41"/>
+      <c r="E61" s="41"/>
       <c r="F61" s="32"/>
       <c r="G61" s="32"/>
       <c r="H61" s="32"/>
@@ -6227,8 +5126,8 @@
       <c r="A62" s="32"/>
       <c r="B62" s="32"/>
       <c r="C62" s="32"/>
-      <c r="D62" s="35"/>
-      <c r="E62" s="35"/>
+      <c r="D62" s="41"/>
+      <c r="E62" s="41"/>
       <c r="F62" s="32"/>
       <c r="G62" s="32"/>
       <c r="H62" s="32"/>
@@ -6242,8 +5141,8 @@
       <c r="A63" s="32"/>
       <c r="B63" s="32"/>
       <c r="C63" s="32"/>
-      <c r="D63" s="35"/>
-      <c r="E63" s="35"/>
+      <c r="D63" s="41"/>
+      <c r="E63" s="41"/>
       <c r="F63" s="32"/>
       <c r="G63" s="32"/>
       <c r="H63" s="32"/>
@@ -6257,8 +5156,8 @@
       <c r="A64" s="32"/>
       <c r="B64" s="32"/>
       <c r="C64" s="32"/>
-      <c r="D64" s="35"/>
-      <c r="E64" s="35"/>
+      <c r="D64" s="41"/>
+      <c r="E64" s="41"/>
       <c r="F64" s="32"/>
       <c r="G64" s="32"/>
       <c r="H64" s="32"/>
@@ -6272,8 +5171,8 @@
       <c r="A65" s="32"/>
       <c r="B65" s="32"/>
       <c r="C65" s="32"/>
-      <c r="D65" s="35"/>
-      <c r="E65" s="35"/>
+      <c r="D65" s="41"/>
+      <c r="E65" s="41"/>
       <c r="F65" s="32"/>
       <c r="G65" s="32"/>
       <c r="H65" s="32"/>
@@ -6287,8 +5186,8 @@
       <c r="A66" s="32"/>
       <c r="B66" s="32"/>
       <c r="C66" s="32"/>
-      <c r="D66" s="35"/>
-      <c r="E66" s="35"/>
+      <c r="D66" s="41"/>
+      <c r="E66" s="41"/>
       <c r="F66" s="32"/>
       <c r="G66" s="32"/>
       <c r="H66" s="32"/>
@@ -6302,8 +5201,8 @@
       <c r="A67" s="32"/>
       <c r="B67" s="32"/>
       <c r="C67" s="32"/>
-      <c r="D67" s="35"/>
-      <c r="E67" s="35"/>
+      <c r="D67" s="41"/>
+      <c r="E67" s="41"/>
       <c r="F67" s="32"/>
       <c r="G67" s="32"/>
       <c r="H67" s="32"/>
@@ -6317,8 +5216,8 @@
       <c r="A68" s="32"/>
       <c r="B68" s="32"/>
       <c r="C68" s="32"/>
-      <c r="D68" s="35"/>
-      <c r="E68" s="35"/>
+      <c r="D68" s="41"/>
+      <c r="E68" s="41"/>
       <c r="F68" s="32"/>
       <c r="G68" s="32"/>
       <c r="H68" s="32"/>
@@ -6332,8 +5231,8 @@
       <c r="A69" s="32"/>
       <c r="B69" s="32"/>
       <c r="C69" s="32"/>
-      <c r="D69" s="35"/>
-      <c r="E69" s="35"/>
+      <c r="D69" s="41"/>
+      <c r="E69" s="41"/>
       <c r="F69" s="32"/>
       <c r="G69" s="32"/>
       <c r="H69" s="32"/>
@@ -6347,8 +5246,8 @@
       <c r="A70" s="32"/>
       <c r="B70" s="32"/>
       <c r="C70" s="32"/>
-      <c r="D70" s="35"/>
-      <c r="E70" s="35"/>
+      <c r="D70" s="41"/>
+      <c r="E70" s="41"/>
       <c r="F70" s="32"/>
       <c r="G70" s="32"/>
       <c r="H70" s="32"/>
@@ -6362,8 +5261,8 @@
       <c r="A71" s="32"/>
       <c r="B71" s="32"/>
       <c r="C71" s="32"/>
-      <c r="D71" s="35"/>
-      <c r="E71" s="35"/>
+      <c r="D71" s="41"/>
+      <c r="E71" s="41"/>
       <c r="F71" s="32"/>
       <c r="G71" s="32"/>
       <c r="H71" s="32"/>
@@ -6377,8 +5276,8 @@
       <c r="A72" s="32"/>
       <c r="B72" s="32"/>
       <c r="C72" s="32"/>
-      <c r="D72" s="35"/>
-      <c r="E72" s="35"/>
+      <c r="D72" s="41"/>
+      <c r="E72" s="41"/>
       <c r="F72" s="32"/>
       <c r="G72" s="32"/>
       <c r="H72" s="32"/>
@@ -6392,8 +5291,8 @@
       <c r="A73" s="32"/>
       <c r="B73" s="32"/>
       <c r="C73" s="32"/>
-      <c r="D73" s="35"/>
-      <c r="E73" s="35"/>
+      <c r="D73" s="41"/>
+      <c r="E73" s="41"/>
       <c r="F73" s="32"/>
       <c r="G73" s="32"/>
       <c r="H73" s="32"/>
@@ -6407,8 +5306,8 @@
       <c r="A74" s="32"/>
       <c r="B74" s="32"/>
       <c r="C74" s="32"/>
-      <c r="D74" s="35"/>
-      <c r="E74" s="35"/>
+      <c r="D74" s="41"/>
+      <c r="E74" s="41"/>
       <c r="F74" s="32"/>
       <c r="G74" s="32"/>
       <c r="H74" s="32"/>
@@ -6422,8 +5321,8 @@
       <c r="A75" s="32"/>
       <c r="B75" s="32"/>
       <c r="C75" s="32"/>
-      <c r="D75" s="35"/>
-      <c r="E75" s="35"/>
+      <c r="D75" s="41"/>
+      <c r="E75" s="41"/>
       <c r="F75" s="32"/>
       <c r="G75" s="32"/>
       <c r="H75" s="32"/>
@@ -6437,8 +5336,8 @@
       <c r="A76" s="32"/>
       <c r="B76" s="32"/>
       <c r="C76" s="32"/>
-      <c r="D76" s="35"/>
-      <c r="E76" s="35"/>
+      <c r="D76" s="41"/>
+      <c r="E76" s="41"/>
       <c r="F76" s="32"/>
       <c r="G76" s="32"/>
       <c r="H76" s="32"/>
@@ -6452,8 +5351,8 @@
       <c r="A77" s="32"/>
       <c r="B77" s="32"/>
       <c r="C77" s="32"/>
-      <c r="D77" s="35"/>
-      <c r="E77" s="35"/>
+      <c r="D77" s="41"/>
+      <c r="E77" s="41"/>
       <c r="F77" s="32"/>
       <c r="G77" s="32"/>
       <c r="H77" s="32"/>
@@ -6467,8 +5366,8 @@
       <c r="A78" s="32"/>
       <c r="B78" s="32"/>
       <c r="C78" s="32"/>
-      <c r="D78" s="35"/>
-      <c r="E78" s="35"/>
+      <c r="D78" s="41"/>
+      <c r="E78" s="41"/>
       <c r="F78" s="32"/>
       <c r="G78" s="32"/>
       <c r="H78" s="32"/>
@@ -6482,8 +5381,8 @@
       <c r="A79" s="32"/>
       <c r="B79" s="32"/>
       <c r="C79" s="32"/>
-      <c r="D79" s="35"/>
-      <c r="E79" s="35"/>
+      <c r="D79" s="41"/>
+      <c r="E79" s="41"/>
       <c r="F79" s="32"/>
       <c r="G79" s="32"/>
       <c r="H79" s="32"/>
@@ -6497,8 +5396,8 @@
       <c r="A80" s="32"/>
       <c r="B80" s="32"/>
       <c r="C80" s="32"/>
-      <c r="D80" s="35"/>
-      <c r="E80" s="35"/>
+      <c r="D80" s="41"/>
+      <c r="E80" s="41"/>
       <c r="F80" s="32"/>
       <c r="G80" s="32"/>
       <c r="H80" s="32"/>
@@ -6512,8 +5411,8 @@
       <c r="A81" s="25"/>
       <c r="B81" s="25"/>
       <c r="C81" s="33"/>
-      <c r="D81" s="36"/>
-      <c r="E81" s="36"/>
+      <c r="D81" s="42"/>
+      <c r="E81" s="42"/>
       <c r="F81" s="33"/>
       <c r="G81" s="33"/>
       <c r="H81" s="25"/>
@@ -6527,8 +5426,8 @@
       <c r="A82" s="25"/>
       <c r="B82" s="25"/>
       <c r="C82" s="33"/>
-      <c r="D82" s="36"/>
-      <c r="E82" s="36"/>
+      <c r="D82" s="42"/>
+      <c r="E82" s="42"/>
       <c r="F82" s="33"/>
       <c r="G82" s="33"/>
       <c r="H82" s="25"/>
@@ -6542,8 +5441,8 @@
       <c r="A83" s="25"/>
       <c r="B83" s="25"/>
       <c r="C83" s="33"/>
-      <c r="D83" s="36"/>
-      <c r="E83" s="36"/>
+      <c r="D83" s="42"/>
+      <c r="E83" s="42"/>
       <c r="F83" s="33"/>
       <c r="G83" s="33"/>
       <c r="H83" s="25"/>
@@ -6557,8 +5456,8 @@
       <c r="A84" s="25"/>
       <c r="B84" s="25"/>
       <c r="C84" s="33"/>
-      <c r="D84" s="36"/>
-      <c r="E84" s="36"/>
+      <c r="D84" s="42"/>
+      <c r="E84" s="42"/>
       <c r="F84" s="33"/>
       <c r="G84" s="33"/>
       <c r="H84" s="25"/>
@@ -6572,8 +5471,8 @@
       <c r="A85" s="25"/>
       <c r="B85" s="25"/>
       <c r="C85" s="33"/>
-      <c r="D85" s="36"/>
-      <c r="E85" s="36"/>
+      <c r="D85" s="42"/>
+      <c r="E85" s="42"/>
       <c r="F85" s="33"/>
       <c r="G85" s="33"/>
       <c r="H85" s="25"/>
@@ -6587,8 +5486,8 @@
       <c r="A86" s="25"/>
       <c r="B86" s="25"/>
       <c r="C86" s="33"/>
-      <c r="D86" s="36"/>
-      <c r="E86" s="36"/>
+      <c r="D86" s="42"/>
+      <c r="E86" s="42"/>
       <c r="F86" s="33"/>
       <c r="G86" s="33"/>
       <c r="H86" s="25"/>
@@ -6602,8 +5501,8 @@
       <c r="A87" s="25"/>
       <c r="B87" s="25"/>
       <c r="C87" s="33"/>
-      <c r="D87" s="36"/>
-      <c r="E87" s="36"/>
+      <c r="D87" s="42"/>
+      <c r="E87" s="42"/>
       <c r="F87" s="33"/>
       <c r="G87" s="33"/>
       <c r="H87" s="25"/>
@@ -6617,8 +5516,8 @@
       <c r="A88" s="25"/>
       <c r="B88" s="25"/>
       <c r="C88" s="33"/>
-      <c r="D88" s="36"/>
-      <c r="E88" s="36"/>
+      <c r="D88" s="42"/>
+      <c r="E88" s="42"/>
       <c r="F88" s="33"/>
       <c r="G88" s="33"/>
       <c r="H88" s="25"/>
@@ -6632,8 +5531,8 @@
       <c r="A89" s="25"/>
       <c r="B89" s="25"/>
       <c r="C89" s="33"/>
-      <c r="D89" s="36"/>
-      <c r="E89" s="36"/>
+      <c r="D89" s="42"/>
+      <c r="E89" s="42"/>
       <c r="F89" s="33"/>
       <c r="G89" s="33"/>
       <c r="H89" s="25"/>
@@ -6647,8 +5546,8 @@
       <c r="A90" s="25"/>
       <c r="B90" s="25"/>
       <c r="C90" s="33"/>
-      <c r="D90" s="36"/>
-      <c r="E90" s="36"/>
+      <c r="D90" s="42"/>
+      <c r="E90" s="42"/>
       <c r="F90" s="33"/>
       <c r="G90" s="33"/>
       <c r="H90" s="25"/>
@@ -6662,8 +5561,8 @@
       <c r="A91" s="25"/>
       <c r="B91" s="25"/>
       <c r="C91" s="33"/>
-      <c r="D91" s="36"/>
-      <c r="E91" s="36"/>
+      <c r="D91" s="42"/>
+      <c r="E91" s="42"/>
       <c r="F91" s="33"/>
       <c r="G91" s="33"/>
       <c r="H91" s="25"/>
@@ -6677,8 +5576,8 @@
       <c r="A92" s="25"/>
       <c r="B92" s="25"/>
       <c r="C92" s="33"/>
-      <c r="D92" s="36"/>
-      <c r="E92" s="36"/>
+      <c r="D92" s="42"/>
+      <c r="E92" s="42"/>
       <c r="F92" s="33"/>
       <c r="G92" s="33"/>
       <c r="H92" s="25"/>
@@ -6692,8 +5591,8 @@
       <c r="A93" s="25"/>
       <c r="B93" s="25"/>
       <c r="C93" s="33"/>
-      <c r="D93" s="36"/>
-      <c r="E93" s="36"/>
+      <c r="D93" s="42"/>
+      <c r="E93" s="42"/>
       <c r="F93" s="33"/>
       <c r="G93" s="33"/>
       <c r="H93" s="25"/>
@@ -6707,8 +5606,8 @@
       <c r="A94" s="25"/>
       <c r="B94" s="25"/>
       <c r="C94" s="33"/>
-      <c r="D94" s="36"/>
-      <c r="E94" s="36"/>
+      <c r="D94" s="42"/>
+      <c r="E94" s="42"/>
       <c r="F94" s="33"/>
       <c r="G94" s="33"/>
       <c r="H94" s="25"/>
@@ -6722,8 +5621,8 @@
       <c r="A95" s="25"/>
       <c r="B95" s="25"/>
       <c r="C95" s="33"/>
-      <c r="D95" s="36"/>
-      <c r="E95" s="36"/>
+      <c r="D95" s="42"/>
+      <c r="E95" s="42"/>
       <c r="F95" s="33"/>
       <c r="G95" s="33"/>
       <c r="H95" s="25"/>
@@ -6737,8 +5636,8 @@
       <c r="A96" s="25"/>
       <c r="B96" s="25"/>
       <c r="C96" s="33"/>
-      <c r="D96" s="36"/>
-      <c r="E96" s="36"/>
+      <c r="D96" s="42"/>
+      <c r="E96" s="42"/>
       <c r="F96" s="33"/>
       <c r="G96" s="33"/>
       <c r="H96" s="25"/>
@@ -6752,8 +5651,8 @@
       <c r="A97" s="25"/>
       <c r="B97" s="25"/>
       <c r="C97" s="33"/>
-      <c r="D97" s="36"/>
-      <c r="E97" s="36"/>
+      <c r="D97" s="42"/>
+      <c r="E97" s="42"/>
       <c r="F97" s="33"/>
       <c r="G97" s="33"/>
       <c r="H97" s="25"/>
@@ -6767,8 +5666,8 @@
       <c r="A98" s="25"/>
       <c r="B98" s="25"/>
       <c r="C98" s="33"/>
-      <c r="D98" s="36"/>
-      <c r="E98" s="36"/>
+      <c r="D98" s="42"/>
+      <c r="E98" s="42"/>
       <c r="F98" s="33"/>
       <c r="G98" s="33"/>
       <c r="H98" s="25"/>
@@ -6782,8 +5681,8 @@
       <c r="A99" s="25"/>
       <c r="B99" s="25"/>
       <c r="C99" s="33"/>
-      <c r="D99" s="36"/>
-      <c r="E99" s="36"/>
+      <c r="D99" s="42"/>
+      <c r="E99" s="42"/>
       <c r="F99" s="33"/>
       <c r="G99" s="33"/>
       <c r="H99" s="25"/>
@@ -6797,8 +5696,8 @@
       <c r="A100" s="25"/>
       <c r="B100" s="25"/>
       <c r="C100" s="33"/>
-      <c r="D100" s="36"/>
-      <c r="E100" s="36"/>
+      <c r="D100" s="42"/>
+      <c r="E100" s="42"/>
       <c r="F100" s="33"/>
       <c r="G100" s="33"/>
       <c r="H100" s="25"/>
@@ -6812,8 +5711,8 @@
       <c r="A101" s="25"/>
       <c r="B101" s="25"/>
       <c r="C101" s="33"/>
-      <c r="D101" s="36"/>
-      <c r="E101" s="36"/>
+      <c r="D101" s="42"/>
+      <c r="E101" s="42"/>
       <c r="F101" s="33"/>
       <c r="G101" s="33"/>
       <c r="H101" s="25"/>
@@ -6827,8 +5726,8 @@
       <c r="A102" s="25"/>
       <c r="B102" s="25"/>
       <c r="C102" s="33"/>
-      <c r="D102" s="36"/>
-      <c r="E102" s="36"/>
+      <c r="D102" s="42"/>
+      <c r="E102" s="42"/>
       <c r="F102" s="33"/>
       <c r="G102" s="33"/>
       <c r="H102" s="25"/>
@@ -6842,8 +5741,8 @@
       <c r="A103" s="25"/>
       <c r="B103" s="25"/>
       <c r="C103" s="33"/>
-      <c r="D103" s="36"/>
-      <c r="E103" s="36"/>
+      <c r="D103" s="42"/>
+      <c r="E103" s="42"/>
       <c r="F103" s="33"/>
       <c r="G103" s="33"/>
       <c r="H103" s="25"/>
@@ -6857,8 +5756,8 @@
       <c r="A104" s="25"/>
       <c r="B104" s="25"/>
       <c r="C104" s="33"/>
-      <c r="D104" s="36"/>
-      <c r="E104" s="36"/>
+      <c r="D104" s="42"/>
+      <c r="E104" s="42"/>
       <c r="F104" s="33"/>
       <c r="G104" s="33"/>
       <c r="H104" s="25"/>
@@ -6872,8 +5771,8 @@
       <c r="A105" s="25"/>
       <c r="B105" s="25"/>
       <c r="C105" s="33"/>
-      <c r="D105" s="36"/>
-      <c r="E105" s="36"/>
+      <c r="D105" s="42"/>
+      <c r="E105" s="42"/>
       <c r="F105" s="33"/>
       <c r="G105" s="33"/>
       <c r="H105" s="25"/>
@@ -6887,8 +5786,8 @@
       <c r="A106" s="25"/>
       <c r="B106" s="25"/>
       <c r="C106" s="33"/>
-      <c r="D106" s="36"/>
-      <c r="E106" s="36"/>
+      <c r="D106" s="42"/>
+      <c r="E106" s="42"/>
       <c r="F106" s="33"/>
       <c r="G106" s="33"/>
       <c r="H106" s="25"/>
@@ -6902,8 +5801,8 @@
       <c r="A107" s="25"/>
       <c r="B107" s="25"/>
       <c r="C107" s="33"/>
-      <c r="D107" s="36"/>
-      <c r="E107" s="36"/>
+      <c r="D107" s="42"/>
+      <c r="E107" s="42"/>
       <c r="F107" s="33"/>
       <c r="G107" s="33"/>
       <c r="H107" s="25"/>
@@ -6917,8 +5816,8 @@
       <c r="A108" s="25"/>
       <c r="B108" s="25"/>
       <c r="C108" s="33"/>
-      <c r="D108" s="36"/>
-      <c r="E108" s="36"/>
+      <c r="D108" s="42"/>
+      <c r="E108" s="42"/>
       <c r="F108" s="33"/>
       <c r="G108" s="33"/>
       <c r="H108" s="25"/>
@@ -6932,8 +5831,8 @@
       <c r="A109" s="25"/>
       <c r="B109" s="25"/>
       <c r="C109" s="33"/>
-      <c r="D109" s="36"/>
-      <c r="E109" s="36"/>
+      <c r="D109" s="42"/>
+      <c r="E109" s="42"/>
       <c r="F109" s="33"/>
       <c r="G109" s="33"/>
       <c r="H109" s="25"/>
@@ -6947,8 +5846,8 @@
       <c r="A110" s="25"/>
       <c r="B110" s="25"/>
       <c r="C110" s="33"/>
-      <c r="D110" s="36"/>
-      <c r="E110" s="36"/>
+      <c r="D110" s="42"/>
+      <c r="E110" s="42"/>
       <c r="F110" s="33"/>
       <c r="G110" s="33"/>
       <c r="H110" s="25"/>
@@ -6962,8 +5861,8 @@
       <c r="A111" s="27"/>
       <c r="B111" s="27"/>
       <c r="C111" s="34"/>
-      <c r="D111" s="37"/>
-      <c r="E111" s="37"/>
+      <c r="D111" s="43"/>
+      <c r="E111" s="43"/>
       <c r="F111" s="34"/>
       <c r="G111" s="34"/>
       <c r="H111" s="27"/>
@@ -7720,10 +6619,10 @@
         <v>233</v>
       </c>
       <c r="P12" s="2" t="s">
+        <v>825</v>
+      </c>
+      <c r="Q12" s="2" t="s">
         <v>826</v>
-      </c>
-      <c r="Q12" s="2" t="s">
-        <v>827</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Now handles replicates indicated in depth by /
</commit_message>
<xml_diff>
--- a/hydrofia/hydrofia_ph_template.xlsx
+++ b/hydrofia/hydrofia_ph_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\mw\git\hydrofia\hydrofia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E89A0025-D37E-4ACB-A73C-E48C200C9CA4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22AFFFE7-6472-45BB-9DC1-95DF68E2B603}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-15" yWindow="165" windowWidth="15600" windowHeight="11610" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55,7 +55,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Nilsson Madeleine:</t>
         </r>
@@ -64,7 +64,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 plats för kommentar</t>
@@ -2732,14 +2732,14 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -2956,15 +2956,6 @@
     <xf numFmtId="49" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2985,6 +2976,15 @@
     </xf>
     <xf numFmtId="49" fontId="19" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3420,14 +3420,14 @@
   <dimension ref="A1:EK112"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+      <selection activeCell="D14" sqref="D14:E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.7109375" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.85546875" style="11" customWidth="1"/>
     <col min="2" max="2" width="4.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.7109375" style="11" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" style="11" customWidth="1"/>
     <col min="4" max="4" width="6.5703125" style="11" customWidth="1"/>
     <col min="5" max="5" width="14.7109375" style="11" customWidth="1"/>
     <col min="6" max="6" width="5.7109375" style="11" customWidth="1"/>
@@ -3443,12 +3443,12 @@
       <c r="A1" s="10"/>
       <c r="B1" s="10"/>
       <c r="D1" s="35"/>
-      <c r="E1" s="44" t="s">
+      <c r="E1" s="41" t="s">
         <v>827</v>
       </c>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
+      <c r="F1" s="41"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="41"/>
       <c r="K1" s="36" t="s">
         <v>833</v>
       </c>
@@ -3579,10 +3579,10 @@
     </row>
     <row r="2" spans="1:141" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D2" s="35"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
       <c r="K2" s="36" t="s">
         <v>2</v>
       </c>
@@ -3717,10 +3717,10 @@
       </c>
       <c r="B3" s="14"/>
       <c r="D3" s="35"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
       <c r="J3" s="37"/>
       <c r="K3" s="37"/>
       <c r="L3" s="37"/>
@@ -3982,27 +3982,27 @@
       <c r="EK4" s="13"/>
     </row>
     <row r="5" spans="1:141" s="4" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="48"/>
-      <c r="C5" s="48"/>
-      <c r="D5" s="48"/>
+      <c r="B5" s="45"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45"/>
       <c r="E5" s="39"/>
-      <c r="F5" s="48" t="s">
+      <c r="F5" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="48"/>
-      <c r="H5" s="48" t="s">
+      <c r="G5" s="45"/>
+      <c r="H5" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="48"/>
-      <c r="J5" s="48" t="s">
+      <c r="I5" s="45"/>
+      <c r="J5" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="48"/>
-      <c r="L5" s="48"/>
-      <c r="M5" s="48"/>
+      <c r="K5" s="45"/>
+      <c r="L5" s="45"/>
+      <c r="M5" s="45"/>
       <c r="N5" s="15"/>
       <c r="S5" s="16"/>
       <c r="T5" s="16"/>
@@ -4129,19 +4129,19 @@
       <c r="EK5" s="16"/>
     </row>
     <row r="6" spans="1:141" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="47"/>
-      <c r="B6" s="47"/>
-      <c r="C6" s="47"/>
-      <c r="D6" s="47"/>
+      <c r="A6" s="44"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
       <c r="E6" s="31"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="47"/>
-      <c r="I6" s="47"/>
-      <c r="J6" s="47"/>
-      <c r="K6" s="47"/>
-      <c r="L6" s="47"/>
-      <c r="M6" s="47"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="44"/>
+      <c r="K6" s="44"/>
+      <c r="L6" s="44"/>
+      <c r="M6" s="44"/>
       <c r="N6" s="17"/>
       <c r="S6" s="13"/>
       <c r="T6" s="13"/>
@@ -4268,34 +4268,34 @@
       <c r="EK6" s="13"/>
     </row>
     <row r="7" spans="1:141" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="47"/>
-      <c r="B7" s="47"/>
-      <c r="C7" s="47"/>
-      <c r="D7" s="47"/>
+      <c r="A7" s="44"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
       <c r="E7" s="31"/>
-      <c r="F7" s="47"/>
-      <c r="G7" s="47"/>
-      <c r="H7" s="47"/>
-      <c r="I7" s="47"/>
-      <c r="J7" s="47"/>
-      <c r="K7" s="47"/>
-      <c r="L7" s="47"/>
-      <c r="M7" s="47"/>
+      <c r="F7" s="44"/>
+      <c r="G7" s="44"/>
+      <c r="H7" s="44"/>
+      <c r="I7" s="44"/>
+      <c r="J7" s="44"/>
+      <c r="K7" s="44"/>
+      <c r="L7" s="44"/>
+      <c r="M7" s="44"/>
     </row>
     <row r="8" spans="1:141" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="47"/>
-      <c r="B8" s="47"/>
-      <c r="C8" s="47"/>
-      <c r="D8" s="47"/>
+      <c r="A8" s="44"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
       <c r="E8" s="31"/>
-      <c r="F8" s="47"/>
-      <c r="G8" s="47"/>
-      <c r="H8" s="47"/>
-      <c r="I8" s="47"/>
-      <c r="J8" s="47"/>
-      <c r="K8" s="47"/>
-      <c r="L8" s="47"/>
-      <c r="M8" s="47"/>
+      <c r="F8" s="44"/>
+      <c r="G8" s="44"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="44"/>
+      <c r="J8" s="44"/>
+      <c r="K8" s="44"/>
+      <c r="L8" s="44"/>
+      <c r="M8" s="44"/>
     </row>
     <row r="9" spans="1:141" s="13" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="18"/>
@@ -4313,17 +4313,17 @@
       <c r="M9" s="19"/>
     </row>
     <row r="10" spans="1:141" s="13" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="45" t="s">
+      <c r="A10" s="42" t="s">
         <v>416</v>
       </c>
-      <c r="B10" s="49"/>
-      <c r="C10" s="45" t="s">
+      <c r="B10" s="46"/>
+      <c r="C10" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="45" t="s">
+      <c r="D10" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="45"/>
+      <c r="E10" s="42"/>
       <c r="F10" s="30" t="s">
         <v>0</v>
       </c>
@@ -4343,16 +4343,16 @@
         <v>830</v>
       </c>
       <c r="L10" s="22"/>
-      <c r="M10" s="45" t="s">
+      <c r="M10" s="42" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:141" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="46"/>
-      <c r="B11" s="50"/>
-      <c r="C11" s="46"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="46"/>
+      <c r="A11" s="43"/>
+      <c r="B11" s="47"/>
+      <c r="C11" s="43"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
       <c r="F11" s="23" t="s">
         <v>5</v>
       </c>
@@ -4370,14 +4370,14 @@
       </c>
       <c r="K11" s="24"/>
       <c r="L11" s="24"/>
-      <c r="M11" s="46"/>
+      <c r="M11" s="43"/>
     </row>
     <row r="12" spans="1:141" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="32"/>
       <c r="B12" s="32"/>
       <c r="C12" s="32"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
+      <c r="D12" s="48"/>
+      <c r="E12" s="48"/>
       <c r="F12" s="32"/>
       <c r="G12" s="32"/>
       <c r="H12" s="32"/>
@@ -4391,8 +4391,8 @@
       <c r="A13" s="32"/>
       <c r="B13" s="32"/>
       <c r="C13" s="32"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
+      <c r="D13" s="48"/>
+      <c r="E13" s="48"/>
       <c r="F13" s="32"/>
       <c r="G13" s="32"/>
       <c r="H13" s="32"/>
@@ -4406,8 +4406,8 @@
       <c r="A14" s="32"/>
       <c r="B14" s="32"/>
       <c r="C14" s="32"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41"/>
+      <c r="D14" s="48"/>
+      <c r="E14" s="48"/>
       <c r="F14" s="32"/>
       <c r="G14" s="32"/>
       <c r="H14" s="32"/>
@@ -4421,8 +4421,8 @@
       <c r="A15" s="32"/>
       <c r="B15" s="32"/>
       <c r="C15" s="32"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
+      <c r="D15" s="48"/>
+      <c r="E15" s="48"/>
       <c r="F15" s="32"/>
       <c r="G15" s="32"/>
       <c r="H15" s="32"/>
@@ -4436,8 +4436,8 @@
       <c r="A16" s="32"/>
       <c r="B16" s="32"/>
       <c r="C16" s="32"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="41"/>
+      <c r="D16" s="48"/>
+      <c r="E16" s="48"/>
       <c r="F16" s="32"/>
       <c r="G16" s="32"/>
       <c r="H16" s="32"/>
@@ -4451,8 +4451,8 @@
       <c r="A17" s="32"/>
       <c r="B17" s="32"/>
       <c r="C17" s="32"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="48"/>
       <c r="F17" s="32"/>
       <c r="G17" s="32"/>
       <c r="H17" s="32"/>
@@ -4466,8 +4466,8 @@
       <c r="A18" s="32"/>
       <c r="B18" s="32"/>
       <c r="C18" s="32"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="48"/>
       <c r="F18" s="32"/>
       <c r="G18" s="32"/>
       <c r="H18" s="32"/>
@@ -4481,8 +4481,8 @@
       <c r="A19" s="32"/>
       <c r="B19" s="32"/>
       <c r="C19" s="32"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="41"/>
+      <c r="D19" s="48"/>
+      <c r="E19" s="48"/>
       <c r="F19" s="32"/>
       <c r="G19" s="32"/>
       <c r="H19" s="32"/>
@@ -4496,8 +4496,8 @@
       <c r="A20" s="32"/>
       <c r="B20" s="32"/>
       <c r="C20" s="32"/>
-      <c r="D20" s="41"/>
-      <c r="E20" s="41"/>
+      <c r="D20" s="48"/>
+      <c r="E20" s="48"/>
       <c r="F20" s="32"/>
       <c r="G20" s="32"/>
       <c r="H20" s="32"/>
@@ -4511,8 +4511,8 @@
       <c r="A21" s="32"/>
       <c r="B21" s="32"/>
       <c r="C21" s="32"/>
-      <c r="D21" s="41"/>
-      <c r="E21" s="41"/>
+      <c r="D21" s="48"/>
+      <c r="E21" s="48"/>
       <c r="F21" s="32"/>
       <c r="G21" s="32"/>
       <c r="H21" s="32"/>
@@ -4526,8 +4526,8 @@
       <c r="A22" s="32"/>
       <c r="B22" s="32"/>
       <c r="C22" s="32"/>
-      <c r="D22" s="41"/>
-      <c r="E22" s="41"/>
+      <c r="D22" s="48"/>
+      <c r="E22" s="48"/>
       <c r="F22" s="32"/>
       <c r="G22" s="32"/>
       <c r="H22" s="32"/>
@@ -4541,8 +4541,8 @@
       <c r="A23" s="32"/>
       <c r="B23" s="32"/>
       <c r="C23" s="32"/>
-      <c r="D23" s="41"/>
-      <c r="E23" s="41"/>
+      <c r="D23" s="48"/>
+      <c r="E23" s="48"/>
       <c r="F23" s="32"/>
       <c r="G23" s="32"/>
       <c r="H23" s="32"/>
@@ -4556,8 +4556,8 @@
       <c r="A24" s="32"/>
       <c r="B24" s="32"/>
       <c r="C24" s="32"/>
-      <c r="D24" s="41"/>
-      <c r="E24" s="41"/>
+      <c r="D24" s="48"/>
+      <c r="E24" s="48"/>
       <c r="F24" s="32"/>
       <c r="G24" s="32"/>
       <c r="H24" s="32"/>
@@ -4571,8 +4571,8 @@
       <c r="A25" s="32"/>
       <c r="B25" s="32"/>
       <c r="C25" s="32"/>
-      <c r="D25" s="41"/>
-      <c r="E25" s="41"/>
+      <c r="D25" s="48"/>
+      <c r="E25" s="48"/>
       <c r="F25" s="32"/>
       <c r="G25" s="32"/>
       <c r="H25" s="32"/>
@@ -4586,8 +4586,8 @@
       <c r="A26" s="32"/>
       <c r="B26" s="32"/>
       <c r="C26" s="32"/>
-      <c r="D26" s="41"/>
-      <c r="E26" s="41"/>
+      <c r="D26" s="48"/>
+      <c r="E26" s="48"/>
       <c r="F26" s="32"/>
       <c r="G26" s="32"/>
       <c r="H26" s="32"/>
@@ -4601,8 +4601,8 @@
       <c r="A27" s="32"/>
       <c r="B27" s="32"/>
       <c r="C27" s="32"/>
-      <c r="D27" s="41"/>
-      <c r="E27" s="41"/>
+      <c r="D27" s="48"/>
+      <c r="E27" s="48"/>
       <c r="F27" s="32"/>
       <c r="G27" s="32"/>
       <c r="H27" s="32"/>
@@ -4616,8 +4616,8 @@
       <c r="A28" s="32"/>
       <c r="B28" s="32"/>
       <c r="C28" s="32"/>
-      <c r="D28" s="41"/>
-      <c r="E28" s="41"/>
+      <c r="D28" s="48"/>
+      <c r="E28" s="48"/>
       <c r="F28" s="32"/>
       <c r="G28" s="32"/>
       <c r="H28" s="32"/>
@@ -4631,8 +4631,8 @@
       <c r="A29" s="32"/>
       <c r="B29" s="32"/>
       <c r="C29" s="32"/>
-      <c r="D29" s="41"/>
-      <c r="E29" s="41"/>
+      <c r="D29" s="48"/>
+      <c r="E29" s="48"/>
       <c r="F29" s="32"/>
       <c r="G29" s="32"/>
       <c r="H29" s="32"/>
@@ -4646,8 +4646,8 @@
       <c r="A30" s="32"/>
       <c r="B30" s="32"/>
       <c r="C30" s="32"/>
-      <c r="D30" s="41"/>
-      <c r="E30" s="41"/>
+      <c r="D30" s="48"/>
+      <c r="E30" s="48"/>
       <c r="F30" s="32"/>
       <c r="G30" s="32"/>
       <c r="H30" s="32"/>
@@ -4661,8 +4661,8 @@
       <c r="A31" s="32"/>
       <c r="B31" s="32"/>
       <c r="C31" s="32"/>
-      <c r="D31" s="41"/>
-      <c r="E31" s="41"/>
+      <c r="D31" s="48"/>
+      <c r="E31" s="48"/>
       <c r="F31" s="32"/>
       <c r="G31" s="32"/>
       <c r="H31" s="32"/>
@@ -4676,8 +4676,8 @@
       <c r="A32" s="32"/>
       <c r="B32" s="32"/>
       <c r="C32" s="32"/>
-      <c r="D32" s="41"/>
-      <c r="E32" s="41"/>
+      <c r="D32" s="48"/>
+      <c r="E32" s="48"/>
       <c r="F32" s="32"/>
       <c r="G32" s="32"/>
       <c r="H32" s="32"/>
@@ -4691,8 +4691,8 @@
       <c r="A33" s="32"/>
       <c r="B33" s="32"/>
       <c r="C33" s="32"/>
-      <c r="D33" s="41"/>
-      <c r="E33" s="41"/>
+      <c r="D33" s="48"/>
+      <c r="E33" s="48"/>
       <c r="F33" s="32"/>
       <c r="G33" s="32"/>
       <c r="H33" s="32"/>
@@ -4706,8 +4706,8 @@
       <c r="A34" s="32"/>
       <c r="B34" s="32"/>
       <c r="C34" s="32"/>
-      <c r="D34" s="41"/>
-      <c r="E34" s="41"/>
+      <c r="D34" s="48"/>
+      <c r="E34" s="48"/>
       <c r="F34" s="32"/>
       <c r="G34" s="32"/>
       <c r="H34" s="32"/>
@@ -4721,8 +4721,8 @@
       <c r="A35" s="32"/>
       <c r="B35" s="32"/>
       <c r="C35" s="32"/>
-      <c r="D35" s="41"/>
-      <c r="E35" s="41"/>
+      <c r="D35" s="48"/>
+      <c r="E35" s="48"/>
       <c r="F35" s="32"/>
       <c r="G35" s="32"/>
       <c r="H35" s="32"/>
@@ -4736,8 +4736,8 @@
       <c r="A36" s="32"/>
       <c r="B36" s="32"/>
       <c r="C36" s="32"/>
-      <c r="D36" s="41"/>
-      <c r="E36" s="41"/>
+      <c r="D36" s="48"/>
+      <c r="E36" s="48"/>
       <c r="F36" s="32"/>
       <c r="G36" s="32"/>
       <c r="H36" s="32"/>
@@ -4751,8 +4751,8 @@
       <c r="A37" s="32"/>
       <c r="B37" s="32"/>
       <c r="C37" s="32"/>
-      <c r="D37" s="41"/>
-      <c r="E37" s="41"/>
+      <c r="D37" s="48"/>
+      <c r="E37" s="48"/>
       <c r="F37" s="32"/>
       <c r="G37" s="32"/>
       <c r="H37" s="32"/>
@@ -4766,8 +4766,8 @@
       <c r="A38" s="32"/>
       <c r="B38" s="32"/>
       <c r="C38" s="32"/>
-      <c r="D38" s="41"/>
-      <c r="E38" s="41"/>
+      <c r="D38" s="48"/>
+      <c r="E38" s="48"/>
       <c r="F38" s="32"/>
       <c r="G38" s="32"/>
       <c r="H38" s="32"/>
@@ -4781,8 +4781,8 @@
       <c r="A39" s="32"/>
       <c r="B39" s="32"/>
       <c r="C39" s="32"/>
-      <c r="D39" s="41"/>
-      <c r="E39" s="41"/>
+      <c r="D39" s="48"/>
+      <c r="E39" s="48"/>
       <c r="F39" s="32"/>
       <c r="G39" s="32"/>
       <c r="H39" s="32"/>
@@ -4796,8 +4796,8 @@
       <c r="A40" s="32"/>
       <c r="B40" s="32"/>
       <c r="C40" s="32"/>
-      <c r="D40" s="41"/>
-      <c r="E40" s="41"/>
+      <c r="D40" s="48"/>
+      <c r="E40" s="48"/>
       <c r="F40" s="32"/>
       <c r="G40" s="32"/>
       <c r="H40" s="32"/>
@@ -4811,8 +4811,8 @@
       <c r="A41" s="32"/>
       <c r="B41" s="32"/>
       <c r="C41" s="32"/>
-      <c r="D41" s="41"/>
-      <c r="E41" s="41"/>
+      <c r="D41" s="48"/>
+      <c r="E41" s="48"/>
       <c r="F41" s="32"/>
       <c r="G41" s="32"/>
       <c r="H41" s="32"/>
@@ -4826,8 +4826,8 @@
       <c r="A42" s="32"/>
       <c r="B42" s="32"/>
       <c r="C42" s="32"/>
-      <c r="D42" s="41"/>
-      <c r="E42" s="41"/>
+      <c r="D42" s="48"/>
+      <c r="E42" s="48"/>
       <c r="F42" s="32"/>
       <c r="G42" s="32"/>
       <c r="H42" s="32"/>
@@ -4841,8 +4841,8 @@
       <c r="A43" s="32"/>
       <c r="B43" s="32"/>
       <c r="C43" s="32"/>
-      <c r="D43" s="41"/>
-      <c r="E43" s="41"/>
+      <c r="D43" s="48"/>
+      <c r="E43" s="48"/>
       <c r="F43" s="32"/>
       <c r="G43" s="32"/>
       <c r="H43" s="32"/>
@@ -4856,8 +4856,8 @@
       <c r="A44" s="32"/>
       <c r="B44" s="32"/>
       <c r="C44" s="32"/>
-      <c r="D44" s="41"/>
-      <c r="E44" s="41"/>
+      <c r="D44" s="48"/>
+      <c r="E44" s="48"/>
       <c r="F44" s="32"/>
       <c r="G44" s="32"/>
       <c r="H44" s="32"/>
@@ -4871,8 +4871,8 @@
       <c r="A45" s="32"/>
       <c r="B45" s="32"/>
       <c r="C45" s="32"/>
-      <c r="D45" s="41"/>
-      <c r="E45" s="41"/>
+      <c r="D45" s="48"/>
+      <c r="E45" s="48"/>
       <c r="F45" s="32"/>
       <c r="G45" s="32"/>
       <c r="H45" s="32"/>
@@ -4886,8 +4886,8 @@
       <c r="A46" s="32"/>
       <c r="B46" s="32"/>
       <c r="C46" s="32"/>
-      <c r="D46" s="41"/>
-      <c r="E46" s="41"/>
+      <c r="D46" s="48"/>
+      <c r="E46" s="48"/>
       <c r="F46" s="32"/>
       <c r="G46" s="32"/>
       <c r="H46" s="32"/>
@@ -4901,8 +4901,8 @@
       <c r="A47" s="32"/>
       <c r="B47" s="32"/>
       <c r="C47" s="32"/>
-      <c r="D47" s="41"/>
-      <c r="E47" s="41"/>
+      <c r="D47" s="48"/>
+      <c r="E47" s="48"/>
       <c r="F47" s="32"/>
       <c r="G47" s="32"/>
       <c r="H47" s="32"/>
@@ -4916,8 +4916,8 @@
       <c r="A48" s="32"/>
       <c r="B48" s="32"/>
       <c r="C48" s="32"/>
-      <c r="D48" s="41"/>
-      <c r="E48" s="41"/>
+      <c r="D48" s="48"/>
+      <c r="E48" s="48"/>
       <c r="F48" s="32"/>
       <c r="G48" s="32"/>
       <c r="H48" s="32"/>
@@ -4931,8 +4931,8 @@
       <c r="A49" s="32"/>
       <c r="B49" s="32"/>
       <c r="C49" s="32"/>
-      <c r="D49" s="41"/>
-      <c r="E49" s="41"/>
+      <c r="D49" s="48"/>
+      <c r="E49" s="48"/>
       <c r="F49" s="32"/>
       <c r="G49" s="32"/>
       <c r="H49" s="32"/>
@@ -4946,8 +4946,8 @@
       <c r="A50" s="32"/>
       <c r="B50" s="32"/>
       <c r="C50" s="32"/>
-      <c r="D50" s="41"/>
-      <c r="E50" s="41"/>
+      <c r="D50" s="48"/>
+      <c r="E50" s="48"/>
       <c r="F50" s="32"/>
       <c r="G50" s="32"/>
       <c r="H50" s="32"/>
@@ -4961,8 +4961,8 @@
       <c r="A51" s="32"/>
       <c r="B51" s="32"/>
       <c r="C51" s="32"/>
-      <c r="D51" s="41"/>
-      <c r="E51" s="41"/>
+      <c r="D51" s="48"/>
+      <c r="E51" s="48"/>
       <c r="F51" s="32"/>
       <c r="G51" s="32"/>
       <c r="H51" s="32"/>
@@ -4976,8 +4976,8 @@
       <c r="A52" s="32"/>
       <c r="B52" s="32"/>
       <c r="C52" s="32"/>
-      <c r="D52" s="41"/>
-      <c r="E52" s="41"/>
+      <c r="D52" s="48"/>
+      <c r="E52" s="48"/>
       <c r="F52" s="32"/>
       <c r="G52" s="32"/>
       <c r="H52" s="32"/>
@@ -4991,8 +4991,8 @@
       <c r="A53" s="32"/>
       <c r="B53" s="32"/>
       <c r="C53" s="32"/>
-      <c r="D53" s="41"/>
-      <c r="E53" s="41"/>
+      <c r="D53" s="48"/>
+      <c r="E53" s="48"/>
       <c r="F53" s="32"/>
       <c r="G53" s="32"/>
       <c r="H53" s="32"/>
@@ -5006,8 +5006,8 @@
       <c r="A54" s="32"/>
       <c r="B54" s="32"/>
       <c r="C54" s="32"/>
-      <c r="D54" s="41"/>
-      <c r="E54" s="41"/>
+      <c r="D54" s="48"/>
+      <c r="E54" s="48"/>
       <c r="F54" s="32"/>
       <c r="G54" s="32"/>
       <c r="H54" s="32"/>
@@ -5021,8 +5021,8 @@
       <c r="A55" s="32"/>
       <c r="B55" s="32"/>
       <c r="C55" s="32"/>
-      <c r="D55" s="41"/>
-      <c r="E55" s="41"/>
+      <c r="D55" s="48"/>
+      <c r="E55" s="48"/>
       <c r="F55" s="32"/>
       <c r="G55" s="32"/>
       <c r="H55" s="32"/>
@@ -5036,8 +5036,8 @@
       <c r="A56" s="32"/>
       <c r="B56" s="32"/>
       <c r="C56" s="32"/>
-      <c r="D56" s="41"/>
-      <c r="E56" s="41"/>
+      <c r="D56" s="48"/>
+      <c r="E56" s="48"/>
       <c r="F56" s="32"/>
       <c r="G56" s="32"/>
       <c r="H56" s="32"/>
@@ -5051,8 +5051,8 @@
       <c r="A57" s="32"/>
       <c r="B57" s="32"/>
       <c r="C57" s="32"/>
-      <c r="D57" s="41"/>
-      <c r="E57" s="41"/>
+      <c r="D57" s="48"/>
+      <c r="E57" s="48"/>
       <c r="F57" s="32"/>
       <c r="G57" s="32"/>
       <c r="H57" s="32"/>
@@ -5066,8 +5066,8 @@
       <c r="A58" s="32"/>
       <c r="B58" s="32"/>
       <c r="C58" s="32"/>
-      <c r="D58" s="41"/>
-      <c r="E58" s="41"/>
+      <c r="D58" s="48"/>
+      <c r="E58" s="48"/>
       <c r="F58" s="32"/>
       <c r="G58" s="32"/>
       <c r="H58" s="32"/>
@@ -5081,8 +5081,8 @@
       <c r="A59" s="32"/>
       <c r="B59" s="32"/>
       <c r="C59" s="32"/>
-      <c r="D59" s="41"/>
-      <c r="E59" s="41"/>
+      <c r="D59" s="48"/>
+      <c r="E59" s="48"/>
       <c r="F59" s="32"/>
       <c r="G59" s="32"/>
       <c r="H59" s="32"/>
@@ -5096,8 +5096,8 @@
       <c r="A60" s="32"/>
       <c r="B60" s="32"/>
       <c r="C60" s="32"/>
-      <c r="D60" s="41"/>
-      <c r="E60" s="41"/>
+      <c r="D60" s="48"/>
+      <c r="E60" s="48"/>
       <c r="F60" s="32"/>
       <c r="G60" s="32"/>
       <c r="H60" s="32"/>
@@ -5111,8 +5111,8 @@
       <c r="A61" s="32"/>
       <c r="B61" s="32"/>
       <c r="C61" s="32"/>
-      <c r="D61" s="41"/>
-      <c r="E61" s="41"/>
+      <c r="D61" s="48"/>
+      <c r="E61" s="48"/>
       <c r="F61" s="32"/>
       <c r="G61" s="32"/>
       <c r="H61" s="32"/>
@@ -5126,8 +5126,8 @@
       <c r="A62" s="32"/>
       <c r="B62" s="32"/>
       <c r="C62" s="32"/>
-      <c r="D62" s="41"/>
-      <c r="E62" s="41"/>
+      <c r="D62" s="48"/>
+      <c r="E62" s="48"/>
       <c r="F62" s="32"/>
       <c r="G62" s="32"/>
       <c r="H62" s="32"/>
@@ -5141,8 +5141,8 @@
       <c r="A63" s="32"/>
       <c r="B63" s="32"/>
       <c r="C63" s="32"/>
-      <c r="D63" s="41"/>
-      <c r="E63" s="41"/>
+      <c r="D63" s="48"/>
+      <c r="E63" s="48"/>
       <c r="F63" s="32"/>
       <c r="G63" s="32"/>
       <c r="H63" s="32"/>
@@ -5156,8 +5156,8 @@
       <c r="A64" s="32"/>
       <c r="B64" s="32"/>
       <c r="C64" s="32"/>
-      <c r="D64" s="41"/>
-      <c r="E64" s="41"/>
+      <c r="D64" s="48"/>
+      <c r="E64" s="48"/>
       <c r="F64" s="32"/>
       <c r="G64" s="32"/>
       <c r="H64" s="32"/>
@@ -5171,8 +5171,8 @@
       <c r="A65" s="32"/>
       <c r="B65" s="32"/>
       <c r="C65" s="32"/>
-      <c r="D65" s="41"/>
-      <c r="E65" s="41"/>
+      <c r="D65" s="48"/>
+      <c r="E65" s="48"/>
       <c r="F65" s="32"/>
       <c r="G65" s="32"/>
       <c r="H65" s="32"/>
@@ -5186,8 +5186,8 @@
       <c r="A66" s="32"/>
       <c r="B66" s="32"/>
       <c r="C66" s="32"/>
-      <c r="D66" s="41"/>
-      <c r="E66" s="41"/>
+      <c r="D66" s="48"/>
+      <c r="E66" s="48"/>
       <c r="F66" s="32"/>
       <c r="G66" s="32"/>
       <c r="H66" s="32"/>
@@ -5201,8 +5201,8 @@
       <c r="A67" s="32"/>
       <c r="B67" s="32"/>
       <c r="C67" s="32"/>
-      <c r="D67" s="41"/>
-      <c r="E67" s="41"/>
+      <c r="D67" s="48"/>
+      <c r="E67" s="48"/>
       <c r="F67" s="32"/>
       <c r="G67" s="32"/>
       <c r="H67" s="32"/>
@@ -5216,8 +5216,8 @@
       <c r="A68" s="32"/>
       <c r="B68" s="32"/>
       <c r="C68" s="32"/>
-      <c r="D68" s="41"/>
-      <c r="E68" s="41"/>
+      <c r="D68" s="48"/>
+      <c r="E68" s="48"/>
       <c r="F68" s="32"/>
       <c r="G68" s="32"/>
       <c r="H68" s="32"/>
@@ -5231,8 +5231,8 @@
       <c r="A69" s="32"/>
       <c r="B69" s="32"/>
       <c r="C69" s="32"/>
-      <c r="D69" s="41"/>
-      <c r="E69" s="41"/>
+      <c r="D69" s="48"/>
+      <c r="E69" s="48"/>
       <c r="F69" s="32"/>
       <c r="G69" s="32"/>
       <c r="H69" s="32"/>
@@ -5246,8 +5246,8 @@
       <c r="A70" s="32"/>
       <c r="B70" s="32"/>
       <c r="C70" s="32"/>
-      <c r="D70" s="41"/>
-      <c r="E70" s="41"/>
+      <c r="D70" s="48"/>
+      <c r="E70" s="48"/>
       <c r="F70" s="32"/>
       <c r="G70" s="32"/>
       <c r="H70" s="32"/>
@@ -5261,8 +5261,8 @@
       <c r="A71" s="32"/>
       <c r="B71" s="32"/>
       <c r="C71" s="32"/>
-      <c r="D71" s="41"/>
-      <c r="E71" s="41"/>
+      <c r="D71" s="48"/>
+      <c r="E71" s="48"/>
       <c r="F71" s="32"/>
       <c r="G71" s="32"/>
       <c r="H71" s="32"/>
@@ -5276,8 +5276,8 @@
       <c r="A72" s="32"/>
       <c r="B72" s="32"/>
       <c r="C72" s="32"/>
-      <c r="D72" s="41"/>
-      <c r="E72" s="41"/>
+      <c r="D72" s="48"/>
+      <c r="E72" s="48"/>
       <c r="F72" s="32"/>
       <c r="G72" s="32"/>
       <c r="H72" s="32"/>
@@ -5291,8 +5291,8 @@
       <c r="A73" s="32"/>
       <c r="B73" s="32"/>
       <c r="C73" s="32"/>
-      <c r="D73" s="41"/>
-      <c r="E73" s="41"/>
+      <c r="D73" s="48"/>
+      <c r="E73" s="48"/>
       <c r="F73" s="32"/>
       <c r="G73" s="32"/>
       <c r="H73" s="32"/>
@@ -5306,8 +5306,8 @@
       <c r="A74" s="32"/>
       <c r="B74" s="32"/>
       <c r="C74" s="32"/>
-      <c r="D74" s="41"/>
-      <c r="E74" s="41"/>
+      <c r="D74" s="48"/>
+      <c r="E74" s="48"/>
       <c r="F74" s="32"/>
       <c r="G74" s="32"/>
       <c r="H74" s="32"/>
@@ -5321,8 +5321,8 @@
       <c r="A75" s="32"/>
       <c r="B75" s="32"/>
       <c r="C75" s="32"/>
-      <c r="D75" s="41"/>
-      <c r="E75" s="41"/>
+      <c r="D75" s="48"/>
+      <c r="E75" s="48"/>
       <c r="F75" s="32"/>
       <c r="G75" s="32"/>
       <c r="H75" s="32"/>
@@ -5336,8 +5336,8 @@
       <c r="A76" s="32"/>
       <c r="B76" s="32"/>
       <c r="C76" s="32"/>
-      <c r="D76" s="41"/>
-      <c r="E76" s="41"/>
+      <c r="D76" s="48"/>
+      <c r="E76" s="48"/>
       <c r="F76" s="32"/>
       <c r="G76" s="32"/>
       <c r="H76" s="32"/>
@@ -5351,8 +5351,8 @@
       <c r="A77" s="32"/>
       <c r="B77" s="32"/>
       <c r="C77" s="32"/>
-      <c r="D77" s="41"/>
-      <c r="E77" s="41"/>
+      <c r="D77" s="48"/>
+      <c r="E77" s="48"/>
       <c r="F77" s="32"/>
       <c r="G77" s="32"/>
       <c r="H77" s="32"/>
@@ -5366,8 +5366,8 @@
       <c r="A78" s="32"/>
       <c r="B78" s="32"/>
       <c r="C78" s="32"/>
-      <c r="D78" s="41"/>
-      <c r="E78" s="41"/>
+      <c r="D78" s="48"/>
+      <c r="E78" s="48"/>
       <c r="F78" s="32"/>
       <c r="G78" s="32"/>
       <c r="H78" s="32"/>
@@ -5381,8 +5381,8 @@
       <c r="A79" s="32"/>
       <c r="B79" s="32"/>
       <c r="C79" s="32"/>
-      <c r="D79" s="41"/>
-      <c r="E79" s="41"/>
+      <c r="D79" s="48"/>
+      <c r="E79" s="48"/>
       <c r="F79" s="32"/>
       <c r="G79" s="32"/>
       <c r="H79" s="32"/>
@@ -5396,8 +5396,8 @@
       <c r="A80" s="32"/>
       <c r="B80" s="32"/>
       <c r="C80" s="32"/>
-      <c r="D80" s="41"/>
-      <c r="E80" s="41"/>
+      <c r="D80" s="48"/>
+      <c r="E80" s="48"/>
       <c r="F80" s="32"/>
       <c r="G80" s="32"/>
       <c r="H80" s="32"/>
@@ -5411,8 +5411,8 @@
       <c r="A81" s="25"/>
       <c r="B81" s="25"/>
       <c r="C81" s="33"/>
-      <c r="D81" s="42"/>
-      <c r="E81" s="42"/>
+      <c r="D81" s="49"/>
+      <c r="E81" s="49"/>
       <c r="F81" s="33"/>
       <c r="G81" s="33"/>
       <c r="H81" s="25"/>
@@ -5426,8 +5426,8 @@
       <c r="A82" s="25"/>
       <c r="B82" s="25"/>
       <c r="C82" s="33"/>
-      <c r="D82" s="42"/>
-      <c r="E82" s="42"/>
+      <c r="D82" s="49"/>
+      <c r="E82" s="49"/>
       <c r="F82" s="33"/>
       <c r="G82" s="33"/>
       <c r="H82" s="25"/>
@@ -5441,8 +5441,8 @@
       <c r="A83" s="25"/>
       <c r="B83" s="25"/>
       <c r="C83" s="33"/>
-      <c r="D83" s="42"/>
-      <c r="E83" s="42"/>
+      <c r="D83" s="49"/>
+      <c r="E83" s="49"/>
       <c r="F83" s="33"/>
       <c r="G83" s="33"/>
       <c r="H83" s="25"/>
@@ -5456,8 +5456,8 @@
       <c r="A84" s="25"/>
       <c r="B84" s="25"/>
       <c r="C84" s="33"/>
-      <c r="D84" s="42"/>
-      <c r="E84" s="42"/>
+      <c r="D84" s="49"/>
+      <c r="E84" s="49"/>
       <c r="F84" s="33"/>
       <c r="G84" s="33"/>
       <c r="H84" s="25"/>
@@ -5471,8 +5471,8 @@
       <c r="A85" s="25"/>
       <c r="B85" s="25"/>
       <c r="C85" s="33"/>
-      <c r="D85" s="42"/>
-      <c r="E85" s="42"/>
+      <c r="D85" s="49"/>
+      <c r="E85" s="49"/>
       <c r="F85" s="33"/>
       <c r="G85" s="33"/>
       <c r="H85" s="25"/>
@@ -5486,8 +5486,8 @@
       <c r="A86" s="25"/>
       <c r="B86" s="25"/>
       <c r="C86" s="33"/>
-      <c r="D86" s="42"/>
-      <c r="E86" s="42"/>
+      <c r="D86" s="49"/>
+      <c r="E86" s="49"/>
       <c r="F86" s="33"/>
       <c r="G86" s="33"/>
       <c r="H86" s="25"/>
@@ -5501,8 +5501,8 @@
       <c r="A87" s="25"/>
       <c r="B87" s="25"/>
       <c r="C87" s="33"/>
-      <c r="D87" s="42"/>
-      <c r="E87" s="42"/>
+      <c r="D87" s="49"/>
+      <c r="E87" s="49"/>
       <c r="F87" s="33"/>
       <c r="G87" s="33"/>
       <c r="H87" s="25"/>
@@ -5516,8 +5516,8 @@
       <c r="A88" s="25"/>
       <c r="B88" s="25"/>
       <c r="C88" s="33"/>
-      <c r="D88" s="42"/>
-      <c r="E88" s="42"/>
+      <c r="D88" s="49"/>
+      <c r="E88" s="49"/>
       <c r="F88" s="33"/>
       <c r="G88" s="33"/>
       <c r="H88" s="25"/>
@@ -5531,8 +5531,8 @@
       <c r="A89" s="25"/>
       <c r="B89" s="25"/>
       <c r="C89" s="33"/>
-      <c r="D89" s="42"/>
-      <c r="E89" s="42"/>
+      <c r="D89" s="49"/>
+      <c r="E89" s="49"/>
       <c r="F89" s="33"/>
       <c r="G89" s="33"/>
       <c r="H89" s="25"/>
@@ -5546,8 +5546,8 @@
       <c r="A90" s="25"/>
       <c r="B90" s="25"/>
       <c r="C90" s="33"/>
-      <c r="D90" s="42"/>
-      <c r="E90" s="42"/>
+      <c r="D90" s="49"/>
+      <c r="E90" s="49"/>
       <c r="F90" s="33"/>
       <c r="G90" s="33"/>
       <c r="H90" s="25"/>
@@ -5561,8 +5561,8 @@
       <c r="A91" s="25"/>
       <c r="B91" s="25"/>
       <c r="C91" s="33"/>
-      <c r="D91" s="42"/>
-      <c r="E91" s="42"/>
+      <c r="D91" s="49"/>
+      <c r="E91" s="49"/>
       <c r="F91" s="33"/>
       <c r="G91" s="33"/>
       <c r="H91" s="25"/>
@@ -5576,8 +5576,8 @@
       <c r="A92" s="25"/>
       <c r="B92" s="25"/>
       <c r="C92" s="33"/>
-      <c r="D92" s="42"/>
-      <c r="E92" s="42"/>
+      <c r="D92" s="49"/>
+      <c r="E92" s="49"/>
       <c r="F92" s="33"/>
       <c r="G92" s="33"/>
       <c r="H92" s="25"/>
@@ -5591,8 +5591,8 @@
       <c r="A93" s="25"/>
       <c r="B93" s="25"/>
       <c r="C93" s="33"/>
-      <c r="D93" s="42"/>
-      <c r="E93" s="42"/>
+      <c r="D93" s="49"/>
+      <c r="E93" s="49"/>
       <c r="F93" s="33"/>
       <c r="G93" s="33"/>
       <c r="H93" s="25"/>
@@ -5606,8 +5606,8 @@
       <c r="A94" s="25"/>
       <c r="B94" s="25"/>
       <c r="C94" s="33"/>
-      <c r="D94" s="42"/>
-      <c r="E94" s="42"/>
+      <c r="D94" s="49"/>
+      <c r="E94" s="49"/>
       <c r="F94" s="33"/>
       <c r="G94" s="33"/>
       <c r="H94" s="25"/>
@@ -5621,8 +5621,8 @@
       <c r="A95" s="25"/>
       <c r="B95" s="25"/>
       <c r="C95" s="33"/>
-      <c r="D95" s="42"/>
-      <c r="E95" s="42"/>
+      <c r="D95" s="49"/>
+      <c r="E95" s="49"/>
       <c r="F95" s="33"/>
       <c r="G95" s="33"/>
       <c r="H95" s="25"/>
@@ -5636,8 +5636,8 @@
       <c r="A96" s="25"/>
       <c r="B96" s="25"/>
       <c r="C96" s="33"/>
-      <c r="D96" s="42"/>
-      <c r="E96" s="42"/>
+      <c r="D96" s="49"/>
+      <c r="E96" s="49"/>
       <c r="F96" s="33"/>
       <c r="G96" s="33"/>
       <c r="H96" s="25"/>
@@ -5651,8 +5651,8 @@
       <c r="A97" s="25"/>
       <c r="B97" s="25"/>
       <c r="C97" s="33"/>
-      <c r="D97" s="42"/>
-      <c r="E97" s="42"/>
+      <c r="D97" s="49"/>
+      <c r="E97" s="49"/>
       <c r="F97" s="33"/>
       <c r="G97" s="33"/>
       <c r="H97" s="25"/>
@@ -5666,8 +5666,8 @@
       <c r="A98" s="25"/>
       <c r="B98" s="25"/>
       <c r="C98" s="33"/>
-      <c r="D98" s="42"/>
-      <c r="E98" s="42"/>
+      <c r="D98" s="49"/>
+      <c r="E98" s="49"/>
       <c r="F98" s="33"/>
       <c r="G98" s="33"/>
       <c r="H98" s="25"/>
@@ -5681,8 +5681,8 @@
       <c r="A99" s="25"/>
       <c r="B99" s="25"/>
       <c r="C99" s="33"/>
-      <c r="D99" s="42"/>
-      <c r="E99" s="42"/>
+      <c r="D99" s="49"/>
+      <c r="E99" s="49"/>
       <c r="F99" s="33"/>
       <c r="G99" s="33"/>
       <c r="H99" s="25"/>
@@ -5696,8 +5696,8 @@
       <c r="A100" s="25"/>
       <c r="B100" s="25"/>
       <c r="C100" s="33"/>
-      <c r="D100" s="42"/>
-      <c r="E100" s="42"/>
+      <c r="D100" s="49"/>
+      <c r="E100" s="49"/>
       <c r="F100" s="33"/>
       <c r="G100" s="33"/>
       <c r="H100" s="25"/>
@@ -5711,8 +5711,8 @@
       <c r="A101" s="25"/>
       <c r="B101" s="25"/>
       <c r="C101" s="33"/>
-      <c r="D101" s="42"/>
-      <c r="E101" s="42"/>
+      <c r="D101" s="49"/>
+      <c r="E101" s="49"/>
       <c r="F101" s="33"/>
       <c r="G101" s="33"/>
       <c r="H101" s="25"/>
@@ -5726,8 +5726,8 @@
       <c r="A102" s="25"/>
       <c r="B102" s="25"/>
       <c r="C102" s="33"/>
-      <c r="D102" s="42"/>
-      <c r="E102" s="42"/>
+      <c r="D102" s="49"/>
+      <c r="E102" s="49"/>
       <c r="F102" s="33"/>
       <c r="G102" s="33"/>
       <c r="H102" s="25"/>
@@ -5741,8 +5741,8 @@
       <c r="A103" s="25"/>
       <c r="B103" s="25"/>
       <c r="C103" s="33"/>
-      <c r="D103" s="42"/>
-      <c r="E103" s="42"/>
+      <c r="D103" s="49"/>
+      <c r="E103" s="49"/>
       <c r="F103" s="33"/>
       <c r="G103" s="33"/>
       <c r="H103" s="25"/>
@@ -5756,8 +5756,8 @@
       <c r="A104" s="25"/>
       <c r="B104" s="25"/>
       <c r="C104" s="33"/>
-      <c r="D104" s="42"/>
-      <c r="E104" s="42"/>
+      <c r="D104" s="49"/>
+      <c r="E104" s="49"/>
       <c r="F104" s="33"/>
       <c r="G104" s="33"/>
       <c r="H104" s="25"/>
@@ -5771,8 +5771,8 @@
       <c r="A105" s="25"/>
       <c r="B105" s="25"/>
       <c r="C105" s="33"/>
-      <c r="D105" s="42"/>
-      <c r="E105" s="42"/>
+      <c r="D105" s="49"/>
+      <c r="E105" s="49"/>
       <c r="F105" s="33"/>
       <c r="G105" s="33"/>
       <c r="H105" s="25"/>
@@ -5786,8 +5786,8 @@
       <c r="A106" s="25"/>
       <c r="B106" s="25"/>
       <c r="C106" s="33"/>
-      <c r="D106" s="42"/>
-      <c r="E106" s="42"/>
+      <c r="D106" s="49"/>
+      <c r="E106" s="49"/>
       <c r="F106" s="33"/>
       <c r="G106" s="33"/>
       <c r="H106" s="25"/>
@@ -5801,8 +5801,8 @@
       <c r="A107" s="25"/>
       <c r="B107" s="25"/>
       <c r="C107" s="33"/>
-      <c r="D107" s="42"/>
-      <c r="E107" s="42"/>
+      <c r="D107" s="49"/>
+      <c r="E107" s="49"/>
       <c r="F107" s="33"/>
       <c r="G107" s="33"/>
       <c r="H107" s="25"/>
@@ -5816,8 +5816,8 @@
       <c r="A108" s="25"/>
       <c r="B108" s="25"/>
       <c r="C108" s="33"/>
-      <c r="D108" s="42"/>
-      <c r="E108" s="42"/>
+      <c r="D108" s="49"/>
+      <c r="E108" s="49"/>
       <c r="F108" s="33"/>
       <c r="G108" s="33"/>
       <c r="H108" s="25"/>
@@ -5831,8 +5831,8 @@
       <c r="A109" s="25"/>
       <c r="B109" s="25"/>
       <c r="C109" s="33"/>
-      <c r="D109" s="42"/>
-      <c r="E109" s="42"/>
+      <c r="D109" s="49"/>
+      <c r="E109" s="49"/>
       <c r="F109" s="33"/>
       <c r="G109" s="33"/>
       <c r="H109" s="25"/>
@@ -5846,8 +5846,8 @@
       <c r="A110" s="25"/>
       <c r="B110" s="25"/>
       <c r="C110" s="33"/>
-      <c r="D110" s="42"/>
-      <c r="E110" s="42"/>
+      <c r="D110" s="49"/>
+      <c r="E110" s="49"/>
       <c r="F110" s="33"/>
       <c r="G110" s="33"/>
       <c r="H110" s="25"/>
@@ -5861,8 +5861,8 @@
       <c r="A111" s="27"/>
       <c r="B111" s="27"/>
       <c r="C111" s="34"/>
-      <c r="D111" s="43"/>
-      <c r="E111" s="43"/>
+      <c r="D111" s="50"/>
+      <c r="E111" s="50"/>
       <c r="F111" s="34"/>
       <c r="G111" s="34"/>
       <c r="H111" s="27"/>
@@ -5877,38 +5877,72 @@
     </row>
   </sheetData>
   <mergeCells count="122">
-    <mergeCell ref="E1:H3"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A8:D8"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="M10:M11"/>
-    <mergeCell ref="D10:E11"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="J8:M8"/>
-    <mergeCell ref="J7:M7"/>
-    <mergeCell ref="J6:M6"/>
-    <mergeCell ref="J5:M5"/>
-    <mergeCell ref="H8:I8"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D18:E18"/>
-    <mergeCell ref="D19:E19"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="D72:E72"/>
+    <mergeCell ref="D73:E73"/>
+    <mergeCell ref="D74:E74"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="D76:E76"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="D68:E68"/>
+    <mergeCell ref="D91:E91"/>
+    <mergeCell ref="D92:E92"/>
+    <mergeCell ref="D69:E69"/>
+    <mergeCell ref="D70:E70"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="D93:E93"/>
+    <mergeCell ref="D84:E84"/>
+    <mergeCell ref="D85:E85"/>
+    <mergeCell ref="D86:E86"/>
+    <mergeCell ref="D77:E77"/>
+    <mergeCell ref="D78:E78"/>
+    <mergeCell ref="D79:E79"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="D81:E81"/>
+    <mergeCell ref="D105:E105"/>
+    <mergeCell ref="D106:E106"/>
+    <mergeCell ref="D107:E107"/>
+    <mergeCell ref="D108:E108"/>
+    <mergeCell ref="D109:E109"/>
+    <mergeCell ref="D110:E110"/>
+    <mergeCell ref="D111:E111"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="D83:E83"/>
+    <mergeCell ref="D94:E94"/>
+    <mergeCell ref="D95:E95"/>
+    <mergeCell ref="D96:E96"/>
+    <mergeCell ref="D97:E97"/>
+    <mergeCell ref="D98:E98"/>
+    <mergeCell ref="D99:E99"/>
+    <mergeCell ref="D100:E100"/>
+    <mergeCell ref="D101:E101"/>
+    <mergeCell ref="D102:E102"/>
+    <mergeCell ref="D103:E103"/>
+    <mergeCell ref="D104:E104"/>
+    <mergeCell ref="D87:E87"/>
+    <mergeCell ref="D88:E88"/>
+    <mergeCell ref="D89:E89"/>
+    <mergeCell ref="D90:E90"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D51:E51"/>
     <mergeCell ref="D27:E27"/>
     <mergeCell ref="D28:E28"/>
     <mergeCell ref="D29:E29"/>
@@ -5933,72 +5967,38 @@
     <mergeCell ref="D32:E32"/>
     <mergeCell ref="D33:E33"/>
     <mergeCell ref="D34:E34"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="D105:E105"/>
-    <mergeCell ref="D106:E106"/>
-    <mergeCell ref="D107:E107"/>
-    <mergeCell ref="D108:E108"/>
-    <mergeCell ref="D109:E109"/>
-    <mergeCell ref="D110:E110"/>
-    <mergeCell ref="D111:E111"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="D83:E83"/>
-    <mergeCell ref="D94:E94"/>
-    <mergeCell ref="D95:E95"/>
-    <mergeCell ref="D96:E96"/>
-    <mergeCell ref="D97:E97"/>
-    <mergeCell ref="D98:E98"/>
-    <mergeCell ref="D99:E99"/>
-    <mergeCell ref="D100:E100"/>
-    <mergeCell ref="D101:E101"/>
-    <mergeCell ref="D102:E102"/>
-    <mergeCell ref="D103:E103"/>
-    <mergeCell ref="D104:E104"/>
-    <mergeCell ref="D87:E87"/>
-    <mergeCell ref="D88:E88"/>
-    <mergeCell ref="D89:E89"/>
-    <mergeCell ref="D90:E90"/>
-    <mergeCell ref="D93:E93"/>
-    <mergeCell ref="D84:E84"/>
-    <mergeCell ref="D85:E85"/>
-    <mergeCell ref="D86:E86"/>
-    <mergeCell ref="D77:E77"/>
-    <mergeCell ref="D78:E78"/>
-    <mergeCell ref="D79:E79"/>
-    <mergeCell ref="D80:E80"/>
-    <mergeCell ref="D81:E81"/>
-    <mergeCell ref="D72:E72"/>
-    <mergeCell ref="D73:E73"/>
-    <mergeCell ref="D74:E74"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="D68:E68"/>
-    <mergeCell ref="D91:E91"/>
-    <mergeCell ref="D92:E92"/>
-    <mergeCell ref="D69:E69"/>
-    <mergeCell ref="D70:E70"/>
-    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D18:E18"/>
+    <mergeCell ref="D19:E19"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="E1:H3"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="M10:M11"/>
+    <mergeCell ref="D10:E11"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="J8:M8"/>
+    <mergeCell ref="J7:M7"/>
+    <mergeCell ref="J6:M6"/>
+    <mergeCell ref="J5:M5"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="H7:I7"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="B10:B11"/>
   </mergeCells>
   <conditionalFormatting sqref="J12:K111">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">

</xml_diff>

<commit_message>
Fix template and add color to report
</commit_message>
<xml_diff>
--- a/hydrofia/hydrofia_ph_template.xlsx
+++ b/hydrofia/hydrofia_ph_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\mw\git\hydrofia\hydrofia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85C73932-D4CC-4ECE-9D39-1678A84A0324}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29C81170-210D-492D-9861-A73E55F5A681}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-15" yWindow="165" windowWidth="15600" windowHeight="11610" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
     <author>Nilsson Madeleine</author>
   </authors>
   <commentList>
-    <comment ref="E5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
       <text>
         <r>
           <rPr>
@@ -47,7 +47,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J10" authorId="1" shapeId="0" xr:uid="{21853188-1459-4735-90C6-F9F3174E1258}">
+    <comment ref="H10" authorId="1" shapeId="0" xr:uid="{21853188-1459-4735-90C6-F9F3174E1258}">
       <text>
         <r>
           <rPr>
@@ -2605,7 +2605,7 @@
     <numFmt numFmtId="165" formatCode="0.000"/>
     <numFmt numFmtId="166" formatCode="[$-41D]General"/>
   </numFmts>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2661,13 +2661,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="30"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -2850,9 +2843,9 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="166" fontId="7" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2872,13 +2865,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -2923,22 +2916,22 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2947,7 +2940,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2956,36 +2949,48 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="20" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="20" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2994,25 +2999,10 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="21" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3044,8 +3034,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>432324</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>879999</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>169500</xdr:rowOff>
     </xdr:to>
@@ -3438,41 +3428,40 @@
   <sheetPr>
     <tabColor theme="9"/>
   </sheetPr>
-  <dimension ref="A1:EJ111"/>
+  <dimension ref="A1:EH111"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6:H6"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.7109375" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.7109375" style="11" customWidth="1"/>
-    <col min="2" max="2" width="8.85546875" style="11" customWidth="1"/>
-    <col min="3" max="3" width="6.5703125" style="11" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" style="11" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" style="11" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="10" style="11" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" style="11" customWidth="1"/>
-    <col min="11" max="11" width="11.140625" style="11" customWidth="1"/>
-    <col min="12" max="12" width="17.28515625" style="11" customWidth="1"/>
-    <col min="13" max="21" width="10.7109375" style="11" customWidth="1"/>
-    <col min="22" max="16384" width="28.7109375" style="11"/>
+    <col min="1" max="1" width="20.85546875" style="11" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" style="11" customWidth="1"/>
+    <col min="3" max="3" width="15.5703125" style="11" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="7" width="10" style="11" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" style="11" customWidth="1"/>
+    <col min="9" max="9" width="11.140625" style="11" customWidth="1"/>
+    <col min="10" max="10" width="17.28515625" style="11" customWidth="1"/>
+    <col min="11" max="19" width="10.7109375" style="11" customWidth="1"/>
+    <col min="20" max="16384" width="28.7109375" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:140" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:138" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="42" t="s">
+      <c r="B1" s="46" t="s">
         <v>824</v>
       </c>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="J1" s="36" t="s">
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="H1" s="35" t="s">
         <v>828</v>
       </c>
-      <c r="L1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
       <c r="R1" s="13"/>
       <c r="S1" s="13"/>
       <c r="T1" s="13"/>
@@ -3594,19 +3583,18 @@
       <c r="EF1" s="13"/>
       <c r="EG1" s="13"/>
       <c r="EH1" s="13"/>
-      <c r="EI1" s="13"/>
-      <c r="EJ1" s="13"/>
-    </row>
-    <row r="2" spans="1:140" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="35"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="J2" s="36" t="s">
+    </row>
+    <row r="2" spans="1:138" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="46"/>
+      <c r="C2" s="46"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="46"/>
+      <c r="H2" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="13"/>
       <c r="R2" s="13"/>
       <c r="S2" s="13"/>
       <c r="T2" s="13"/>
@@ -3728,22 +3716,21 @@
       <c r="EF2" s="13"/>
       <c r="EG2" s="13"/>
       <c r="EH2" s="13"/>
-      <c r="EI2" s="13"/>
-      <c r="EJ2" s="13"/>
-    </row>
-    <row r="3" spans="1:140" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:138" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="35"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="12"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="G3" s="36"/>
+      <c r="H3" s="36"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="12"/>
+      <c r="P3" s="13"/>
+      <c r="Q3" s="13"/>
       <c r="R3" s="13"/>
       <c r="S3" s="13"/>
       <c r="T3" s="13"/>
@@ -3865,17 +3852,16 @@
       <c r="EF3" s="13"/>
       <c r="EG3" s="13"/>
       <c r="EH3" s="13"/>
-      <c r="EI3" s="13"/>
-      <c r="EJ3" s="13"/>
-    </row>
-    <row r="4" spans="1:140" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C4" s="35"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="36"/>
+    </row>
+    <row r="4" spans="1:138" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="37"/>
+      <c r="C4" s="37"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="37"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="P4" s="13"/>
+      <c r="Q4" s="13"/>
       <c r="R4" s="13"/>
       <c r="S4" s="13"/>
       <c r="T4" s="13"/>
@@ -3997,31 +3983,29 @@
       <c r="EF4" s="13"/>
       <c r="EG4" s="13"/>
       <c r="EH4" s="13"/>
-      <c r="EI4" s="13"/>
-      <c r="EJ4" s="13"/>
-    </row>
-    <row r="5" spans="1:140" s="4" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="44" t="s">
+    </row>
+    <row r="5" spans="1:138" s="4" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="44"/>
-      <c r="C5" s="44"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="52" t="s">
+      <c r="B5" s="38"/>
+      <c r="C5" s="51" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="53"/>
-      <c r="G5" s="52" t="s">
+      <c r="D5" s="52"/>
+      <c r="E5" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="53"/>
-      <c r="I5" s="44" t="s">
+      <c r="F5" s="52"/>
+      <c r="G5" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="J5" s="44"/>
-      <c r="K5" s="44"/>
-      <c r="L5" s="44"/>
-      <c r="M5" s="15"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="48"/>
+      <c r="K5" s="15"/>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="16"/>
       <c r="R5" s="16"/>
       <c r="S5" s="16"/>
       <c r="T5" s="16"/>
@@ -4143,23 +4127,21 @@
       <c r="EF5" s="16"/>
       <c r="EG5" s="16"/>
       <c r="EH5" s="16"/>
-      <c r="EI5" s="16"/>
-      <c r="EJ5" s="16"/>
-    </row>
-    <row r="6" spans="1:140" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="43"/>
-      <c r="B6" s="43"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="31"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
-      <c r="J6" s="43"/>
-      <c r="K6" s="43"/>
-      <c r="L6" s="43"/>
-      <c r="M6" s="17"/>
+    </row>
+    <row r="6" spans="1:138" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="41"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
+      <c r="J6" s="47"/>
+      <c r="K6" s="17"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="13"/>
       <c r="R6" s="13"/>
       <c r="S6" s="13"/>
       <c r="T6" s="13"/>
@@ -4281,1623 +4263,1306 @@
       <c r="EF6" s="13"/>
       <c r="EG6" s="13"/>
       <c r="EH6" s="13"/>
-      <c r="EI6" s="13"/>
-      <c r="EJ6" s="13"/>
-    </row>
-    <row r="7" spans="1:140" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="43"/>
-      <c r="B7" s="43"/>
-      <c r="C7" s="43"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="43"/>
-      <c r="F7" s="43"/>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="43"/>
-      <c r="K7" s="43"/>
-      <c r="L7" s="43"/>
-    </row>
-    <row r="8" spans="1:140" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="43"/>
-      <c r="B8" s="43"/>
-      <c r="C8" s="43"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="43"/>
-      <c r="I8" s="43"/>
-      <c r="J8" s="43"/>
-      <c r="K8" s="43"/>
-      <c r="L8" s="43"/>
-    </row>
-    <row r="9" spans="1:140" s="13" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:138" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="41"/>
+      <c r="B7" s="31"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="47"/>
+      <c r="J7" s="47"/>
+    </row>
+    <row r="8" spans="1:138" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="41"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="47"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="47"/>
+      <c r="G8" s="47"/>
+      <c r="H8" s="47"/>
+      <c r="I8" s="47"/>
+      <c r="J8" s="47"/>
+    </row>
+    <row r="9" spans="1:138" s="13" customFormat="1" ht="5.0999999999999996" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="18"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="19"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="20"/>
       <c r="I9" s="20"/>
-      <c r="J9" s="20"/>
-      <c r="K9" s="20"/>
-      <c r="L9" s="19"/>
-    </row>
-    <row r="10" spans="1:140" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="45" t="s">
+      <c r="J9" s="19"/>
+    </row>
+    <row r="10" spans="1:138" s="13" customFormat="1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A10" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="47"/>
-      <c r="C10" s="45" t="s">
+      <c r="B10" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="45"/>
-      <c r="E10" s="30" t="s">
+      <c r="C10" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="F10" s="22" t="s">
+      <c r="D10" s="22" t="s">
         <v>827</v>
       </c>
+      <c r="E10" s="21" t="s">
+        <v>825</v>
+      </c>
+      <c r="F10" s="21" t="s">
+        <v>826</v>
+      </c>
       <c r="G10" s="21" t="s">
-        <v>825</v>
-      </c>
-      <c r="H10" s="21" t="s">
-        <v>826</v>
-      </c>
-      <c r="I10" s="21" t="s">
         <v>831</v>
       </c>
-      <c r="J10" s="45" t="s">
+      <c r="H10" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="K10" s="22"/>
-    </row>
-    <row r="11" spans="1:140" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="46"/>
-      <c r="B11" s="48"/>
-      <c r="C11" s="46"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="23" t="s">
+      <c r="I10" s="22"/>
+    </row>
+    <row r="11" spans="1:138" s="13" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="50"/>
+      <c r="B11" s="50"/>
+      <c r="C11" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="24" t="s">
+      <c r="D11" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="G11" s="24"/>
-      <c r="H11" s="40" t="s">
+      <c r="E11" s="24"/>
+      <c r="F11" s="39" t="s">
         <v>829</v>
       </c>
-      <c r="I11" s="24" t="s">
+      <c r="G11" s="24" t="s">
         <v>830</v>
       </c>
-      <c r="J11" s="46"/>
-      <c r="K11" s="41"/>
-    </row>
-    <row r="12" spans="1:140" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H11" s="50"/>
+      <c r="I11" s="40"/>
+    </row>
+    <row r="12" spans="1:138" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="32"/>
-      <c r="B12" s="32"/>
-      <c r="C12" s="49"/>
-      <c r="D12" s="49"/>
+      <c r="B12" s="43"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
       <c r="E12" s="32"/>
       <c r="F12" s="32"/>
       <c r="G12" s="32"/>
       <c r="H12" s="32"/>
       <c r="I12" s="32"/>
       <c r="J12" s="32"/>
-      <c r="K12" s="32"/>
-      <c r="L12" s="32"/>
-    </row>
-    <row r="13" spans="1:140" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:138" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="32"/>
-      <c r="B13" s="32"/>
-      <c r="C13" s="49"/>
-      <c r="D13" s="49"/>
+      <c r="B13" s="43"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
       <c r="E13" s="32"/>
       <c r="F13" s="32"/>
       <c r="G13" s="32"/>
       <c r="H13" s="32"/>
       <c r="I13" s="32"/>
       <c r="J13" s="32"/>
-      <c r="K13" s="32"/>
-      <c r="L13" s="32"/>
-    </row>
-    <row r="14" spans="1:140" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:138" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="32"/>
-      <c r="B14" s="32"/>
-      <c r="C14" s="49"/>
-      <c r="D14" s="49"/>
+      <c r="B14" s="43"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
       <c r="E14" s="32"/>
       <c r="F14" s="32"/>
       <c r="G14" s="32"/>
       <c r="H14" s="32"/>
       <c r="I14" s="32"/>
       <c r="J14" s="32"/>
-      <c r="K14" s="32"/>
-      <c r="L14" s="32"/>
-    </row>
-    <row r="15" spans="1:140" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:138" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="32"/>
-      <c r="B15" s="32"/>
-      <c r="C15" s="49"/>
-      <c r="D15" s="49"/>
+      <c r="B15" s="43"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
       <c r="E15" s="32"/>
       <c r="F15" s="32"/>
       <c r="G15" s="32"/>
       <c r="H15" s="32"/>
       <c r="I15" s="32"/>
       <c r="J15" s="32"/>
-      <c r="K15" s="32"/>
-      <c r="L15" s="32"/>
-    </row>
-    <row r="16" spans="1:140" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:138" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="32"/>
-      <c r="B16" s="32"/>
-      <c r="C16" s="49"/>
-      <c r="D16" s="49"/>
+      <c r="B16" s="43"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
       <c r="E16" s="32"/>
       <c r="F16" s="32"/>
       <c r="G16" s="32"/>
       <c r="H16" s="32"/>
       <c r="I16" s="32"/>
       <c r="J16" s="32"/>
-      <c r="K16" s="32"/>
-      <c r="L16" s="32"/>
-    </row>
-    <row r="17" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="32"/>
-      <c r="B17" s="32"/>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49"/>
+      <c r="B17" s="43"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="32"/>
       <c r="E17" s="32"/>
       <c r="F17" s="32"/>
       <c r="G17" s="32"/>
       <c r="H17" s="32"/>
       <c r="I17" s="32"/>
       <c r="J17" s="32"/>
-      <c r="K17" s="32"/>
-      <c r="L17" s="32"/>
-    </row>
-    <row r="18" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="32"/>
-      <c r="B18" s="32"/>
-      <c r="C18" s="49"/>
-      <c r="D18" s="49"/>
+      <c r="B18" s="43"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
       <c r="E18" s="32"/>
       <c r="F18" s="32"/>
       <c r="G18" s="32"/>
       <c r="H18" s="32"/>
       <c r="I18" s="32"/>
       <c r="J18" s="32"/>
-      <c r="K18" s="32"/>
-      <c r="L18" s="32"/>
-    </row>
-    <row r="19" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="32"/>
-      <c r="B19" s="32"/>
-      <c r="C19" s="49"/>
-      <c r="D19" s="49"/>
+      <c r="B19" s="43"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
       <c r="E19" s="32"/>
       <c r="F19" s="32"/>
       <c r="G19" s="32"/>
       <c r="H19" s="32"/>
       <c r="I19" s="32"/>
       <c r="J19" s="32"/>
-      <c r="K19" s="32"/>
-      <c r="L19" s="32"/>
-    </row>
-    <row r="20" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="32"/>
-      <c r="B20" s="32"/>
-      <c r="C20" s="49"/>
-      <c r="D20" s="49"/>
+      <c r="B20" s="43"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
       <c r="E20" s="32"/>
       <c r="F20" s="32"/>
       <c r="G20" s="32"/>
       <c r="H20" s="32"/>
       <c r="I20" s="32"/>
       <c r="J20" s="32"/>
-      <c r="K20" s="32"/>
-      <c r="L20" s="32"/>
-    </row>
-    <row r="21" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="32"/>
-      <c r="B21" s="32"/>
-      <c r="C21" s="49"/>
-      <c r="D21" s="49"/>
+      <c r="B21" s="43"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
       <c r="E21" s="32"/>
       <c r="F21" s="32"/>
       <c r="G21" s="32"/>
       <c r="H21" s="32"/>
       <c r="I21" s="32"/>
       <c r="J21" s="32"/>
-      <c r="K21" s="32"/>
-      <c r="L21" s="32"/>
-    </row>
-    <row r="22" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="32"/>
-      <c r="B22" s="32"/>
-      <c r="C22" s="49"/>
-      <c r="D22" s="49"/>
+      <c r="B22" s="43"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
       <c r="E22" s="32"/>
       <c r="F22" s="32"/>
       <c r="G22" s="32"/>
       <c r="H22" s="32"/>
       <c r="I22" s="32"/>
       <c r="J22" s="32"/>
-      <c r="K22" s="32"/>
-      <c r="L22" s="32"/>
-    </row>
-    <row r="23" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="32"/>
-      <c r="B23" s="32"/>
-      <c r="C23" s="49"/>
-      <c r="D23" s="49"/>
+      <c r="B23" s="43"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
       <c r="E23" s="32"/>
       <c r="F23" s="32"/>
       <c r="G23" s="32"/>
       <c r="H23" s="32"/>
       <c r="I23" s="32"/>
       <c r="J23" s="32"/>
-      <c r="K23" s="32"/>
-      <c r="L23" s="32"/>
-    </row>
-    <row r="24" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="32"/>
-      <c r="B24" s="32"/>
-      <c r="C24" s="49"/>
-      <c r="D24" s="49"/>
+      <c r="B24" s="43"/>
+      <c r="C24" s="32"/>
+      <c r="D24" s="32"/>
       <c r="E24" s="32"/>
       <c r="F24" s="32"/>
       <c r="G24" s="32"/>
       <c r="H24" s="32"/>
       <c r="I24" s="32"/>
       <c r="J24" s="32"/>
-      <c r="K24" s="32"/>
-      <c r="L24" s="32"/>
-    </row>
-    <row r="25" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="32"/>
-      <c r="B25" s="32"/>
-      <c r="C25" s="49"/>
-      <c r="D25" s="49"/>
+      <c r="B25" s="43"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="32"/>
       <c r="E25" s="32"/>
       <c r="F25" s="32"/>
       <c r="G25" s="32"/>
       <c r="H25" s="32"/>
       <c r="I25" s="32"/>
       <c r="J25" s="32"/>
-      <c r="K25" s="32"/>
-      <c r="L25" s="32"/>
-    </row>
-    <row r="26" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="32"/>
-      <c r="B26" s="32"/>
-      <c r="C26" s="49"/>
-      <c r="D26" s="49"/>
+      <c r="B26" s="43"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="32"/>
       <c r="E26" s="32"/>
       <c r="F26" s="32"/>
       <c r="G26" s="32"/>
       <c r="H26" s="32"/>
       <c r="I26" s="32"/>
       <c r="J26" s="32"/>
-      <c r="K26" s="32"/>
-      <c r="L26" s="32"/>
-    </row>
-    <row r="27" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="32"/>
-      <c r="B27" s="32"/>
-      <c r="C27" s="49"/>
-      <c r="D27" s="49"/>
+      <c r="B27" s="43"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="32"/>
       <c r="E27" s="32"/>
       <c r="F27" s="32"/>
       <c r="G27" s="32"/>
       <c r="H27" s="32"/>
       <c r="I27" s="32"/>
       <c r="J27" s="32"/>
-      <c r="K27" s="32"/>
-      <c r="L27" s="32"/>
-    </row>
-    <row r="28" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="32"/>
-      <c r="B28" s="32"/>
-      <c r="C28" s="49"/>
-      <c r="D28" s="49"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
       <c r="E28" s="32"/>
       <c r="F28" s="32"/>
       <c r="G28" s="32"/>
       <c r="H28" s="32"/>
       <c r="I28" s="32"/>
       <c r="J28" s="32"/>
-      <c r="K28" s="32"/>
-      <c r="L28" s="32"/>
-    </row>
-    <row r="29" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="32"/>
-      <c r="B29" s="32"/>
-      <c r="C29" s="49"/>
-      <c r="D29" s="49"/>
+      <c r="B29" s="43"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
       <c r="E29" s="32"/>
       <c r="F29" s="32"/>
       <c r="G29" s="32"/>
       <c r="H29" s="32"/>
       <c r="I29" s="32"/>
       <c r="J29" s="32"/>
-      <c r="K29" s="32"/>
-      <c r="L29" s="32"/>
-    </row>
-    <row r="30" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="32"/>
-      <c r="B30" s="32"/>
-      <c r="C30" s="49"/>
-      <c r="D30" s="49"/>
+      <c r="B30" s="43"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="32"/>
       <c r="E30" s="32"/>
       <c r="F30" s="32"/>
       <c r="G30" s="32"/>
       <c r="H30" s="32"/>
       <c r="I30" s="32"/>
       <c r="J30" s="32"/>
-      <c r="K30" s="32"/>
-      <c r="L30" s="32"/>
-    </row>
-    <row r="31" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="32"/>
-      <c r="B31" s="32"/>
-      <c r="C31" s="49"/>
-      <c r="D31" s="49"/>
+      <c r="B31" s="43"/>
+      <c r="C31" s="32"/>
+      <c r="D31" s="32"/>
       <c r="E31" s="32"/>
       <c r="F31" s="32"/>
       <c r="G31" s="32"/>
       <c r="H31" s="32"/>
       <c r="I31" s="32"/>
       <c r="J31" s="32"/>
-      <c r="K31" s="32"/>
-      <c r="L31" s="32"/>
-    </row>
-    <row r="32" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="32"/>
-      <c r="B32" s="32"/>
-      <c r="C32" s="49"/>
-      <c r="D32" s="49"/>
+      <c r="B32" s="43"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="32"/>
       <c r="E32" s="32"/>
       <c r="F32" s="32"/>
       <c r="G32" s="32"/>
       <c r="H32" s="32"/>
       <c r="I32" s="32"/>
       <c r="J32" s="32"/>
-      <c r="K32" s="32"/>
-      <c r="L32" s="32"/>
-    </row>
-    <row r="33" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="32"/>
-      <c r="B33" s="32"/>
-      <c r="C33" s="49"/>
-      <c r="D33" s="49"/>
+      <c r="B33" s="43"/>
+      <c r="C33" s="32"/>
+      <c r="D33" s="32"/>
       <c r="E33" s="32"/>
       <c r="F33" s="32"/>
       <c r="G33" s="32"/>
       <c r="H33" s="32"/>
       <c r="I33" s="32"/>
       <c r="J33" s="32"/>
-      <c r="K33" s="32"/>
-      <c r="L33" s="32"/>
-    </row>
-    <row r="34" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="32"/>
-      <c r="B34" s="32"/>
-      <c r="C34" s="49"/>
-      <c r="D34" s="49"/>
+      <c r="B34" s="43"/>
+      <c r="C34" s="32"/>
+      <c r="D34" s="32"/>
       <c r="E34" s="32"/>
       <c r="F34" s="32"/>
       <c r="G34" s="32"/>
       <c r="H34" s="32"/>
       <c r="I34" s="32"/>
       <c r="J34" s="32"/>
-      <c r="K34" s="32"/>
-      <c r="L34" s="32"/>
-    </row>
-    <row r="35" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="32"/>
-      <c r="B35" s="32"/>
-      <c r="C35" s="49"/>
-      <c r="D35" s="49"/>
+      <c r="B35" s="43"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="32"/>
       <c r="E35" s="32"/>
       <c r="F35" s="32"/>
       <c r="G35" s="32"/>
       <c r="H35" s="32"/>
       <c r="I35" s="32"/>
       <c r="J35" s="32"/>
-      <c r="K35" s="32"/>
-      <c r="L35" s="32"/>
-    </row>
-    <row r="36" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="32"/>
-      <c r="B36" s="32"/>
-      <c r="C36" s="49"/>
-      <c r="D36" s="49"/>
+      <c r="B36" s="43"/>
+      <c r="C36" s="32"/>
+      <c r="D36" s="32"/>
       <c r="E36" s="32"/>
       <c r="F36" s="32"/>
       <c r="G36" s="32"/>
       <c r="H36" s="32"/>
       <c r="I36" s="32"/>
       <c r="J36" s="32"/>
-      <c r="K36" s="32"/>
-      <c r="L36" s="32"/>
-    </row>
-    <row r="37" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="32"/>
-      <c r="B37" s="32"/>
-      <c r="C37" s="49"/>
-      <c r="D37" s="49"/>
+      <c r="B37" s="43"/>
+      <c r="C37" s="32"/>
+      <c r="D37" s="32"/>
       <c r="E37" s="32"/>
       <c r="F37" s="32"/>
       <c r="G37" s="32"/>
       <c r="H37" s="32"/>
       <c r="I37" s="32"/>
       <c r="J37" s="32"/>
-      <c r="K37" s="32"/>
-      <c r="L37" s="32"/>
-    </row>
-    <row r="38" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="32"/>
-      <c r="B38" s="32"/>
-      <c r="C38" s="49"/>
-      <c r="D38" s="49"/>
+      <c r="B38" s="43"/>
+      <c r="C38" s="32"/>
+      <c r="D38" s="32"/>
       <c r="E38" s="32"/>
       <c r="F38" s="32"/>
       <c r="G38" s="32"/>
       <c r="H38" s="32"/>
       <c r="I38" s="32"/>
       <c r="J38" s="32"/>
-      <c r="K38" s="32"/>
-      <c r="L38" s="32"/>
-    </row>
-    <row r="39" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="32"/>
-      <c r="B39" s="32"/>
-      <c r="C39" s="49"/>
-      <c r="D39" s="49"/>
+      <c r="B39" s="43"/>
+      <c r="C39" s="32"/>
+      <c r="D39" s="32"/>
       <c r="E39" s="32"/>
       <c r="F39" s="32"/>
       <c r="G39" s="32"/>
       <c r="H39" s="32"/>
       <c r="I39" s="32"/>
       <c r="J39" s="32"/>
-      <c r="K39" s="32"/>
-      <c r="L39" s="32"/>
-    </row>
-    <row r="40" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="32"/>
-      <c r="B40" s="32"/>
-      <c r="C40" s="49"/>
-      <c r="D40" s="49"/>
+      <c r="B40" s="43"/>
+      <c r="C40" s="32"/>
+      <c r="D40" s="32"/>
       <c r="E40" s="32"/>
       <c r="F40" s="32"/>
       <c r="G40" s="32"/>
       <c r="H40" s="32"/>
       <c r="I40" s="32"/>
       <c r="J40" s="32"/>
-      <c r="K40" s="32"/>
-      <c r="L40" s="32"/>
-    </row>
-    <row r="41" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="32"/>
-      <c r="B41" s="32"/>
-      <c r="C41" s="49"/>
-      <c r="D41" s="49"/>
+      <c r="B41" s="43"/>
+      <c r="C41" s="32"/>
+      <c r="D41" s="32"/>
       <c r="E41" s="32"/>
       <c r="F41" s="32"/>
       <c r="G41" s="32"/>
       <c r="H41" s="32"/>
       <c r="I41" s="32"/>
       <c r="J41" s="32"/>
-      <c r="K41" s="32"/>
-      <c r="L41" s="32"/>
-    </row>
-    <row r="42" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="32"/>
-      <c r="B42" s="32"/>
-      <c r="C42" s="49"/>
-      <c r="D42" s="49"/>
+      <c r="B42" s="43"/>
+      <c r="C42" s="32"/>
+      <c r="D42" s="32"/>
       <c r="E42" s="32"/>
       <c r="F42" s="32"/>
       <c r="G42" s="32"/>
       <c r="H42" s="32"/>
       <c r="I42" s="32"/>
       <c r="J42" s="32"/>
-      <c r="K42" s="32"/>
-      <c r="L42" s="32"/>
-    </row>
-    <row r="43" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="32"/>
-      <c r="B43" s="32"/>
-      <c r="C43" s="49"/>
-      <c r="D43" s="49"/>
+      <c r="B43" s="43"/>
+      <c r="C43" s="32"/>
+      <c r="D43" s="32"/>
       <c r="E43" s="32"/>
       <c r="F43" s="32"/>
       <c r="G43" s="32"/>
       <c r="H43" s="32"/>
       <c r="I43" s="32"/>
       <c r="J43" s="32"/>
-      <c r="K43" s="32"/>
-      <c r="L43" s="32"/>
-    </row>
-    <row r="44" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="32"/>
-      <c r="B44" s="32"/>
-      <c r="C44" s="49"/>
-      <c r="D44" s="49"/>
+      <c r="B44" s="43"/>
+      <c r="C44" s="32"/>
+      <c r="D44" s="32"/>
       <c r="E44" s="32"/>
       <c r="F44" s="32"/>
       <c r="G44" s="32"/>
       <c r="H44" s="32"/>
       <c r="I44" s="32"/>
       <c r="J44" s="32"/>
-      <c r="K44" s="32"/>
-      <c r="L44" s="32"/>
-    </row>
-    <row r="45" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="32"/>
-      <c r="B45" s="32"/>
-      <c r="C45" s="49"/>
-      <c r="D45" s="49"/>
+      <c r="B45" s="43"/>
+      <c r="C45" s="32"/>
+      <c r="D45" s="32"/>
       <c r="E45" s="32"/>
       <c r="F45" s="32"/>
       <c r="G45" s="32"/>
       <c r="H45" s="32"/>
       <c r="I45" s="32"/>
       <c r="J45" s="32"/>
-      <c r="K45" s="32"/>
-      <c r="L45" s="32"/>
-    </row>
-    <row r="46" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="32"/>
-      <c r="B46" s="32"/>
-      <c r="C46" s="49"/>
-      <c r="D46" s="49"/>
+      <c r="B46" s="43"/>
+      <c r="C46" s="32"/>
+      <c r="D46" s="32"/>
       <c r="E46" s="32"/>
       <c r="F46" s="32"/>
       <c r="G46" s="32"/>
       <c r="H46" s="32"/>
       <c r="I46" s="32"/>
       <c r="J46" s="32"/>
-      <c r="K46" s="32"/>
-      <c r="L46" s="32"/>
-    </row>
-    <row r="47" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="32"/>
-      <c r="B47" s="32"/>
-      <c r="C47" s="49"/>
-      <c r="D47" s="49"/>
+      <c r="B47" s="43"/>
+      <c r="C47" s="32"/>
+      <c r="D47" s="32"/>
       <c r="E47" s="32"/>
       <c r="F47" s="32"/>
       <c r="G47" s="32"/>
       <c r="H47" s="32"/>
       <c r="I47" s="32"/>
       <c r="J47" s="32"/>
-      <c r="K47" s="32"/>
-      <c r="L47" s="32"/>
-    </row>
-    <row r="48" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="32"/>
-      <c r="B48" s="32"/>
-      <c r="C48" s="49"/>
-      <c r="D48" s="49"/>
+      <c r="B48" s="43"/>
+      <c r="C48" s="32"/>
+      <c r="D48" s="32"/>
       <c r="E48" s="32"/>
       <c r="F48" s="32"/>
       <c r="G48" s="32"/>
       <c r="H48" s="32"/>
       <c r="I48" s="32"/>
       <c r="J48" s="32"/>
-      <c r="K48" s="32"/>
-      <c r="L48" s="32"/>
-    </row>
-    <row r="49" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="32"/>
-      <c r="B49" s="32"/>
-      <c r="C49" s="49"/>
-      <c r="D49" s="49"/>
+      <c r="B49" s="43"/>
+      <c r="C49" s="32"/>
+      <c r="D49" s="32"/>
       <c r="E49" s="32"/>
       <c r="F49" s="32"/>
       <c r="G49" s="32"/>
       <c r="H49" s="32"/>
       <c r="I49" s="32"/>
       <c r="J49" s="32"/>
-      <c r="K49" s="32"/>
-      <c r="L49" s="32"/>
-    </row>
-    <row r="50" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="32"/>
-      <c r="B50" s="32"/>
-      <c r="C50" s="49"/>
-      <c r="D50" s="49"/>
+      <c r="B50" s="43"/>
+      <c r="C50" s="32"/>
+      <c r="D50" s="32"/>
       <c r="E50" s="32"/>
       <c r="F50" s="32"/>
       <c r="G50" s="32"/>
       <c r="H50" s="32"/>
       <c r="I50" s="32"/>
       <c r="J50" s="32"/>
-      <c r="K50" s="32"/>
-      <c r="L50" s="32"/>
-    </row>
-    <row r="51" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="32"/>
-      <c r="B51" s="32"/>
-      <c r="C51" s="49"/>
-      <c r="D51" s="49"/>
+      <c r="B51" s="43"/>
+      <c r="C51" s="32"/>
+      <c r="D51" s="32"/>
       <c r="E51" s="32"/>
       <c r="F51" s="32"/>
       <c r="G51" s="32"/>
       <c r="H51" s="32"/>
       <c r="I51" s="32"/>
       <c r="J51" s="32"/>
-      <c r="K51" s="32"/>
-      <c r="L51" s="32"/>
-    </row>
-    <row r="52" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="32"/>
-      <c r="B52" s="32"/>
-      <c r="C52" s="49"/>
-      <c r="D52" s="49"/>
+      <c r="B52" s="43"/>
+      <c r="C52" s="32"/>
+      <c r="D52" s="32"/>
       <c r="E52" s="32"/>
       <c r="F52" s="32"/>
       <c r="G52" s="32"/>
       <c r="H52" s="32"/>
       <c r="I52" s="32"/>
       <c r="J52" s="32"/>
-      <c r="K52" s="32"/>
-      <c r="L52" s="32"/>
-    </row>
-    <row r="53" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="32"/>
-      <c r="B53" s="32"/>
-      <c r="C53" s="49"/>
-      <c r="D53" s="49"/>
+      <c r="B53" s="43"/>
+      <c r="C53" s="32"/>
+      <c r="D53" s="32"/>
       <c r="E53" s="32"/>
       <c r="F53" s="32"/>
       <c r="G53" s="32"/>
       <c r="H53" s="32"/>
       <c r="I53" s="32"/>
       <c r="J53" s="32"/>
-      <c r="K53" s="32"/>
-      <c r="L53" s="32"/>
-    </row>
-    <row r="54" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="32"/>
-      <c r="B54" s="32"/>
-      <c r="C54" s="49"/>
-      <c r="D54" s="49"/>
+      <c r="B54" s="43"/>
+      <c r="C54" s="32"/>
+      <c r="D54" s="32"/>
       <c r="E54" s="32"/>
       <c r="F54" s="32"/>
       <c r="G54" s="32"/>
       <c r="H54" s="32"/>
       <c r="I54" s="32"/>
       <c r="J54" s="32"/>
-      <c r="K54" s="32"/>
-      <c r="L54" s="32"/>
-    </row>
-    <row r="55" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="32"/>
-      <c r="B55" s="32"/>
-      <c r="C55" s="49"/>
-      <c r="D55" s="49"/>
+      <c r="B55" s="43"/>
+      <c r="C55" s="32"/>
+      <c r="D55" s="32"/>
       <c r="E55" s="32"/>
       <c r="F55" s="32"/>
       <c r="G55" s="32"/>
       <c r="H55" s="32"/>
       <c r="I55" s="32"/>
       <c r="J55" s="32"/>
-      <c r="K55" s="32"/>
-      <c r="L55" s="32"/>
-    </row>
-    <row r="56" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="32"/>
-      <c r="B56" s="32"/>
-      <c r="C56" s="49"/>
-      <c r="D56" s="49"/>
+      <c r="B56" s="43"/>
+      <c r="C56" s="32"/>
+      <c r="D56" s="32"/>
       <c r="E56" s="32"/>
       <c r="F56" s="32"/>
       <c r="G56" s="32"/>
       <c r="H56" s="32"/>
       <c r="I56" s="32"/>
       <c r="J56" s="32"/>
-      <c r="K56" s="32"/>
-      <c r="L56" s="32"/>
-    </row>
-    <row r="57" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="32"/>
-      <c r="B57" s="32"/>
-      <c r="C57" s="49"/>
-      <c r="D57" s="49"/>
+      <c r="B57" s="43"/>
+      <c r="C57" s="32"/>
+      <c r="D57" s="32"/>
       <c r="E57" s="32"/>
       <c r="F57" s="32"/>
       <c r="G57" s="32"/>
       <c r="H57" s="32"/>
       <c r="I57" s="32"/>
       <c r="J57" s="32"/>
-      <c r="K57" s="32"/>
-      <c r="L57" s="32"/>
-    </row>
-    <row r="58" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="32"/>
-      <c r="B58" s="32"/>
-      <c r="C58" s="49"/>
-      <c r="D58" s="49"/>
+      <c r="B58" s="43"/>
+      <c r="C58" s="32"/>
+      <c r="D58" s="32"/>
       <c r="E58" s="32"/>
       <c r="F58" s="32"/>
       <c r="G58" s="32"/>
       <c r="H58" s="32"/>
       <c r="I58" s="32"/>
       <c r="J58" s="32"/>
-      <c r="K58" s="32"/>
-      <c r="L58" s="32"/>
-    </row>
-    <row r="59" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="32"/>
-      <c r="B59" s="32"/>
-      <c r="C59" s="49"/>
-      <c r="D59" s="49"/>
+      <c r="B59" s="43"/>
+      <c r="C59" s="32"/>
+      <c r="D59" s="32"/>
       <c r="E59" s="32"/>
       <c r="F59" s="32"/>
       <c r="G59" s="32"/>
       <c r="H59" s="32"/>
       <c r="I59" s="32"/>
       <c r="J59" s="32"/>
-      <c r="K59" s="32"/>
-      <c r="L59" s="32"/>
-    </row>
-    <row r="60" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="32"/>
-      <c r="B60" s="32"/>
-      <c r="C60" s="49"/>
-      <c r="D60" s="49"/>
+      <c r="B60" s="43"/>
+      <c r="C60" s="32"/>
+      <c r="D60" s="32"/>
       <c r="E60" s="32"/>
       <c r="F60" s="32"/>
       <c r="G60" s="32"/>
       <c r="H60" s="32"/>
       <c r="I60" s="32"/>
       <c r="J60" s="32"/>
-      <c r="K60" s="32"/>
-      <c r="L60" s="32"/>
-    </row>
-    <row r="61" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="32"/>
-      <c r="B61" s="32"/>
-      <c r="C61" s="49"/>
-      <c r="D61" s="49"/>
+      <c r="B61" s="43"/>
+      <c r="C61" s="32"/>
+      <c r="D61" s="32"/>
       <c r="E61" s="32"/>
       <c r="F61" s="32"/>
       <c r="G61" s="32"/>
       <c r="H61" s="32"/>
       <c r="I61" s="32"/>
       <c r="J61" s="32"/>
-      <c r="K61" s="32"/>
-      <c r="L61" s="32"/>
-    </row>
-    <row r="62" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="32"/>
-      <c r="B62" s="32"/>
-      <c r="C62" s="49"/>
-      <c r="D62" s="49"/>
+      <c r="B62" s="43"/>
+      <c r="C62" s="32"/>
+      <c r="D62" s="32"/>
       <c r="E62" s="32"/>
       <c r="F62" s="32"/>
       <c r="G62" s="32"/>
       <c r="H62" s="32"/>
       <c r="I62" s="32"/>
       <c r="J62" s="32"/>
-      <c r="K62" s="32"/>
-      <c r="L62" s="32"/>
-    </row>
-    <row r="63" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="32"/>
-      <c r="B63" s="32"/>
-      <c r="C63" s="49"/>
-      <c r="D63" s="49"/>
+      <c r="B63" s="43"/>
+      <c r="C63" s="32"/>
+      <c r="D63" s="32"/>
       <c r="E63" s="32"/>
       <c r="F63" s="32"/>
       <c r="G63" s="32"/>
       <c r="H63" s="32"/>
       <c r="I63" s="32"/>
       <c r="J63" s="32"/>
-      <c r="K63" s="32"/>
-      <c r="L63" s="32"/>
-    </row>
-    <row r="64" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="32"/>
-      <c r="B64" s="32"/>
-      <c r="C64" s="49"/>
-      <c r="D64" s="49"/>
+      <c r="B64" s="43"/>
+      <c r="C64" s="32"/>
+      <c r="D64" s="32"/>
       <c r="E64" s="32"/>
       <c r="F64" s="32"/>
       <c r="G64" s="32"/>
       <c r="H64" s="32"/>
       <c r="I64" s="32"/>
       <c r="J64" s="32"/>
-      <c r="K64" s="32"/>
-      <c r="L64" s="32"/>
-    </row>
-    <row r="65" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="32"/>
-      <c r="B65" s="32"/>
-      <c r="C65" s="49"/>
-      <c r="D65" s="49"/>
+      <c r="B65" s="43"/>
+      <c r="C65" s="32"/>
+      <c r="D65" s="32"/>
       <c r="E65" s="32"/>
       <c r="F65" s="32"/>
       <c r="G65" s="32"/>
       <c r="H65" s="32"/>
       <c r="I65" s="32"/>
       <c r="J65" s="32"/>
-      <c r="K65" s="32"/>
-      <c r="L65" s="32"/>
-    </row>
-    <row r="66" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="32"/>
-      <c r="B66" s="32"/>
-      <c r="C66" s="49"/>
-      <c r="D66" s="49"/>
+      <c r="B66" s="43"/>
+      <c r="C66" s="32"/>
+      <c r="D66" s="32"/>
       <c r="E66" s="32"/>
       <c r="F66" s="32"/>
       <c r="G66" s="32"/>
       <c r="H66" s="32"/>
       <c r="I66" s="32"/>
       <c r="J66" s="32"/>
-      <c r="K66" s="32"/>
-      <c r="L66" s="32"/>
-    </row>
-    <row r="67" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="32"/>
-      <c r="B67" s="32"/>
-      <c r="C67" s="49"/>
-      <c r="D67" s="49"/>
+      <c r="B67" s="43"/>
+      <c r="C67" s="32"/>
+      <c r="D67" s="32"/>
       <c r="E67" s="32"/>
       <c r="F67" s="32"/>
       <c r="G67" s="32"/>
       <c r="H67" s="32"/>
       <c r="I67" s="32"/>
       <c r="J67" s="32"/>
-      <c r="K67" s="32"/>
-      <c r="L67" s="32"/>
-    </row>
-    <row r="68" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="32"/>
-      <c r="B68" s="32"/>
-      <c r="C68" s="49"/>
-      <c r="D68" s="49"/>
+      <c r="B68" s="43"/>
+      <c r="C68" s="32"/>
+      <c r="D68" s="32"/>
       <c r="E68" s="32"/>
       <c r="F68" s="32"/>
       <c r="G68" s="32"/>
       <c r="H68" s="32"/>
       <c r="I68" s="32"/>
       <c r="J68" s="32"/>
-      <c r="K68" s="32"/>
-      <c r="L68" s="32"/>
-    </row>
-    <row r="69" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="32"/>
-      <c r="B69" s="32"/>
-      <c r="C69" s="49"/>
-      <c r="D69" s="49"/>
+      <c r="B69" s="43"/>
+      <c r="C69" s="32"/>
+      <c r="D69" s="32"/>
       <c r="E69" s="32"/>
       <c r="F69" s="32"/>
       <c r="G69" s="32"/>
       <c r="H69" s="32"/>
       <c r="I69" s="32"/>
       <c r="J69" s="32"/>
-      <c r="K69" s="32"/>
-      <c r="L69" s="32"/>
-    </row>
-    <row r="70" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="32"/>
-      <c r="B70" s="32"/>
-      <c r="C70" s="49"/>
-      <c r="D70" s="49"/>
+      <c r="B70" s="43"/>
+      <c r="C70" s="32"/>
+      <c r="D70" s="32"/>
       <c r="E70" s="32"/>
       <c r="F70" s="32"/>
       <c r="G70" s="32"/>
       <c r="H70" s="32"/>
       <c r="I70" s="32"/>
       <c r="J70" s="32"/>
-      <c r="K70" s="32"/>
-      <c r="L70" s="32"/>
-    </row>
-    <row r="71" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="32"/>
-      <c r="B71" s="32"/>
-      <c r="C71" s="49"/>
-      <c r="D71" s="49"/>
+      <c r="B71" s="43"/>
+      <c r="C71" s="32"/>
+      <c r="D71" s="32"/>
       <c r="E71" s="32"/>
       <c r="F71" s="32"/>
       <c r="G71" s="32"/>
       <c r="H71" s="32"/>
       <c r="I71" s="32"/>
       <c r="J71" s="32"/>
-      <c r="K71" s="32"/>
-      <c r="L71" s="32"/>
-    </row>
-    <row r="72" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="32"/>
-      <c r="B72" s="32"/>
-      <c r="C72" s="49"/>
-      <c r="D72" s="49"/>
+      <c r="B72" s="43"/>
+      <c r="C72" s="32"/>
+      <c r="D72" s="32"/>
       <c r="E72" s="32"/>
       <c r="F72" s="32"/>
       <c r="G72" s="32"/>
       <c r="H72" s="32"/>
       <c r="I72" s="32"/>
       <c r="J72" s="32"/>
-      <c r="K72" s="32"/>
-      <c r="L72" s="32"/>
-    </row>
-    <row r="73" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="32"/>
-      <c r="B73" s="32"/>
-      <c r="C73" s="49"/>
-      <c r="D73" s="49"/>
+      <c r="B73" s="43"/>
+      <c r="C73" s="32"/>
+      <c r="D73" s="32"/>
       <c r="E73" s="32"/>
       <c r="F73" s="32"/>
       <c r="G73" s="32"/>
       <c r="H73" s="32"/>
       <c r="I73" s="32"/>
       <c r="J73" s="32"/>
-      <c r="K73" s="32"/>
-      <c r="L73" s="32"/>
-    </row>
-    <row r="74" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="32"/>
-      <c r="B74" s="32"/>
-      <c r="C74" s="49"/>
-      <c r="D74" s="49"/>
+      <c r="B74" s="43"/>
+      <c r="C74" s="32"/>
+      <c r="D74" s="32"/>
       <c r="E74" s="32"/>
       <c r="F74" s="32"/>
       <c r="G74" s="32"/>
       <c r="H74" s="32"/>
       <c r="I74" s="32"/>
       <c r="J74" s="32"/>
-      <c r="K74" s="32"/>
-      <c r="L74" s="32"/>
-    </row>
-    <row r="75" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="32"/>
-      <c r="B75" s="32"/>
-      <c r="C75" s="49"/>
-      <c r="D75" s="49"/>
+      <c r="B75" s="43"/>
+      <c r="C75" s="32"/>
+      <c r="D75" s="32"/>
       <c r="E75" s="32"/>
       <c r="F75" s="32"/>
       <c r="G75" s="32"/>
       <c r="H75" s="32"/>
       <c r="I75" s="32"/>
       <c r="J75" s="32"/>
-      <c r="K75" s="32"/>
-      <c r="L75" s="32"/>
-    </row>
-    <row r="76" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="32"/>
-      <c r="B76" s="32"/>
-      <c r="C76" s="49"/>
-      <c r="D76" s="49"/>
+      <c r="B76" s="43"/>
+      <c r="C76" s="32"/>
+      <c r="D76" s="32"/>
       <c r="E76" s="32"/>
       <c r="F76" s="32"/>
       <c r="G76" s="32"/>
       <c r="H76" s="32"/>
       <c r="I76" s="32"/>
       <c r="J76" s="32"/>
-      <c r="K76" s="32"/>
-      <c r="L76" s="32"/>
-    </row>
-    <row r="77" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="32"/>
-      <c r="B77" s="32"/>
-      <c r="C77" s="49"/>
-      <c r="D77" s="49"/>
+      <c r="B77" s="43"/>
+      <c r="C77" s="32"/>
+      <c r="D77" s="32"/>
       <c r="E77" s="32"/>
       <c r="F77" s="32"/>
       <c r="G77" s="32"/>
       <c r="H77" s="32"/>
       <c r="I77" s="32"/>
       <c r="J77" s="32"/>
-      <c r="K77" s="32"/>
-      <c r="L77" s="32"/>
-    </row>
-    <row r="78" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="32"/>
-      <c r="B78" s="32"/>
-      <c r="C78" s="49"/>
-      <c r="D78" s="49"/>
+      <c r="B78" s="43"/>
+      <c r="C78" s="32"/>
+      <c r="D78" s="32"/>
       <c r="E78" s="32"/>
       <c r="F78" s="32"/>
       <c r="G78" s="32"/>
       <c r="H78" s="32"/>
       <c r="I78" s="32"/>
       <c r="J78" s="32"/>
-      <c r="K78" s="32"/>
-      <c r="L78" s="32"/>
-    </row>
-    <row r="79" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="32"/>
-      <c r="B79" s="32"/>
-      <c r="C79" s="49"/>
-      <c r="D79" s="49"/>
+      <c r="B79" s="43"/>
+      <c r="C79" s="32"/>
+      <c r="D79" s="32"/>
       <c r="E79" s="32"/>
       <c r="F79" s="32"/>
       <c r="G79" s="32"/>
       <c r="H79" s="32"/>
       <c r="I79" s="32"/>
       <c r="J79" s="32"/>
-      <c r="K79" s="32"/>
-      <c r="L79" s="32"/>
-    </row>
-    <row r="80" spans="1:12" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="1:10" s="29" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="32"/>
-      <c r="B80" s="32"/>
-      <c r="C80" s="49"/>
-      <c r="D80" s="49"/>
+      <c r="B80" s="43"/>
+      <c r="C80" s="32"/>
+      <c r="D80" s="32"/>
       <c r="E80" s="32"/>
       <c r="F80" s="32"/>
       <c r="G80" s="32"/>
       <c r="H80" s="32"/>
       <c r="I80" s="32"/>
       <c r="J80" s="32"/>
-      <c r="K80" s="32"/>
-      <c r="L80" s="32"/>
-    </row>
-    <row r="81" spans="1:12" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="25"/>
-      <c r="B81" s="33"/>
-      <c r="C81" s="50"/>
-      <c r="D81" s="50"/>
-      <c r="E81" s="33"/>
+      <c r="B81" s="44"/>
+      <c r="C81" s="33"/>
+      <c r="D81" s="33"/>
+      <c r="E81" s="25"/>
       <c r="F81" s="33"/>
-      <c r="G81" s="25"/>
+      <c r="G81" s="33"/>
       <c r="H81" s="33"/>
       <c r="I81" s="33"/>
-      <c r="J81" s="33"/>
-      <c r="K81" s="33"/>
-      <c r="L81" s="25"/>
-    </row>
-    <row r="82" spans="1:12" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J81" s="25"/>
+    </row>
+    <row r="82" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="25"/>
-      <c r="B82" s="33"/>
-      <c r="C82" s="50"/>
-      <c r="D82" s="50"/>
-      <c r="E82" s="33"/>
+      <c r="B82" s="44"/>
+      <c r="C82" s="33"/>
+      <c r="D82" s="33"/>
+      <c r="E82" s="25"/>
       <c r="F82" s="33"/>
-      <c r="G82" s="25"/>
+      <c r="G82" s="33"/>
       <c r="H82" s="33"/>
       <c r="I82" s="33"/>
-      <c r="J82" s="33"/>
-      <c r="K82" s="33"/>
-      <c r="L82" s="25"/>
-    </row>
-    <row r="83" spans="1:12" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J82" s="25"/>
+    </row>
+    <row r="83" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="25"/>
-      <c r="B83" s="33"/>
-      <c r="C83" s="50"/>
-      <c r="D83" s="50"/>
-      <c r="E83" s="33"/>
+      <c r="B83" s="44"/>
+      <c r="C83" s="33"/>
+      <c r="D83" s="33"/>
+      <c r="E83" s="25"/>
       <c r="F83" s="33"/>
-      <c r="G83" s="25"/>
+      <c r="G83" s="33"/>
       <c r="H83" s="33"/>
       <c r="I83" s="33"/>
-      <c r="J83" s="33"/>
-      <c r="K83" s="33"/>
-      <c r="L83" s="25"/>
-    </row>
-    <row r="84" spans="1:12" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J83" s="25"/>
+    </row>
+    <row r="84" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="25"/>
-      <c r="B84" s="33"/>
-      <c r="C84" s="50"/>
-      <c r="D84" s="50"/>
-      <c r="E84" s="33"/>
+      <c r="B84" s="44"/>
+      <c r="C84" s="33"/>
+      <c r="D84" s="33"/>
+      <c r="E84" s="25"/>
       <c r="F84" s="33"/>
-      <c r="G84" s="25"/>
+      <c r="G84" s="33"/>
       <c r="H84" s="33"/>
       <c r="I84" s="33"/>
-      <c r="J84" s="33"/>
-      <c r="K84" s="33"/>
-      <c r="L84" s="25"/>
-    </row>
-    <row r="85" spans="1:12" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J84" s="25"/>
+    </row>
+    <row r="85" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="25"/>
-      <c r="B85" s="33"/>
-      <c r="C85" s="50"/>
-      <c r="D85" s="50"/>
-      <c r="E85" s="33"/>
+      <c r="B85" s="44"/>
+      <c r="C85" s="33"/>
+      <c r="D85" s="33"/>
+      <c r="E85" s="25"/>
       <c r="F85" s="33"/>
-      <c r="G85" s="25"/>
+      <c r="G85" s="33"/>
       <c r="H85" s="33"/>
       <c r="I85" s="33"/>
-      <c r="J85" s="33"/>
-      <c r="K85" s="33"/>
-      <c r="L85" s="25"/>
-    </row>
-    <row r="86" spans="1:12" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J85" s="25"/>
+    </row>
+    <row r="86" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="25"/>
-      <c r="B86" s="33"/>
-      <c r="C86" s="50"/>
-      <c r="D86" s="50"/>
-      <c r="E86" s="33"/>
+      <c r="B86" s="44"/>
+      <c r="C86" s="33"/>
+      <c r="D86" s="33"/>
+      <c r="E86" s="25"/>
       <c r="F86" s="33"/>
-      <c r="G86" s="25"/>
+      <c r="G86" s="33"/>
       <c r="H86" s="33"/>
       <c r="I86" s="33"/>
-      <c r="J86" s="33"/>
-      <c r="K86" s="33"/>
-      <c r="L86" s="25"/>
-    </row>
-    <row r="87" spans="1:12" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J86" s="25"/>
+    </row>
+    <row r="87" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="25"/>
-      <c r="B87" s="33"/>
-      <c r="C87" s="50"/>
-      <c r="D87" s="50"/>
-      <c r="E87" s="33"/>
+      <c r="B87" s="44"/>
+      <c r="C87" s="33"/>
+      <c r="D87" s="33"/>
+      <c r="E87" s="25"/>
       <c r="F87" s="33"/>
-      <c r="G87" s="25"/>
+      <c r="G87" s="33"/>
       <c r="H87" s="33"/>
       <c r="I87" s="33"/>
-      <c r="J87" s="33"/>
-      <c r="K87" s="33"/>
-      <c r="L87" s="25"/>
-    </row>
-    <row r="88" spans="1:12" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J87" s="25"/>
+    </row>
+    <row r="88" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="25"/>
-      <c r="B88" s="33"/>
-      <c r="C88" s="50"/>
-      <c r="D88" s="50"/>
-      <c r="E88" s="33"/>
+      <c r="B88" s="44"/>
+      <c r="C88" s="33"/>
+      <c r="D88" s="33"/>
+      <c r="E88" s="25"/>
       <c r="F88" s="33"/>
-      <c r="G88" s="25"/>
+      <c r="G88" s="33"/>
       <c r="H88" s="33"/>
       <c r="I88" s="33"/>
-      <c r="J88" s="33"/>
-      <c r="K88" s="33"/>
-      <c r="L88" s="25"/>
-    </row>
-    <row r="89" spans="1:12" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J88" s="25"/>
+    </row>
+    <row r="89" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="25"/>
-      <c r="B89" s="33"/>
-      <c r="C89" s="50"/>
-      <c r="D89" s="50"/>
-      <c r="E89" s="33"/>
+      <c r="B89" s="44"/>
+      <c r="C89" s="33"/>
+      <c r="D89" s="33"/>
+      <c r="E89" s="25"/>
       <c r="F89" s="33"/>
-      <c r="G89" s="25"/>
+      <c r="G89" s="33"/>
       <c r="H89" s="33"/>
       <c r="I89" s="33"/>
-      <c r="J89" s="33"/>
-      <c r="K89" s="33"/>
-      <c r="L89" s="25"/>
-    </row>
-    <row r="90" spans="1:12" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J89" s="25"/>
+    </row>
+    <row r="90" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="25"/>
-      <c r="B90" s="33"/>
-      <c r="C90" s="50"/>
-      <c r="D90" s="50"/>
-      <c r="E90" s="33"/>
+      <c r="B90" s="44"/>
+      <c r="C90" s="33"/>
+      <c r="D90" s="33"/>
+      <c r="E90" s="25"/>
       <c r="F90" s="33"/>
-      <c r="G90" s="25"/>
+      <c r="G90" s="33"/>
       <c r="H90" s="33"/>
       <c r="I90" s="33"/>
-      <c r="J90" s="33"/>
-      <c r="K90" s="33"/>
-      <c r="L90" s="25"/>
-    </row>
-    <row r="91" spans="1:12" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J90" s="25"/>
+    </row>
+    <row r="91" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="25"/>
-      <c r="B91" s="33"/>
-      <c r="C91" s="50"/>
-      <c r="D91" s="50"/>
-      <c r="E91" s="33"/>
+      <c r="B91" s="44"/>
+      <c r="C91" s="33"/>
+      <c r="D91" s="33"/>
+      <c r="E91" s="25"/>
       <c r="F91" s="33"/>
-      <c r="G91" s="25"/>
+      <c r="G91" s="33"/>
       <c r="H91" s="33"/>
       <c r="I91" s="33"/>
-      <c r="J91" s="33"/>
-      <c r="K91" s="33"/>
-      <c r="L91" s="25"/>
-    </row>
-    <row r="92" spans="1:12" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J91" s="25"/>
+    </row>
+    <row r="92" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="25"/>
-      <c r="B92" s="33"/>
-      <c r="C92" s="50"/>
-      <c r="D92" s="50"/>
-      <c r="E92" s="33"/>
+      <c r="B92" s="44"/>
+      <c r="C92" s="33"/>
+      <c r="D92" s="33"/>
+      <c r="E92" s="25"/>
       <c r="F92" s="33"/>
-      <c r="G92" s="25"/>
+      <c r="G92" s="33"/>
       <c r="H92" s="33"/>
       <c r="I92" s="33"/>
-      <c r="J92" s="33"/>
-      <c r="K92" s="33"/>
-      <c r="L92" s="25"/>
-    </row>
-    <row r="93" spans="1:12" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J92" s="25"/>
+    </row>
+    <row r="93" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="25"/>
-      <c r="B93" s="33"/>
-      <c r="C93" s="50"/>
-      <c r="D93" s="50"/>
-      <c r="E93" s="33"/>
+      <c r="B93" s="44"/>
+      <c r="C93" s="33"/>
+      <c r="D93" s="33"/>
+      <c r="E93" s="25"/>
       <c r="F93" s="33"/>
-      <c r="G93" s="25"/>
+      <c r="G93" s="33"/>
       <c r="H93" s="33"/>
       <c r="I93" s="33"/>
-      <c r="J93" s="33"/>
-      <c r="K93" s="33"/>
-      <c r="L93" s="25"/>
-    </row>
-    <row r="94" spans="1:12" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J93" s="25"/>
+    </row>
+    <row r="94" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="25"/>
-      <c r="B94" s="33"/>
-      <c r="C94" s="50"/>
-      <c r="D94" s="50"/>
-      <c r="E94" s="33"/>
+      <c r="B94" s="44"/>
+      <c r="C94" s="33"/>
+      <c r="D94" s="33"/>
+      <c r="E94" s="25"/>
       <c r="F94" s="33"/>
-      <c r="G94" s="25"/>
+      <c r="G94" s="33"/>
       <c r="H94" s="33"/>
       <c r="I94" s="33"/>
-      <c r="J94" s="33"/>
-      <c r="K94" s="33"/>
-      <c r="L94" s="25"/>
-    </row>
-    <row r="95" spans="1:12" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J94" s="25"/>
+    </row>
+    <row r="95" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="25"/>
-      <c r="B95" s="33"/>
-      <c r="C95" s="50"/>
-      <c r="D95" s="50"/>
-      <c r="E95" s="33"/>
+      <c r="B95" s="44"/>
+      <c r="C95" s="33"/>
+      <c r="D95" s="33"/>
+      <c r="E95" s="25"/>
       <c r="F95" s="33"/>
-      <c r="G95" s="25"/>
+      <c r="G95" s="33"/>
       <c r="H95" s="33"/>
       <c r="I95" s="33"/>
-      <c r="J95" s="33"/>
-      <c r="K95" s="33"/>
-      <c r="L95" s="25"/>
-    </row>
-    <row r="96" spans="1:12" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J95" s="25"/>
+    </row>
+    <row r="96" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="25"/>
-      <c r="B96" s="33"/>
-      <c r="C96" s="50"/>
-      <c r="D96" s="50"/>
-      <c r="E96" s="33"/>
+      <c r="B96" s="44"/>
+      <c r="C96" s="33"/>
+      <c r="D96" s="33"/>
+      <c r="E96" s="25"/>
       <c r="F96" s="33"/>
-      <c r="G96" s="25"/>
+      <c r="G96" s="33"/>
       <c r="H96" s="33"/>
       <c r="I96" s="33"/>
-      <c r="J96" s="33"/>
-      <c r="K96" s="33"/>
-      <c r="L96" s="25"/>
-    </row>
-    <row r="97" spans="1:12" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J96" s="25"/>
+    </row>
+    <row r="97" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="25"/>
-      <c r="B97" s="33"/>
-      <c r="C97" s="50"/>
-      <c r="D97" s="50"/>
-      <c r="E97" s="33"/>
+      <c r="B97" s="44"/>
+      <c r="C97" s="33"/>
+      <c r="D97" s="33"/>
+      <c r="E97" s="25"/>
       <c r="F97" s="33"/>
-      <c r="G97" s="25"/>
+      <c r="G97" s="33"/>
       <c r="H97" s="33"/>
       <c r="I97" s="33"/>
-      <c r="J97" s="33"/>
-      <c r="K97" s="33"/>
-      <c r="L97" s="25"/>
-    </row>
-    <row r="98" spans="1:12" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J97" s="25"/>
+    </row>
+    <row r="98" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="25"/>
-      <c r="B98" s="33"/>
-      <c r="C98" s="50"/>
-      <c r="D98" s="50"/>
-      <c r="E98" s="33"/>
+      <c r="B98" s="44"/>
+      <c r="C98" s="33"/>
+      <c r="D98" s="33"/>
+      <c r="E98" s="25"/>
       <c r="F98" s="33"/>
-      <c r="G98" s="25"/>
+      <c r="G98" s="33"/>
       <c r="H98" s="33"/>
       <c r="I98" s="33"/>
-      <c r="J98" s="33"/>
-      <c r="K98" s="33"/>
-      <c r="L98" s="25"/>
-    </row>
-    <row r="99" spans="1:12" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J98" s="25"/>
+    </row>
+    <row r="99" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="25"/>
-      <c r="B99" s="33"/>
-      <c r="C99" s="50"/>
-      <c r="D99" s="50"/>
-      <c r="E99" s="33"/>
+      <c r="B99" s="44"/>
+      <c r="C99" s="33"/>
+      <c r="D99" s="33"/>
+      <c r="E99" s="25"/>
       <c r="F99" s="33"/>
-      <c r="G99" s="25"/>
+      <c r="G99" s="33"/>
       <c r="H99" s="33"/>
       <c r="I99" s="33"/>
-      <c r="J99" s="33"/>
-      <c r="K99" s="33"/>
-      <c r="L99" s="25"/>
-    </row>
-    <row r="100" spans="1:12" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J99" s="25"/>
+    </row>
+    <row r="100" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="25"/>
-      <c r="B100" s="33"/>
-      <c r="C100" s="50"/>
-      <c r="D100" s="50"/>
-      <c r="E100" s="33"/>
+      <c r="B100" s="44"/>
+      <c r="C100" s="33"/>
+      <c r="D100" s="33"/>
+      <c r="E100" s="25"/>
       <c r="F100" s="33"/>
-      <c r="G100" s="25"/>
+      <c r="G100" s="33"/>
       <c r="H100" s="33"/>
       <c r="I100" s="33"/>
-      <c r="J100" s="33"/>
-      <c r="K100" s="33"/>
-      <c r="L100" s="25"/>
-    </row>
-    <row r="101" spans="1:12" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J100" s="25"/>
+    </row>
+    <row r="101" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="25"/>
-      <c r="B101" s="33"/>
-      <c r="C101" s="50"/>
-      <c r="D101" s="50"/>
-      <c r="E101" s="33"/>
+      <c r="B101" s="44"/>
+      <c r="C101" s="33"/>
+      <c r="D101" s="33"/>
+      <c r="E101" s="25"/>
       <c r="F101" s="33"/>
-      <c r="G101" s="25"/>
+      <c r="G101" s="33"/>
       <c r="H101" s="33"/>
       <c r="I101" s="33"/>
-      <c r="J101" s="33"/>
-      <c r="K101" s="33"/>
-      <c r="L101" s="25"/>
-    </row>
-    <row r="102" spans="1:12" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J101" s="25"/>
+    </row>
+    <row r="102" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="25"/>
-      <c r="B102" s="33"/>
-      <c r="C102" s="50"/>
-      <c r="D102" s="50"/>
-      <c r="E102" s="33"/>
+      <c r="B102" s="44"/>
+      <c r="C102" s="33"/>
+      <c r="D102" s="33"/>
+      <c r="E102" s="25"/>
       <c r="F102" s="33"/>
-      <c r="G102" s="25"/>
+      <c r="G102" s="33"/>
       <c r="H102" s="33"/>
       <c r="I102" s="33"/>
-      <c r="J102" s="33"/>
-      <c r="K102" s="33"/>
-      <c r="L102" s="25"/>
-    </row>
-    <row r="103" spans="1:12" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J102" s="25"/>
+    </row>
+    <row r="103" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="25"/>
-      <c r="B103" s="33"/>
-      <c r="C103" s="50"/>
-      <c r="D103" s="50"/>
-      <c r="E103" s="33"/>
+      <c r="B103" s="44"/>
+      <c r="C103" s="33"/>
+      <c r="D103" s="33"/>
+      <c r="E103" s="25"/>
       <c r="F103" s="33"/>
-      <c r="G103" s="25"/>
+      <c r="G103" s="33"/>
       <c r="H103" s="33"/>
       <c r="I103" s="33"/>
-      <c r="J103" s="33"/>
-      <c r="K103" s="33"/>
-      <c r="L103" s="25"/>
-    </row>
-    <row r="104" spans="1:12" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J103" s="25"/>
+    </row>
+    <row r="104" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="25"/>
-      <c r="B104" s="33"/>
-      <c r="C104" s="50"/>
-      <c r="D104" s="50"/>
-      <c r="E104" s="33"/>
+      <c r="B104" s="44"/>
+      <c r="C104" s="33"/>
+      <c r="D104" s="33"/>
+      <c r="E104" s="25"/>
       <c r="F104" s="33"/>
-      <c r="G104" s="25"/>
+      <c r="G104" s="33"/>
       <c r="H104" s="33"/>
       <c r="I104" s="33"/>
-      <c r="J104" s="33"/>
-      <c r="K104" s="33"/>
-      <c r="L104" s="25"/>
-    </row>
-    <row r="105" spans="1:12" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J104" s="25"/>
+    </row>
+    <row r="105" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="25"/>
-      <c r="B105" s="33"/>
-      <c r="C105" s="50"/>
-      <c r="D105" s="50"/>
-      <c r="E105" s="33"/>
+      <c r="B105" s="44"/>
+      <c r="C105" s="33"/>
+      <c r="D105" s="33"/>
+      <c r="E105" s="25"/>
       <c r="F105" s="33"/>
-      <c r="G105" s="25"/>
+      <c r="G105" s="33"/>
       <c r="H105" s="33"/>
       <c r="I105" s="33"/>
-      <c r="J105" s="33"/>
-      <c r="K105" s="33"/>
-      <c r="L105" s="25"/>
-    </row>
-    <row r="106" spans="1:12" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J105" s="25"/>
+    </row>
+    <row r="106" spans="1:10" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="25"/>
-      <c r="B106" s="33"/>
-      <c r="C106" s="50"/>
-      <c r="D106" s="50"/>
-      <c r="E106" s="33"/>
+      <c r="B106" s="44"/>
+      <c r="C106" s="33"/>
+      <c r="D106" s="33"/>
+      <c r="E106" s="25"/>
       <c r="F106" s="33"/>
-      <c r="G106" s="25"/>
+      <c r="G106" s="33"/>
       <c r="H106" s="33"/>
       <c r="I106" s="33"/>
-      <c r="J106" s="33"/>
-      <c r="K106" s="33"/>
-      <c r="L106" s="25"/>
-    </row>
-    <row r="107" spans="1:12" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J106" s="25"/>
+    </row>
+    <row r="107" spans="1:10" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="25"/>
-      <c r="B107" s="33"/>
-      <c r="C107" s="50"/>
-      <c r="D107" s="50"/>
-      <c r="E107" s="33"/>
+      <c r="B107" s="44"/>
+      <c r="C107" s="33"/>
+      <c r="D107" s="33"/>
+      <c r="E107" s="25"/>
       <c r="F107" s="33"/>
-      <c r="G107" s="25"/>
+      <c r="G107" s="33"/>
       <c r="H107" s="33"/>
       <c r="I107" s="33"/>
-      <c r="J107" s="33"/>
-      <c r="K107" s="33"/>
-      <c r="L107" s="25"/>
-    </row>
-    <row r="108" spans="1:12" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J107" s="25"/>
+    </row>
+    <row r="108" spans="1:10" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="25"/>
-      <c r="B108" s="33"/>
-      <c r="C108" s="50"/>
-      <c r="D108" s="50"/>
-      <c r="E108" s="33"/>
+      <c r="B108" s="44"/>
+      <c r="C108" s="33"/>
+      <c r="D108" s="33"/>
+      <c r="E108" s="25"/>
       <c r="F108" s="33"/>
-      <c r="G108" s="25"/>
+      <c r="G108" s="33"/>
       <c r="H108" s="33"/>
       <c r="I108" s="33"/>
-      <c r="J108" s="33"/>
-      <c r="K108" s="33"/>
-      <c r="L108" s="25"/>
-    </row>
-    <row r="109" spans="1:12" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J108" s="25"/>
+    </row>
+    <row r="109" spans="1:10" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="25"/>
-      <c r="B109" s="33"/>
-      <c r="C109" s="50"/>
-      <c r="D109" s="50"/>
-      <c r="E109" s="33"/>
+      <c r="B109" s="44"/>
+      <c r="C109" s="33"/>
+      <c r="D109" s="33"/>
+      <c r="E109" s="25"/>
       <c r="F109" s="33"/>
-      <c r="G109" s="25"/>
+      <c r="G109" s="33"/>
       <c r="H109" s="33"/>
       <c r="I109" s="33"/>
-      <c r="J109" s="33"/>
-      <c r="K109" s="33"/>
-      <c r="L109" s="25"/>
-    </row>
-    <row r="110" spans="1:12" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J109" s="25"/>
+    </row>
+    <row r="110" spans="1:10" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="25"/>
-      <c r="B110" s="33"/>
-      <c r="C110" s="50"/>
-      <c r="D110" s="50"/>
-      <c r="E110" s="33"/>
+      <c r="B110" s="44"/>
+      <c r="C110" s="33"/>
+      <c r="D110" s="33"/>
+      <c r="E110" s="25"/>
       <c r="F110" s="33"/>
-      <c r="G110" s="25"/>
+      <c r="G110" s="33"/>
       <c r="H110" s="33"/>
       <c r="I110" s="33"/>
-      <c r="J110" s="33"/>
-      <c r="K110" s="33"/>
-      <c r="L110" s="25"/>
-    </row>
-    <row r="111" spans="1:12" s="28" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="J110" s="25"/>
+    </row>
+    <row r="111" spans="1:10" s="28" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="27"/>
-      <c r="B111" s="34"/>
-      <c r="C111" s="51"/>
-      <c r="D111" s="51"/>
-      <c r="E111" s="34"/>
+      <c r="B111" s="45"/>
+      <c r="C111" s="34"/>
+      <c r="D111" s="34"/>
+      <c r="E111" s="27"/>
       <c r="F111" s="34"/>
-      <c r="G111" s="27"/>
+      <c r="G111" s="34"/>
       <c r="H111" s="34"/>
       <c r="I111" s="34"/>
-      <c r="J111" s="34"/>
-      <c r="K111" s="34"/>
-      <c r="L111" s="27"/>
+      <c r="J111" s="27"/>
     </row>
   </sheetData>
-  <mergeCells count="121">
-    <mergeCell ref="C72:D72"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="C75:D75"/>
-    <mergeCell ref="C76:D76"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="C68:D68"/>
-    <mergeCell ref="C91:D91"/>
-    <mergeCell ref="C92:D92"/>
-    <mergeCell ref="C69:D69"/>
-    <mergeCell ref="C70:D70"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="C93:D93"/>
-    <mergeCell ref="C84:D84"/>
-    <mergeCell ref="C85:D85"/>
-    <mergeCell ref="C86:D86"/>
-    <mergeCell ref="C77:D77"/>
-    <mergeCell ref="C78:D78"/>
-    <mergeCell ref="C79:D79"/>
-    <mergeCell ref="C80:D80"/>
-    <mergeCell ref="C81:D81"/>
-    <mergeCell ref="C105:D105"/>
-    <mergeCell ref="C106:D106"/>
-    <mergeCell ref="C107:D107"/>
-    <mergeCell ref="C108:D108"/>
-    <mergeCell ref="C109:D109"/>
-    <mergeCell ref="C110:D110"/>
-    <mergeCell ref="C111:D111"/>
-    <mergeCell ref="C82:D82"/>
-    <mergeCell ref="C83:D83"/>
-    <mergeCell ref="C94:D94"/>
-    <mergeCell ref="C95:D95"/>
-    <mergeCell ref="C96:D96"/>
-    <mergeCell ref="C97:D97"/>
-    <mergeCell ref="C98:D98"/>
-    <mergeCell ref="C99:D99"/>
-    <mergeCell ref="C100:D100"/>
-    <mergeCell ref="C101:D101"/>
-    <mergeCell ref="C102:D102"/>
-    <mergeCell ref="C103:D103"/>
-    <mergeCell ref="C104:D104"/>
-    <mergeCell ref="C87:D87"/>
-    <mergeCell ref="C88:D88"/>
-    <mergeCell ref="C89:D89"/>
-    <mergeCell ref="C90:D90"/>
-    <mergeCell ref="C62:D62"/>
-    <mergeCell ref="C63:D63"/>
-    <mergeCell ref="C64:D64"/>
-    <mergeCell ref="C65:D65"/>
-    <mergeCell ref="C66:D66"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="C60:D60"/>
-    <mergeCell ref="C61:D61"/>
-    <mergeCell ref="C35:D35"/>
-    <mergeCell ref="C36:D36"/>
-    <mergeCell ref="C52:D52"/>
-    <mergeCell ref="C53:D53"/>
-    <mergeCell ref="C54:D54"/>
-    <mergeCell ref="C55:D55"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="C48:D48"/>
-    <mergeCell ref="C49:D49"/>
-    <mergeCell ref="C50:D50"/>
-    <mergeCell ref="C51:D51"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="C47:D47"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C23:D23"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="C45:D45"/>
-    <mergeCell ref="C46:D46"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C33:D33"/>
-    <mergeCell ref="C34:D34"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="D1:G3"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A6:C6"/>
-    <mergeCell ref="A5:C5"/>
-    <mergeCell ref="J10:J11"/>
-    <mergeCell ref="C10:D11"/>
+  <mergeCells count="16">
+    <mergeCell ref="B1:E3"/>
+    <mergeCell ref="H10:H11"/>
     <mergeCell ref="A10:A11"/>
-    <mergeCell ref="I8:L8"/>
-    <mergeCell ref="I7:L7"/>
-    <mergeCell ref="I6:L6"/>
-    <mergeCell ref="I5:L5"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="G8:J8"/>
+    <mergeCell ref="G7:J7"/>
+    <mergeCell ref="G6:J6"/>
+    <mergeCell ref="G5:J5"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E6:F6"/>
     <mergeCell ref="E5:F5"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C5:D5"/>
     <mergeCell ref="B10:B11"/>
   </mergeCells>
   <pageMargins left="0.78740157480314965" right="0.39370078740157483" top="0.59055118110236227" bottom="0.59055118110236227" header="0.31496062992125984" footer="0.19685039370078741"/>

</xml_diff>

<commit_message>
Add python package pillow to keep image in template
</commit_message>
<xml_diff>
--- a/hydrofia/hydrofia_ph_template.xlsx
+++ b/hydrofia/hydrofia_ph_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\mw\git\hydrofia\hydrofia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2AB210F-1FAE-45DD-A432-E471AC254D1D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3E44B11-F599-4B6D-9073-BA50B4295FA4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-15" yWindow="165" windowWidth="15600" windowHeight="11610" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -925,7 +925,7 @@
   <dimension ref="A1:EH111"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.7109375" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>